<commit_message>
Algunas Correcciones a la parte de impacto
</commit_message>
<xml_diff>
--- a/evsim/Impac.Amb..xlsx
+++ b/evsim/Impac.Amb..xlsx
@@ -848,61 +848,61 @@
         <v>22</v>
       </c>
       <c r="I1" s="15">
-        <v>100.5</v>
+        <v>149.5</v>
       </c>
       <c r="J1" s="15">
-        <v>197.5</v>
+        <v>301</v>
       </c>
       <c r="K1" s="15">
-        <v>290.5</v>
+        <v>440.5</v>
       </c>
       <c r="L1" s="15">
-        <v>380</v>
+        <v>564</v>
       </c>
       <c r="M1" s="15">
-        <v>465.5</v>
+        <v>698.5</v>
       </c>
       <c r="N1" s="15">
-        <v>547.5</v>
+        <v>826.5</v>
       </c>
       <c r="O1" s="15">
-        <v>626</v>
+        <v>952.5</v>
       </c>
       <c r="P1" s="15">
-        <v>701</v>
+        <v>1058.5</v>
       </c>
       <c r="Q1" s="15">
-        <v>773</v>
+        <v>1156</v>
       </c>
       <c r="R1" s="15">
-        <v>841.5</v>
+        <v>1264.5</v>
       </c>
       <c r="S1" s="15">
-        <v>907</v>
+        <v>1367.5</v>
       </c>
       <c r="T1" s="15">
-        <v>969.5</v>
+        <v>1470</v>
       </c>
       <c r="U1" s="15">
-        <v>1029</v>
-      </c>
-      <c r="V1" s="15">
-        <v>1085.5</v>
-      </c>
-      <c r="W1" s="15">
-        <v>1139.5</v>
-      </c>
-      <c r="X1" s="15">
-        <v>1191</v>
-      </c>
-      <c r="Y1" s="15">
-        <v>1240</v>
-      </c>
-      <c r="Z1" s="15">
-        <v>1286.5</v>
-      </c>
-      <c r="AA1" s="15">
-        <v>1330.5</v>
+        <v>1553.5</v>
+      </c>
+      <c r="V1" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="W1" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="X1" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Y1" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Z1" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AA1" s="15" t="e">
+        <v>#N/A</v>
       </c>
       <c r="AB1" s="19" t="e">
         <v>#N/A</v>
@@ -937,61 +937,61 @@
         <v>61.155072000000004</v>
       </c>
       <c r="I2" s="17">
-        <v>100.5</v>
+        <v>149.5</v>
       </c>
       <c r="J2" s="15">
-        <v>197.5</v>
+        <v>301</v>
       </c>
       <c r="K2" s="17">
-        <v>290.5</v>
+        <v>440.5</v>
       </c>
       <c r="L2" s="15">
-        <v>380</v>
+        <v>564</v>
       </c>
       <c r="M2" s="17">
-        <v>465.5</v>
+        <v>698.5</v>
       </c>
       <c r="N2" s="15">
-        <v>547.5</v>
+        <v>826.5</v>
       </c>
       <c r="O2" s="17">
-        <v>626</v>
+        <v>952.5</v>
       </c>
       <c r="P2" s="15">
-        <v>701</v>
+        <v>1058.5</v>
       </c>
       <c r="Q2" s="17">
-        <v>773</v>
+        <v>1156</v>
       </c>
       <c r="R2" s="15">
-        <v>841.5</v>
+        <v>1264.5</v>
       </c>
       <c r="S2" s="17">
-        <v>907</v>
+        <v>1367.5</v>
       </c>
       <c r="T2" s="15">
-        <v>969.5</v>
+        <v>1470</v>
       </c>
       <c r="U2" s="17">
-        <v>1029</v>
-      </c>
-      <c r="V2" s="15">
-        <v>1085.5</v>
-      </c>
-      <c r="W2" s="17">
-        <v>1139.5</v>
-      </c>
-      <c r="X2" s="15">
-        <v>1191</v>
-      </c>
-      <c r="Y2" s="17">
-        <v>1240</v>
-      </c>
-      <c r="Z2" s="15">
-        <v>1286.5</v>
-      </c>
-      <c r="AA2" s="17">
-        <v>1330.5</v>
+        <v>1553.5</v>
+      </c>
+      <c r="V2" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="W2" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="X2" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Y2" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Z2" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AA2" s="17" t="e">
+        <v>#N/A</v>
       </c>
       <c r="AB2" s="19" t="e">
         <v>#N/A</v>
@@ -1026,61 +1026,61 @@
         <v>185</v>
       </c>
       <c r="I3" s="18">
-        <v>43</v>
+        <v>142.5</v>
       </c>
       <c r="J3" s="15">
-        <v>84.5</v>
+        <v>270.5</v>
       </c>
       <c r="K3" s="18">
-        <v>124.5</v>
+        <v>385.5</v>
       </c>
       <c r="L3" s="15">
-        <v>163</v>
+        <v>512.5</v>
       </c>
       <c r="M3" s="18">
-        <v>200</v>
+        <v>634.5</v>
       </c>
       <c r="N3" s="15">
-        <v>235.5</v>
+        <v>743.5</v>
       </c>
       <c r="O3" s="18">
-        <v>269.5</v>
+        <v>850.5</v>
       </c>
       <c r="P3" s="15">
-        <v>302</v>
+        <v>966</v>
       </c>
       <c r="Q3" s="18">
-        <v>333</v>
+        <v>1076</v>
       </c>
       <c r="R3" s="15">
-        <v>362.5</v>
+        <v>1165.5</v>
       </c>
       <c r="S3" s="18">
-        <v>390.5</v>
+        <v>1245</v>
       </c>
       <c r="T3" s="15">
-        <v>417.5</v>
+        <v>1336.5</v>
       </c>
       <c r="U3" s="18">
-        <v>443</v>
-      </c>
-      <c r="V3" s="15">
-        <v>467.5</v>
-      </c>
-      <c r="W3" s="18">
-        <v>490.5</v>
-      </c>
-      <c r="X3" s="15">
-        <v>512.5</v>
-      </c>
-      <c r="Y3" s="18">
-        <v>533.5</v>
-      </c>
-      <c r="Z3" s="15">
-        <v>553.5</v>
-      </c>
-      <c r="AA3" s="18">
-        <v>572.5</v>
+        <v>1423.5</v>
+      </c>
+      <c r="V3" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="W3" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="X3" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Y3" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Z3" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AA3" s="18" t="e">
+        <v>#N/A</v>
       </c>
       <c r="AB3" s="19" t="e">
         <v>#N/A</v>
@@ -1115,61 +1115,61 @@
         <v>141.62227200000001</v>
       </c>
       <c r="I4" s="17">
-        <v>43</v>
+        <v>142.5</v>
       </c>
       <c r="J4" s="15">
-        <v>84.5</v>
+        <v>270.5</v>
       </c>
       <c r="K4" s="17">
-        <v>124.5</v>
+        <v>385.5</v>
       </c>
       <c r="L4" s="15">
-        <v>163</v>
+        <v>512.5</v>
       </c>
       <c r="M4" s="17">
-        <v>200</v>
+        <v>634.5</v>
       </c>
       <c r="N4" s="15">
-        <v>235.5</v>
+        <v>743.5</v>
       </c>
       <c r="O4" s="17">
-        <v>269.5</v>
+        <v>850.5</v>
       </c>
       <c r="P4" s="15">
-        <v>302</v>
+        <v>966</v>
       </c>
       <c r="Q4" s="17">
-        <v>333</v>
+        <v>1076</v>
       </c>
       <c r="R4" s="15">
-        <v>362.5</v>
+        <v>1165.5</v>
       </c>
       <c r="S4" s="17">
-        <v>390.5</v>
+        <v>1245</v>
       </c>
       <c r="T4" s="15">
-        <v>417.5</v>
+        <v>1336.5</v>
       </c>
       <c r="U4" s="17">
-        <v>443</v>
-      </c>
-      <c r="V4" s="15">
-        <v>467.5</v>
-      </c>
-      <c r="W4" s="17">
-        <v>490.5</v>
-      </c>
-      <c r="X4" s="15">
-        <v>512.5</v>
-      </c>
-      <c r="Y4" s="17">
-        <v>533.5</v>
-      </c>
-      <c r="Z4" s="15">
-        <v>553.5</v>
-      </c>
-      <c r="AA4" s="17">
-        <v>572.5</v>
+        <v>1423.5</v>
+      </c>
+      <c r="V4" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="W4" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="X4" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Y4" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Z4" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AA4" s="17" t="e">
+        <v>#N/A</v>
       </c>
       <c r="AB4" s="19" t="e">
         <v>#N/A</v>
@@ -1204,61 +1204,61 @@
         <v>33.796224000000002</v>
       </c>
       <c r="I5" s="15">
-        <v>133</v>
+        <v>95.5</v>
       </c>
       <c r="J5" s="15">
-        <v>261</v>
+        <v>196</v>
       </c>
       <c r="K5" s="15">
-        <v>384</v>
+        <v>297.5</v>
       </c>
       <c r="L5" s="15">
-        <v>502</v>
+        <v>382.5</v>
       </c>
       <c r="M5" s="15">
-        <v>615</v>
+        <v>461</v>
       </c>
       <c r="N5" s="15">
-        <v>723.5</v>
+        <v>546.5</v>
       </c>
       <c r="O5" s="15">
-        <v>827.5</v>
+        <v>617.5</v>
       </c>
       <c r="P5" s="15">
-        <v>927</v>
+        <v>688.5</v>
       </c>
       <c r="Q5" s="15">
-        <v>1022</v>
+        <v>770.5</v>
       </c>
       <c r="R5" s="15">
-        <v>1112.5</v>
+        <v>830</v>
       </c>
       <c r="S5" s="15">
-        <v>1199</v>
+        <v>896</v>
       </c>
       <c r="T5" s="15">
-        <v>1281.5</v>
+        <v>948.5</v>
       </c>
       <c r="U5" s="15">
-        <v>1360</v>
-      </c>
-      <c r="V5" s="15">
-        <v>1435</v>
-      </c>
-      <c r="W5" s="15">
-        <v>1506.5</v>
-      </c>
-      <c r="X5" s="15">
-        <v>1574.5</v>
-      </c>
-      <c r="Y5" s="15">
-        <v>1639</v>
-      </c>
-      <c r="Z5" s="15">
-        <v>1700</v>
-      </c>
-      <c r="AA5" s="15">
-        <v>1758</v>
+        <v>1008.5</v>
+      </c>
+      <c r="V5" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="W5" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="X5" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Y5" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Z5" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AA5" s="15" t="e">
+        <v>#N/A</v>
       </c>
       <c r="AB5" s="19" t="e">
         <v>#N/A</v>
@@ -1293,61 +1293,61 @@
         <v>50</v>
       </c>
       <c r="I6" s="16">
-        <v>133</v>
+        <v>95.5</v>
       </c>
       <c r="J6" s="15">
-        <v>261</v>
+        <v>196</v>
       </c>
       <c r="K6" s="16">
-        <v>384</v>
+        <v>297.5</v>
       </c>
       <c r="L6" s="15">
-        <v>502</v>
+        <v>382.5</v>
       </c>
       <c r="M6" s="16">
-        <v>615</v>
+        <v>461</v>
       </c>
       <c r="N6" s="15">
-        <v>723.5</v>
+        <v>546.5</v>
       </c>
       <c r="O6" s="16">
-        <v>827.5</v>
+        <v>617.5</v>
       </c>
       <c r="P6" s="15">
-        <v>927</v>
+        <v>688.5</v>
       </c>
       <c r="Q6" s="16">
-        <v>1022</v>
+        <v>770.5</v>
       </c>
       <c r="R6" s="15">
-        <v>1112.5</v>
+        <v>830</v>
       </c>
       <c r="S6" s="16">
-        <v>1199</v>
+        <v>896</v>
       </c>
       <c r="T6" s="15">
-        <v>1281.5</v>
+        <v>948.5</v>
       </c>
       <c r="U6" s="16">
-        <v>1360</v>
-      </c>
-      <c r="V6" s="15">
-        <v>1435</v>
-      </c>
-      <c r="W6" s="16">
-        <v>1506.5</v>
-      </c>
-      <c r="X6" s="15">
-        <v>1574.5</v>
-      </c>
-      <c r="Y6" s="16">
-        <v>1639</v>
-      </c>
-      <c r="Z6" s="15">
-        <v>1700</v>
-      </c>
-      <c r="AA6" s="16">
-        <v>1758</v>
+        <v>1008.5</v>
+      </c>
+      <c r="V6" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="W6" s="16" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="X6" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Y6" s="16" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Z6" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AA6" s="16" t="e">
+        <v>#N/A</v>
       </c>
       <c r="AB6" s="16" t="e">
         <v>#N/A</v>
@@ -1382,61 +1382,61 @@
         <v>0</v>
       </c>
       <c r="I7" s="18">
-        <v>686</v>
+        <v>463</v>
       </c>
       <c r="J7" s="18">
-        <v>1346</v>
+        <v>894</v>
       </c>
       <c r="K7" s="18">
-        <v>1980</v>
+        <v>1326</v>
       </c>
       <c r="L7" s="18">
-        <v>2588</v>
+        <v>1753</v>
       </c>
       <c r="M7" s="18">
-        <v>3172</v>
+        <v>2136</v>
       </c>
       <c r="N7" s="18">
-        <v>3731</v>
+        <v>2500</v>
       </c>
       <c r="O7" s="18">
-        <v>4266</v>
+        <v>2858</v>
       </c>
       <c r="P7" s="18">
-        <v>4778</v>
+        <v>3197</v>
       </c>
       <c r="Q7" s="18">
-        <v>5267</v>
+        <v>3501</v>
       </c>
       <c r="R7" s="18">
-        <v>5734</v>
+        <v>3829</v>
       </c>
       <c r="S7" s="18">
-        <v>6180</v>
+        <v>4137</v>
       </c>
       <c r="T7" s="18">
-        <v>6605</v>
+        <v>4411</v>
       </c>
       <c r="U7" s="18">
-        <v>7010</v>
-      </c>
-      <c r="V7" s="18">
-        <v>7396</v>
-      </c>
-      <c r="W7" s="18">
-        <v>7763</v>
-      </c>
-      <c r="X7" s="18">
-        <v>8112</v>
-      </c>
-      <c r="Y7" s="18">
-        <v>8444</v>
-      </c>
-      <c r="Z7" s="18">
-        <v>8760</v>
-      </c>
-      <c r="AA7" s="18">
-        <v>9060</v>
+        <v>4681</v>
+      </c>
+      <c r="V7" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="W7" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="X7" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Y7" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Z7" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="AA7" s="18" t="e">
+        <v>#N/A</v>
       </c>
       <c r="AB7" s="18" t="e">
         <v>#N/A</v>
@@ -1466,13 +1466,13 @@
       </c>
       <c r="B10" s="31">
         <f>+I1</f>
-        <v>100.5</v>
+        <v>149.5</v>
       </c>
       <c r="C10" s="22">
-        <v>4924.5</v>
+        <v>7325.5</v>
       </c>
       <c r="D10" s="25">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="H10" s="13">
         <v>40.49153908138598</v>
@@ -1484,13 +1484,13 @@
       </c>
       <c r="B11" s="31">
         <f t="shared" ref="B11:B15" si="0">+I2</f>
-        <v>100.5</v>
+        <v>149.5</v>
       </c>
       <c r="C11" s="22">
-        <v>3226.6944864000002</v>
+        <v>4799.9087136000007</v>
       </c>
       <c r="D11" s="25">
-        <v>40</v>
+        <v>59</v>
       </c>
       <c r="H11" s="13">
         <v>40.30748663101604</v>
@@ -1502,7 +1502,7 @@
       </c>
       <c r="B12" s="31">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>142.5</v>
       </c>
       <c r="C12" s="22">
         <v>0</v>
@@ -1520,7 +1520,7 @@
       </c>
       <c r="B13" s="31">
         <f t="shared" si="0"/>
-        <v>43</v>
+        <v>142.5</v>
       </c>
       <c r="C13" s="22">
         <v>0</v>
@@ -1538,13 +1538,13 @@
       </c>
       <c r="B14" s="31">
         <f t="shared" si="0"/>
-        <v>133</v>
+        <v>95.5</v>
       </c>
       <c r="C14" s="22">
-        <v>15257.181405312</v>
+        <v>10955.344542912</v>
       </c>
       <c r="D14" s="25">
-        <v>128</v>
+        <v>92</v>
       </c>
       <c r="H14" s="13">
         <v>128.49516129032256</v>
@@ -1556,13 +1556,13 @@
       </c>
       <c r="B15" s="34">
         <f t="shared" si="0"/>
-        <v>133</v>
+        <v>95.5</v>
       </c>
       <c r="C15" s="26">
-        <v>14497</v>
+        <v>10409.5</v>
       </c>
       <c r="D15" s="27">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="H15" s="13">
         <v>116.02240896358543</v>
@@ -1592,79 +1592,79 @@
     <row r="3" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D3" s="13">
         <f>+a!I5*a!$D$5</f>
-        <v>1.1969999999999998</v>
+        <v>0.85949999999999993</v>
       </c>
       <c r="E3" s="13">
         <f>+a!J5*a!$D$5</f>
-        <v>2.3489999999999998</v>
+        <v>1.7639999999999998</v>
       </c>
       <c r="F3" s="13">
         <f>+a!K5*a!$D$5</f>
-        <v>3.4559999999999995</v>
+        <v>2.6774999999999998</v>
       </c>
       <c r="G3" s="13">
         <f>+a!L5*a!$D$5</f>
-        <v>4.5179999999999998</v>
+        <v>3.4424999999999999</v>
       </c>
       <c r="H3" s="13">
         <f>+a!M5*a!$D$5</f>
-        <v>5.5349999999999993</v>
+        <v>4.149</v>
       </c>
       <c r="I3" s="13">
         <f>+a!N5*a!$D$5</f>
-        <v>6.5114999999999998</v>
+        <v>4.9184999999999999</v>
       </c>
       <c r="J3" s="13">
         <f>+a!O5*a!$D$5</f>
-        <v>7.4474999999999998</v>
+        <v>5.5574999999999992</v>
       </c>
       <c r="K3" s="13">
         <f>+a!P5*a!$D$5</f>
-        <v>8.343</v>
+        <v>6.1964999999999995</v>
       </c>
       <c r="L3" s="13">
         <f>+a!Q5*a!$D$5</f>
-        <v>9.1979999999999986</v>
+        <v>6.9344999999999999</v>
       </c>
       <c r="M3" s="13">
         <f>+a!R5*a!$D$5</f>
-        <v>10.012499999999999</v>
+        <v>7.47</v>
       </c>
       <c r="N3" s="13">
         <f>+a!S5*a!$D$5</f>
-        <v>10.790999999999999</v>
+        <v>8.0640000000000001</v>
       </c>
       <c r="O3" s="13">
         <f>+a!T5*a!$D$5</f>
-        <v>11.533499999999998</v>
+        <v>8.5365000000000002</v>
       </c>
       <c r="P3" s="13">
         <f>+a!U5*a!$D$5</f>
-        <v>12.239999999999998</v>
-      </c>
-      <c r="Q3" s="13">
+        <v>9.0764999999999993</v>
+      </c>
+      <c r="Q3" s="13" t="e">
         <f>+a!V5*a!$D$5</f>
-        <v>12.914999999999999</v>
-      </c>
-      <c r="R3" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="R3" s="13" t="e">
         <f>+a!W5*a!$D$5</f>
-        <v>13.558499999999999</v>
-      </c>
-      <c r="S3" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="S3" s="13" t="e">
         <f>+a!X5*a!$D$5</f>
-        <v>14.170499999999999</v>
-      </c>
-      <c r="T3" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="T3" s="13" t="e">
         <f>+a!Y5*a!$D$5</f>
-        <v>14.750999999999999</v>
-      </c>
-      <c r="U3" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="U3" s="13" t="e">
         <f>+a!Z5*a!$D$5</f>
-        <v>15.299999999999999</v>
-      </c>
-      <c r="V3" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="V3" s="13" t="e">
         <f>+a!AA5*a!$D$5</f>
-        <v>15.821999999999999</v>
+        <v>#N/A</v>
       </c>
       <c r="W3" s="13" t="e">
         <f>+a!AB5*a!$D$5</f>
@@ -1678,79 +1678,79 @@
     <row r="4" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D4" s="13">
         <f>+a!I6*a!$D$6</f>
-        <v>16.757999999999999</v>
+        <v>12.032999999999999</v>
       </c>
       <c r="E4" s="13">
         <f>+a!J6*a!$D$6</f>
-        <v>32.886000000000003</v>
+        <v>24.696000000000002</v>
       </c>
       <c r="F4" s="13">
         <f>+a!K6*a!$D$6</f>
-        <v>48.384</v>
+        <v>37.484999999999999</v>
       </c>
       <c r="G4" s="13">
         <f>+a!L6*a!$D$6</f>
-        <v>63.252000000000002</v>
+        <v>48.195</v>
       </c>
       <c r="H4" s="13">
         <f>+a!M6*a!$D$6</f>
-        <v>77.489999999999995</v>
+        <v>58.085999999999999</v>
       </c>
       <c r="I4" s="13">
         <f>+a!N6*a!$D$6</f>
-        <v>91.161000000000001</v>
+        <v>68.858999999999995</v>
       </c>
       <c r="J4" s="13">
         <f>+a!O6*a!$D$6</f>
-        <v>104.265</v>
+        <v>77.805000000000007</v>
       </c>
       <c r="K4" s="13">
         <f>+a!P6*a!$D$6</f>
-        <v>116.80200000000001</v>
+        <v>86.751000000000005</v>
       </c>
       <c r="L4" s="13">
         <f>+a!Q6*a!$D$6</f>
-        <v>128.77199999999999</v>
+        <v>97.082999999999998</v>
       </c>
       <c r="M4" s="13">
         <f>+a!R6*a!$D$6</f>
-        <v>140.17500000000001</v>
+        <v>104.58</v>
       </c>
       <c r="N4" s="13">
         <f>+a!S6*a!$D$6</f>
-        <v>151.07400000000001</v>
+        <v>112.896</v>
       </c>
       <c r="O4" s="13">
         <f>+a!T6*a!$D$6</f>
-        <v>161.46899999999999</v>
+        <v>119.511</v>
       </c>
       <c r="P4" s="13">
         <f>+a!U6*a!$D$6</f>
-        <v>171.36</v>
-      </c>
-      <c r="Q4" s="13">
+        <v>127.071</v>
+      </c>
+      <c r="Q4" s="13" t="e">
         <f>+a!V6*a!$D$6</f>
-        <v>180.81</v>
-      </c>
-      <c r="R4" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="R4" s="13" t="e">
         <f>+a!W6*a!$D$6</f>
-        <v>189.81899999999999</v>
-      </c>
-      <c r="S4" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="S4" s="13" t="e">
         <f>+a!X6*a!$D$6</f>
-        <v>198.387</v>
-      </c>
-      <c r="T4" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="T4" s="13" t="e">
         <f>+a!Y6*a!$D$6</f>
-        <v>206.51400000000001</v>
-      </c>
-      <c r="U4" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="U4" s="13" t="e">
         <f>+a!Z6*a!$D$6</f>
-        <v>214.2</v>
-      </c>
-      <c r="V4" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="V4" s="13" t="e">
         <f>+a!AA6*a!$D$6</f>
-        <v>221.50800000000001</v>
+        <v>#N/A</v>
       </c>
       <c r="W4" s="13" t="e">
         <f>+a!AB6*a!$D$6</f>
@@ -1764,79 +1764,79 @@
     <row r="5" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D5" s="13">
         <f>+a!I1*a!$D$1</f>
-        <v>3.3165</v>
+        <v>4.9335000000000004</v>
       </c>
       <c r="E5" s="13">
         <f>+a!J1*a!$D$1</f>
-        <v>6.5175000000000001</v>
+        <v>9.9329999999999998</v>
       </c>
       <c r="F5" s="13">
         <f>+a!K1*a!$D$1</f>
-        <v>9.5865000000000009</v>
+        <v>14.5365</v>
       </c>
       <c r="G5" s="13">
         <f>+a!L1*a!$D$1</f>
-        <v>12.540000000000001</v>
+        <v>18.612000000000002</v>
       </c>
       <c r="H5" s="13">
         <f>+a!M1*a!$D$1</f>
-        <v>15.361500000000001</v>
+        <v>23.0505</v>
       </c>
       <c r="I5" s="13">
         <f>+a!N1*a!$D$1</f>
-        <v>18.067500000000003</v>
+        <v>27.2745</v>
       </c>
       <c r="J5" s="13">
         <f>+a!O1*a!$D$1</f>
-        <v>20.658000000000001</v>
+        <v>31.432500000000001</v>
       </c>
       <c r="K5" s="13">
         <f>+a!P1*a!$D$1</f>
-        <v>23.133000000000003</v>
+        <v>34.930500000000002</v>
       </c>
       <c r="L5" s="13">
         <f>+a!Q1*a!$D$1</f>
-        <v>25.509</v>
+        <v>38.148000000000003</v>
       </c>
       <c r="M5" s="13">
         <f>+a!R1*a!$D$1</f>
-        <v>27.769500000000001</v>
+        <v>41.728500000000004</v>
       </c>
       <c r="N5" s="13">
         <f>+a!S1*a!$D$1</f>
-        <v>29.931000000000001</v>
+        <v>45.127500000000005</v>
       </c>
       <c r="O5" s="13">
         <f>+a!T1*a!$D$1</f>
-        <v>31.993500000000001</v>
+        <v>48.510000000000005</v>
       </c>
       <c r="P5" s="13">
         <f>+a!U1*a!$D$1</f>
-        <v>33.957000000000001</v>
-      </c>
-      <c r="Q5" s="13">
+        <v>51.265500000000003</v>
+      </c>
+      <c r="Q5" s="13" t="e">
         <f>+a!V1*a!$D$1</f>
-        <v>35.8215</v>
-      </c>
-      <c r="R5" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="R5" s="13" t="e">
         <f>+a!W1*a!$D$1</f>
-        <v>37.603500000000004</v>
-      </c>
-      <c r="S5" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="S5" s="13" t="e">
         <f>+a!X1*a!$D$1</f>
-        <v>39.303000000000004</v>
-      </c>
-      <c r="T5" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="T5" s="13" t="e">
         <f>+a!Y1*a!$D$1</f>
-        <v>40.92</v>
-      </c>
-      <c r="U5" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="U5" s="13" t="e">
         <f>+a!Z1*a!$D$1</f>
-        <v>42.454500000000003</v>
-      </c>
-      <c r="V5" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="V5" s="13" t="e">
         <f>+a!AA1*a!$D$1</f>
-        <v>43.906500000000001</v>
+        <v>#N/A</v>
       </c>
       <c r="W5" s="13" t="e">
         <f>+a!AB1*a!$D$1</f>
@@ -1850,79 +1850,79 @@
     <row r="6" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D6" s="13">
         <f>+a!I2*a!$D$2</f>
-        <v>10.452</v>
+        <v>15.548</v>
       </c>
       <c r="E6" s="13">
         <f>+a!J2*a!$D$2</f>
-        <v>20.54</v>
+        <v>31.303999999999998</v>
       </c>
       <c r="F6" s="13">
         <f>+a!K2*a!$D$2</f>
-        <v>30.212</v>
+        <v>45.811999999999998</v>
       </c>
       <c r="G6" s="13">
         <f>+a!L2*a!$D$2</f>
-        <v>39.519999999999996</v>
+        <v>58.655999999999999</v>
       </c>
       <c r="H6" s="13">
         <f>+a!M2*a!$D$2</f>
-        <v>48.411999999999999</v>
+        <v>72.643999999999991</v>
       </c>
       <c r="I6" s="13">
         <f>+a!N2*a!$D$2</f>
-        <v>56.94</v>
+        <v>85.956000000000003</v>
       </c>
       <c r="J6" s="13">
         <f>+a!O2*a!$D$2</f>
-        <v>65.103999999999999</v>
+        <v>99.06</v>
       </c>
       <c r="K6" s="13">
         <f>+a!P2*a!$D$2</f>
-        <v>72.903999999999996</v>
+        <v>110.08399999999999</v>
       </c>
       <c r="L6" s="13">
         <f>+a!Q2*a!$D$2</f>
-        <v>80.391999999999996</v>
+        <v>120.22399999999999</v>
       </c>
       <c r="M6" s="13">
         <f>+a!R2*a!$D$2</f>
-        <v>87.515999999999991</v>
+        <v>131.50799999999998</v>
       </c>
       <c r="N6" s="13">
         <f>+a!S2*a!$D$2</f>
-        <v>94.327999999999989</v>
+        <v>142.22</v>
       </c>
       <c r="O6" s="13">
         <f>+a!T2*a!$D$2</f>
-        <v>100.82799999999999</v>
+        <v>152.88</v>
       </c>
       <c r="P6" s="13">
         <f>+a!U2*a!$D$2</f>
-        <v>107.01599999999999</v>
-      </c>
-      <c r="Q6" s="13">
+        <v>161.56399999999999</v>
+      </c>
+      <c r="Q6" s="13" t="e">
         <f>+a!V2*a!$D$2</f>
-        <v>112.892</v>
-      </c>
-      <c r="R6" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="R6" s="13" t="e">
         <f>+a!W2*a!$D$2</f>
-        <v>118.508</v>
-      </c>
-      <c r="S6" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="S6" s="13" t="e">
         <f>+a!X2*a!$D$2</f>
-        <v>123.86399999999999</v>
-      </c>
-      <c r="T6" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="T6" s="13" t="e">
         <f>+a!Y2*a!$D$2</f>
-        <v>128.96</v>
-      </c>
-      <c r="U6" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="U6" s="13" t="e">
         <f>+a!Z2*a!$D$2</f>
-        <v>133.79599999999999</v>
-      </c>
-      <c r="V6" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="V6" s="13" t="e">
         <f>+a!AA2*a!$D$2</f>
-        <v>138.37199999999999</v>
+        <v>#N/A</v>
       </c>
       <c r="W6" s="13" t="e">
         <f>+a!AB2*a!$D$2</f>
@@ -1936,79 +1936,79 @@
     <row r="7" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D7" s="13">
         <f>+a!I3*a!$D$3</f>
-        <v>12.040000000000001</v>
+        <v>39.900000000000006</v>
       </c>
       <c r="E7" s="13">
         <f>+a!J3*a!$D$3</f>
-        <v>23.660000000000004</v>
+        <v>75.740000000000009</v>
       </c>
       <c r="F7" s="13">
         <f>+a!K3*a!$D$3</f>
-        <v>34.860000000000007</v>
+        <v>107.94000000000001</v>
       </c>
       <c r="G7" s="13">
         <f>+a!L3*a!$D$3</f>
-        <v>45.640000000000008</v>
+        <v>143.5</v>
       </c>
       <c r="H7" s="13">
         <f>+a!M3*a!$D$3</f>
-        <v>56.000000000000007</v>
+        <v>177.66000000000003</v>
       </c>
       <c r="I7" s="13">
         <f>+a!N3*a!$D$3</f>
-        <v>65.940000000000012</v>
+        <v>208.18</v>
       </c>
       <c r="J7" s="13">
         <f>+a!O3*a!$D$3</f>
-        <v>75.460000000000008</v>
+        <v>238.14000000000001</v>
       </c>
       <c r="K7" s="13">
         <f>+a!P3*a!$D$3</f>
-        <v>84.56</v>
+        <v>270.48</v>
       </c>
       <c r="L7" s="13">
         <f>+a!Q3*a!$D$3</f>
-        <v>93.240000000000009</v>
+        <v>301.28000000000003</v>
       </c>
       <c r="M7" s="13">
         <f>+a!R3*a!$D$3</f>
-        <v>101.50000000000001</v>
+        <v>326.34000000000003</v>
       </c>
       <c r="N7" s="13">
         <f>+a!S3*a!$D$3</f>
-        <v>109.34</v>
+        <v>348.6</v>
       </c>
       <c r="O7" s="13">
         <f>+a!T3*a!$D$3</f>
-        <v>116.9</v>
+        <v>374.22</v>
       </c>
       <c r="P7" s="13">
         <f>+a!U3*a!$D$3</f>
-        <v>124.04</v>
-      </c>
-      <c r="Q7" s="13">
+        <v>398.58000000000004</v>
+      </c>
+      <c r="Q7" s="13" t="e">
         <f>+a!V3*a!$D$3</f>
-        <v>130.9</v>
-      </c>
-      <c r="R7" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="R7" s="13" t="e">
         <f>+a!W3*a!$D$3</f>
-        <v>137.34</v>
-      </c>
-      <c r="S7" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="S7" s="13" t="e">
         <f>+a!X3*a!$D$3</f>
-        <v>143.5</v>
-      </c>
-      <c r="T7" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="T7" s="13" t="e">
         <f>+a!Y3*a!$D$3</f>
-        <v>149.38000000000002</v>
-      </c>
-      <c r="U7" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="U7" s="13" t="e">
         <f>+a!Z3*a!$D$3</f>
-        <v>154.98000000000002</v>
-      </c>
-      <c r="V7" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="V7" s="13" t="e">
         <f>+a!AA3*a!$D$3</f>
-        <v>160.30000000000001</v>
+        <v>#N/A</v>
       </c>
       <c r="W7" s="13" t="e">
         <f>+a!AB3*a!$D$3</f>
@@ -2022,79 +2022,79 @@
     <row r="8" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D8" s="13">
         <f>+a!I4*a!$D$4</f>
-        <v>8.9870000000000001</v>
+        <v>29.782499999999999</v>
       </c>
       <c r="E8" s="13">
         <f>+a!J4*a!$D$4</f>
-        <v>17.660499999999999</v>
+        <v>56.534499999999994</v>
       </c>
       <c r="F8" s="13">
         <f>+a!K4*a!$D$4</f>
-        <v>26.020499999999998</v>
+        <v>80.569499999999991</v>
       </c>
       <c r="G8" s="13">
         <f>+a!L4*a!$D$4</f>
-        <v>34.067</v>
+        <v>107.1125</v>
       </c>
       <c r="H8" s="13">
         <f>+a!M4*a!$D$4</f>
-        <v>41.8</v>
+        <v>132.6105</v>
       </c>
       <c r="I8" s="13">
         <f>+a!N4*a!$D$4</f>
-        <v>49.219499999999996</v>
+        <v>155.39150000000001</v>
       </c>
       <c r="J8" s="13">
         <f>+a!O4*a!$D$4</f>
-        <v>56.325499999999998</v>
+        <v>177.75449999999998</v>
       </c>
       <c r="K8" s="13">
         <f>+a!P4*a!$D$4</f>
-        <v>63.117999999999995</v>
+        <v>201.89400000000001</v>
       </c>
       <c r="L8" s="13">
         <f>+a!Q4*a!$D$4</f>
-        <v>69.596999999999994</v>
+        <v>224.88399999999999</v>
       </c>
       <c r="M8" s="13">
         <f>+a!R4*a!$D$4</f>
-        <v>75.762500000000003</v>
+        <v>243.58949999999999</v>
       </c>
       <c r="N8" s="13">
         <f>+a!S4*a!$D$4</f>
-        <v>81.614499999999992</v>
+        <v>260.20499999999998</v>
       </c>
       <c r="O8" s="13">
         <f>+a!T4*a!$D$4</f>
-        <v>87.257499999999993</v>
+        <v>279.32849999999996</v>
       </c>
       <c r="P8" s="13">
         <f>+a!U4*a!$D$4</f>
-        <v>92.586999999999989</v>
-      </c>
-      <c r="Q8" s="13">
+        <v>297.51150000000001</v>
+      </c>
+      <c r="Q8" s="13" t="e">
         <f>+a!V4*a!$D$4</f>
-        <v>97.707499999999996</v>
-      </c>
-      <c r="R8" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="R8" s="13" t="e">
         <f>+a!W4*a!$D$4</f>
-        <v>102.5145</v>
-      </c>
-      <c r="S8" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="S8" s="13" t="e">
         <f>+a!X4*a!$D$4</f>
-        <v>107.1125</v>
-      </c>
-      <c r="T8" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="T8" s="13" t="e">
         <f>+a!Y4*a!$D$4</f>
-        <v>111.50149999999999</v>
-      </c>
-      <c r="U8" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="U8" s="13" t="e">
         <f>+a!Z4*a!$D$4</f>
-        <v>115.6815</v>
-      </c>
-      <c r="V8" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="V8" s="13" t="e">
         <f>+a!AA4*a!$D$4</f>
-        <v>119.65249999999999</v>
+        <v>#N/A</v>
       </c>
       <c r="W8" s="13" t="e">
         <f>+a!AB4*a!$D$4</f>
@@ -2108,79 +2108,79 @@
     <row r="9" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D9" s="13">
         <f>+a!I7*a!$D$5</f>
-        <v>6.1739999999999995</v>
+        <v>4.1669999999999998</v>
       </c>
       <c r="E9" s="13">
         <f>+a!J7*a!$D$5</f>
-        <v>12.113999999999999</v>
+        <v>8.0459999999999994</v>
       </c>
       <c r="F9" s="13">
         <f>+a!K7*a!$D$5</f>
-        <v>17.82</v>
+        <v>11.933999999999999</v>
       </c>
       <c r="G9" s="13">
         <f>+a!L7*a!$D$5</f>
-        <v>23.291999999999998</v>
+        <v>15.776999999999999</v>
       </c>
       <c r="H9" s="13">
         <f>+a!M7*a!$D$5</f>
-        <v>28.547999999999998</v>
+        <v>19.224</v>
       </c>
       <c r="I9" s="13">
         <f>+a!N7*a!$D$5</f>
-        <v>33.579000000000001</v>
+        <v>22.5</v>
       </c>
       <c r="J9" s="13">
         <f>+a!O7*a!$D$5</f>
-        <v>38.393999999999998</v>
+        <v>25.721999999999998</v>
       </c>
       <c r="K9" s="13">
         <f>+a!P7*a!$D$5</f>
-        <v>43.001999999999995</v>
+        <v>28.772999999999996</v>
       </c>
       <c r="L9" s="13">
         <f>+a!Q7*a!$D$5</f>
-        <v>47.402999999999999</v>
+        <v>31.508999999999997</v>
       </c>
       <c r="M9" s="13">
         <f>+a!R7*a!$D$5</f>
-        <v>51.605999999999995</v>
+        <v>34.460999999999999</v>
       </c>
       <c r="N9" s="13">
         <f>+a!S7*a!$D$5</f>
-        <v>55.62</v>
+        <v>37.232999999999997</v>
       </c>
       <c r="O9" s="13">
         <f>+a!T7*a!$D$5</f>
-        <v>59.444999999999993</v>
+        <v>39.698999999999998</v>
       </c>
       <c r="P9" s="13">
         <f>+a!U7*a!$D$5</f>
-        <v>63.089999999999996</v>
-      </c>
-      <c r="Q9" s="13">
+        <v>42.128999999999998</v>
+      </c>
+      <c r="Q9" s="13" t="e">
         <f>+a!V7*a!$D$5</f>
-        <v>66.563999999999993</v>
-      </c>
-      <c r="R9" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="R9" s="13" t="e">
         <f>+a!W7*a!$D$5</f>
-        <v>69.86699999999999</v>
-      </c>
-      <c r="S9" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="S9" s="13" t="e">
         <f>+a!X7*a!$D$5</f>
-        <v>73.007999999999996</v>
-      </c>
-      <c r="T9" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="T9" s="13" t="e">
         <f>+a!Y7*a!$D$5</f>
-        <v>75.995999999999995</v>
-      </c>
-      <c r="U9" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="U9" s="13" t="e">
         <f>+a!Z7*a!$D$5</f>
-        <v>78.839999999999989</v>
-      </c>
-      <c r="V9" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="V9" s="13" t="e">
         <f>+a!AA7*a!$D$5</f>
-        <v>81.539999999999992</v>
+        <v>#N/A</v>
       </c>
       <c r="W9" s="13" t="e">
         <f>+a!AB7*a!$D$5</f>
@@ -2194,49 +2194,49 @@
     <row r="10" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D10">
         <f>SUM(D3:D8)</f>
-        <v>52.750500000000002</v>
+        <v>103.0565</v>
       </c>
       <c r="E10" s="13">
         <f t="shared" ref="E10:M10" si="1">SUM(E3:E8)</f>
-        <v>103.613</v>
+        <v>199.97149999999999</v>
       </c>
       <c r="F10" s="13">
         <f t="shared" si="1"/>
-        <v>152.51900000000001</v>
+        <v>289.02050000000003</v>
       </c>
       <c r="G10" s="13">
         <f t="shared" si="1"/>
-        <v>199.53700000000001</v>
+        <v>379.51800000000003</v>
       </c>
       <c r="H10" s="13">
         <f t="shared" si="1"/>
-        <v>244.5985</v>
+        <v>468.20000000000005</v>
       </c>
       <c r="I10" s="13">
         <f t="shared" si="1"/>
-        <v>287.83949999999999</v>
+        <v>550.57950000000005</v>
       </c>
       <c r="J10" s="13">
         <f t="shared" si="1"/>
-        <v>329.25999999999993</v>
+        <v>629.74950000000001</v>
       </c>
       <c r="K10" s="13">
         <f t="shared" si="1"/>
-        <v>368.86</v>
+        <v>710.33600000000001</v>
       </c>
       <c r="L10" s="13">
         <f t="shared" si="1"/>
-        <v>406.70799999999997</v>
+        <v>788.55349999999999</v>
       </c>
       <c r="M10" s="13">
         <f t="shared" si="1"/>
-        <v>442.73549999999994</v>
+        <v>855.21600000000012</v>
       </c>
     </row>
     <row r="14" spans="4:24" x14ac:dyDescent="0.25">
       <c r="E14" s="13">
         <f>+a!G5*a!E5*a!I5</f>
-        <v>15257181.405312002</v>
+        <v>10955344.542912001</v>
       </c>
       <c r="G14" s="13">
         <f>+(a!G5+a!H5)*a!$E$7</f>
@@ -2244,13 +2244,13 @@
       </c>
       <c r="H14">
         <f>+E14/G14</f>
-        <v>128.49516129032259</v>
+        <v>92.265322580645162</v>
       </c>
     </row>
     <row r="15" spans="4:24" x14ac:dyDescent="0.25">
       <c r="E15" s="13">
         <f>+a!G6*a!E6*a!I6</f>
-        <v>14497000</v>
+        <v>10409500</v>
       </c>
       <c r="G15" s="13">
         <f>+(a!G6+a!H6)*a!$E$7</f>
@@ -2258,13 +2258,13 @@
       </c>
       <c r="H15" s="13">
         <f t="shared" ref="H15:H19" si="2">+E15/G15</f>
-        <v>116.02240896358543</v>
+        <v>83.309323729491794</v>
       </c>
     </row>
     <row r="16" spans="4:24" x14ac:dyDescent="0.25">
       <c r="E16" s="13">
         <f>+a!G1*a!E1*a!I1</f>
-        <v>4924500</v>
+        <v>7325500</v>
       </c>
       <c r="G16" s="13">
         <f>+(a!G1+a!H1)*a!$E$7</f>
@@ -2272,13 +2272,13 @@
       </c>
       <c r="H16" s="13">
         <f t="shared" si="2"/>
-        <v>40.49153908138598</v>
+        <v>60.233682514101531</v>
       </c>
     </row>
     <row r="17" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E17" s="13">
         <f>+a!G2*a!E2*a!I2</f>
-        <v>3226694.4864000003</v>
+        <v>4799908.7136000004</v>
       </c>
       <c r="G17" s="13">
         <f>+(a!G2+a!H2)*a!$E$7</f>
@@ -2286,7 +2286,7 @@
       </c>
       <c r="H17" s="13">
         <f t="shared" si="2"/>
-        <v>40.30748663101604</v>
+        <v>59.959893048128336</v>
       </c>
     </row>
     <row r="18" spans="5:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modificaciones en la interfaz Grafica por solicitud de la ingeniera Laura inestroza.
</commit_message>
<xml_diff>
--- a/evsim/Impac.Amb..xlsx
+++ b/evsim/Impac.Amb..xlsx
@@ -848,58 +848,58 @@
         <v>22</v>
       </c>
       <c r="I1" s="15">
-        <v>149.5</v>
+        <v>169</v>
       </c>
       <c r="J1" s="15">
-        <v>301</v>
+        <v>329.5</v>
       </c>
       <c r="K1" s="15">
-        <v>440.5</v>
+        <v>491.5</v>
       </c>
       <c r="L1" s="15">
-        <v>564</v>
+        <v>631</v>
       </c>
       <c r="M1" s="15">
-        <v>698.5</v>
+        <v>776.5</v>
       </c>
       <c r="N1" s="15">
-        <v>826.5</v>
+        <v>914</v>
       </c>
       <c r="O1" s="15">
-        <v>952.5</v>
+        <v>1054</v>
       </c>
       <c r="P1" s="15">
-        <v>1058.5</v>
+        <v>1169</v>
       </c>
       <c r="Q1" s="15">
-        <v>1156</v>
+        <v>1283.5</v>
       </c>
       <c r="R1" s="15">
-        <v>1264.5</v>
+        <v>1402</v>
       </c>
       <c r="S1" s="15">
-        <v>1367.5</v>
+        <v>1516.5</v>
       </c>
       <c r="T1" s="15">
-        <v>1470</v>
+        <v>1628</v>
       </c>
       <c r="U1" s="15">
-        <v>1553.5</v>
-      </c>
-      <c r="V1" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="W1" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="X1" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Y1" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Z1" s="15" t="e">
-        <v>#N/A</v>
+        <v>1721</v>
+      </c>
+      <c r="V1" s="15">
+        <v>1811</v>
+      </c>
+      <c r="W1" s="15">
+        <v>1897.5</v>
+      </c>
+      <c r="X1" s="15">
+        <v>1981.5</v>
+      </c>
+      <c r="Y1" s="15">
+        <v>2059</v>
+      </c>
+      <c r="Z1" s="15">
+        <v>2140.5</v>
       </c>
       <c r="AA1" s="15" t="e">
         <v>#N/A</v>
@@ -937,58 +937,58 @@
         <v>61.155072000000004</v>
       </c>
       <c r="I2" s="17">
-        <v>149.5</v>
+        <v>169</v>
       </c>
       <c r="J2" s="15">
-        <v>301</v>
+        <v>329.5</v>
       </c>
       <c r="K2" s="17">
-        <v>440.5</v>
+        <v>491.5</v>
       </c>
       <c r="L2" s="15">
-        <v>564</v>
+        <v>631</v>
       </c>
       <c r="M2" s="17">
-        <v>698.5</v>
+        <v>776.5</v>
       </c>
       <c r="N2" s="15">
-        <v>826.5</v>
+        <v>914</v>
       </c>
       <c r="O2" s="17">
-        <v>952.5</v>
+        <v>1054</v>
       </c>
       <c r="P2" s="15">
-        <v>1058.5</v>
+        <v>1169</v>
       </c>
       <c r="Q2" s="17">
-        <v>1156</v>
+        <v>1283.5</v>
       </c>
       <c r="R2" s="15">
-        <v>1264.5</v>
+        <v>1402</v>
       </c>
       <c r="S2" s="17">
-        <v>1367.5</v>
+        <v>1516.5</v>
       </c>
       <c r="T2" s="15">
-        <v>1470</v>
+        <v>1628</v>
       </c>
       <c r="U2" s="17">
-        <v>1553.5</v>
-      </c>
-      <c r="V2" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="W2" s="17" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="X2" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Y2" s="17" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Z2" s="15" t="e">
-        <v>#N/A</v>
+        <v>1721</v>
+      </c>
+      <c r="V2" s="15">
+        <v>1811</v>
+      </c>
+      <c r="W2" s="17">
+        <v>1897.5</v>
+      </c>
+      <c r="X2" s="15">
+        <v>1981.5</v>
+      </c>
+      <c r="Y2" s="17">
+        <v>2059</v>
+      </c>
+      <c r="Z2" s="15">
+        <v>2140.5</v>
       </c>
       <c r="AA2" s="17" t="e">
         <v>#N/A</v>
@@ -1026,58 +1026,58 @@
         <v>185</v>
       </c>
       <c r="I3" s="18">
-        <v>142.5</v>
+        <v>140</v>
       </c>
       <c r="J3" s="15">
-        <v>270.5</v>
+        <v>267</v>
       </c>
       <c r="K3" s="18">
-        <v>385.5</v>
+        <v>381</v>
       </c>
       <c r="L3" s="15">
-        <v>512.5</v>
+        <v>507.5</v>
       </c>
       <c r="M3" s="18">
-        <v>634.5</v>
+        <v>628.5</v>
       </c>
       <c r="N3" s="15">
-        <v>743.5</v>
+        <v>735.5</v>
       </c>
       <c r="O3" s="18">
-        <v>850.5</v>
+        <v>842</v>
       </c>
       <c r="P3" s="15">
-        <v>966</v>
+        <v>956</v>
       </c>
       <c r="Q3" s="18">
-        <v>1076</v>
+        <v>1064.5</v>
       </c>
       <c r="R3" s="15">
-        <v>1165.5</v>
+        <v>1152.5</v>
       </c>
       <c r="S3" s="18">
-        <v>1245</v>
+        <v>1231.5</v>
       </c>
       <c r="T3" s="15">
-        <v>1336.5</v>
+        <v>1322</v>
       </c>
       <c r="U3" s="18">
-        <v>1423.5</v>
-      </c>
-      <c r="V3" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="W3" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="X3" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Y3" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Z3" s="15" t="e">
-        <v>#N/A</v>
+        <v>1409</v>
+      </c>
+      <c r="V3" s="15">
+        <v>1487</v>
+      </c>
+      <c r="W3" s="18">
+        <v>1560</v>
+      </c>
+      <c r="X3" s="15">
+        <v>1636</v>
+      </c>
+      <c r="Y3" s="18">
+        <v>1707</v>
+      </c>
+      <c r="Z3" s="15">
+        <v>1768.5</v>
       </c>
       <c r="AA3" s="18" t="e">
         <v>#N/A</v>
@@ -1115,58 +1115,58 @@
         <v>141.62227200000001</v>
       </c>
       <c r="I4" s="17">
-        <v>142.5</v>
+        <v>140</v>
       </c>
       <c r="J4" s="15">
-        <v>270.5</v>
+        <v>267</v>
       </c>
       <c r="K4" s="17">
-        <v>385.5</v>
+        <v>381</v>
       </c>
       <c r="L4" s="15">
-        <v>512.5</v>
+        <v>507.5</v>
       </c>
       <c r="M4" s="17">
-        <v>634.5</v>
+        <v>628.5</v>
       </c>
       <c r="N4" s="15">
-        <v>743.5</v>
+        <v>735.5</v>
       </c>
       <c r="O4" s="17">
-        <v>850.5</v>
+        <v>842</v>
       </c>
       <c r="P4" s="15">
-        <v>966</v>
+        <v>956</v>
       </c>
       <c r="Q4" s="17">
-        <v>1076</v>
+        <v>1064.5</v>
       </c>
       <c r="R4" s="15">
-        <v>1165.5</v>
+        <v>1152.5</v>
       </c>
       <c r="S4" s="17">
-        <v>1245</v>
+        <v>1231.5</v>
       </c>
       <c r="T4" s="15">
-        <v>1336.5</v>
+        <v>1322</v>
       </c>
       <c r="U4" s="17">
-        <v>1423.5</v>
-      </c>
-      <c r="V4" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="W4" s="17" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="X4" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Y4" s="17" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Z4" s="15" t="e">
-        <v>#N/A</v>
+        <v>1409</v>
+      </c>
+      <c r="V4" s="15">
+        <v>1487</v>
+      </c>
+      <c r="W4" s="17">
+        <v>1560</v>
+      </c>
+      <c r="X4" s="15">
+        <v>1636</v>
+      </c>
+      <c r="Y4" s="17">
+        <v>1707</v>
+      </c>
+      <c r="Z4" s="15">
+        <v>1768.5</v>
       </c>
       <c r="AA4" s="17" t="e">
         <v>#N/A</v>
@@ -1204,58 +1204,58 @@
         <v>33.796224000000002</v>
       </c>
       <c r="I5" s="15">
-        <v>95.5</v>
+        <v>91.5</v>
       </c>
       <c r="J5" s="15">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="K5" s="15">
-        <v>297.5</v>
+        <v>280.5</v>
       </c>
       <c r="L5" s="15">
-        <v>382.5</v>
+        <v>366</v>
       </c>
       <c r="M5" s="15">
-        <v>461</v>
+        <v>449.5</v>
       </c>
       <c r="N5" s="15">
-        <v>546.5</v>
+        <v>536.5</v>
       </c>
       <c r="O5" s="15">
-        <v>617.5</v>
+        <v>601.5</v>
       </c>
       <c r="P5" s="15">
-        <v>688.5</v>
+        <v>678.5</v>
       </c>
       <c r="Q5" s="15">
-        <v>770.5</v>
+        <v>755.5</v>
       </c>
       <c r="R5" s="15">
-        <v>830</v>
+        <v>814</v>
       </c>
       <c r="S5" s="15">
-        <v>896</v>
+        <v>876.5</v>
       </c>
       <c r="T5" s="15">
-        <v>948.5</v>
+        <v>928.5</v>
       </c>
       <c r="U5" s="15">
-        <v>1008.5</v>
-      </c>
-      <c r="V5" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="W5" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="X5" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Y5" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Z5" s="15" t="e">
-        <v>#N/A</v>
+        <v>986.5</v>
+      </c>
+      <c r="V5" s="15">
+        <v>1042</v>
+      </c>
+      <c r="W5" s="15">
+        <v>1099</v>
+      </c>
+      <c r="X5" s="15">
+        <v>1141</v>
+      </c>
+      <c r="Y5" s="15">
+        <v>1182.5</v>
+      </c>
+      <c r="Z5" s="15">
+        <v>1224.5</v>
       </c>
       <c r="AA5" s="15" t="e">
         <v>#N/A</v>
@@ -1293,58 +1293,58 @@
         <v>50</v>
       </c>
       <c r="I6" s="16">
-        <v>95.5</v>
+        <v>91.5</v>
       </c>
       <c r="J6" s="15">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="K6" s="16">
-        <v>297.5</v>
+        <v>280.5</v>
       </c>
       <c r="L6" s="15">
-        <v>382.5</v>
+        <v>366</v>
       </c>
       <c r="M6" s="16">
-        <v>461</v>
+        <v>449.5</v>
       </c>
       <c r="N6" s="15">
-        <v>546.5</v>
+        <v>536.5</v>
       </c>
       <c r="O6" s="16">
-        <v>617.5</v>
+        <v>601.5</v>
       </c>
       <c r="P6" s="15">
-        <v>688.5</v>
+        <v>678.5</v>
       </c>
       <c r="Q6" s="16">
-        <v>770.5</v>
+        <v>755.5</v>
       </c>
       <c r="R6" s="15">
-        <v>830</v>
+        <v>814</v>
       </c>
       <c r="S6" s="16">
-        <v>896</v>
+        <v>876.5</v>
       </c>
       <c r="T6" s="15">
-        <v>948.5</v>
+        <v>928.5</v>
       </c>
       <c r="U6" s="16">
-        <v>1008.5</v>
-      </c>
-      <c r="V6" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="W6" s="16" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="X6" s="15" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Y6" s="16" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Z6" s="15" t="e">
-        <v>#N/A</v>
+        <v>986.5</v>
+      </c>
+      <c r="V6" s="15">
+        <v>1042</v>
+      </c>
+      <c r="W6" s="16">
+        <v>1099</v>
+      </c>
+      <c r="X6" s="15">
+        <v>1141</v>
+      </c>
+      <c r="Y6" s="16">
+        <v>1182.5</v>
+      </c>
+      <c r="Z6" s="15">
+        <v>1224.5</v>
       </c>
       <c r="AA6" s="16" t="e">
         <v>#N/A</v>
@@ -1382,58 +1382,58 @@
         <v>0</v>
       </c>
       <c r="I7" s="18">
-        <v>463</v>
+        <v>437</v>
       </c>
       <c r="J7" s="18">
-        <v>894</v>
+        <v>852</v>
       </c>
       <c r="K7" s="18">
-        <v>1326</v>
+        <v>1267</v>
       </c>
       <c r="L7" s="18">
-        <v>1753</v>
+        <v>1662</v>
       </c>
       <c r="M7" s="18">
-        <v>2136</v>
+        <v>2015</v>
       </c>
       <c r="N7" s="18">
-        <v>2500</v>
+        <v>2361</v>
       </c>
       <c r="O7" s="18">
-        <v>2858</v>
+        <v>2704</v>
       </c>
       <c r="P7" s="18">
-        <v>3197</v>
+        <v>3016</v>
       </c>
       <c r="Q7" s="18">
-        <v>3501</v>
+        <v>3299</v>
       </c>
       <c r="R7" s="18">
-        <v>3829</v>
+        <v>3612</v>
       </c>
       <c r="S7" s="18">
-        <v>4137</v>
+        <v>3905</v>
       </c>
       <c r="T7" s="18">
-        <v>4411</v>
+        <v>4164</v>
       </c>
       <c r="U7" s="18">
-        <v>4681</v>
-      </c>
-      <c r="V7" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="W7" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="X7" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Y7" s="18" t="e">
-        <v>#N/A</v>
-      </c>
-      <c r="Z7" s="18" t="e">
-        <v>#N/A</v>
+        <v>4419</v>
+      </c>
+      <c r="V7" s="18">
+        <v>4668</v>
+      </c>
+      <c r="W7" s="18">
+        <v>4898</v>
+      </c>
+      <c r="X7" s="18">
+        <v>5124</v>
+      </c>
+      <c r="Y7" s="18">
+        <v>5343</v>
+      </c>
+      <c r="Z7" s="18">
+        <v>5542</v>
       </c>
       <c r="AA7" s="18" t="e">
         <v>#N/A</v>
@@ -1466,13 +1466,13 @@
       </c>
       <c r="B10" s="31">
         <f>+I1</f>
-        <v>149.5</v>
+        <v>169</v>
       </c>
       <c r="C10" s="22">
-        <v>7325.5</v>
+        <v>8281</v>
       </c>
       <c r="D10" s="25">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="H10" s="13">
         <v>40.49153908138598</v>
@@ -1484,13 +1484,13 @@
       </c>
       <c r="B11" s="31">
         <f t="shared" ref="B11:B15" si="0">+I2</f>
-        <v>149.5</v>
+        <v>169</v>
       </c>
       <c r="C11" s="22">
-        <v>4799.9087136000007</v>
+        <v>5425.9837632000008</v>
       </c>
       <c r="D11" s="25">
-        <v>59</v>
+        <v>67</v>
       </c>
       <c r="H11" s="13">
         <v>40.30748663101604</v>
@@ -1502,7 +1502,7 @@
       </c>
       <c r="B12" s="31">
         <f t="shared" si="0"/>
-        <v>142.5</v>
+        <v>140</v>
       </c>
       <c r="C12" s="22">
         <v>0</v>
@@ -1520,7 +1520,7 @@
       </c>
       <c r="B13" s="31">
         <f t="shared" si="0"/>
-        <v>142.5</v>
+        <v>140</v>
       </c>
       <c r="C13" s="22">
         <v>0</v>
@@ -1538,13 +1538,13 @@
       </c>
       <c r="B14" s="31">
         <f t="shared" si="0"/>
-        <v>95.5</v>
+        <v>91.5</v>
       </c>
       <c r="C14" s="22">
-        <v>10955.344542912</v>
+        <v>10496.481944256</v>
       </c>
       <c r="D14" s="25">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H14" s="13">
         <v>128.49516129032256</v>
@@ -1556,13 +1556,13 @@
       </c>
       <c r="B15" s="34">
         <f t="shared" si="0"/>
-        <v>95.5</v>
+        <v>91.5</v>
       </c>
       <c r="C15" s="26">
-        <v>10409.5</v>
+        <v>9973.5</v>
       </c>
       <c r="D15" s="27">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H15" s="13">
         <v>116.02240896358543</v>
@@ -1592,75 +1592,75 @@
     <row r="3" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D3" s="13">
         <f>+a!I5*a!$D$5</f>
-        <v>0.85949999999999993</v>
+        <v>0.8234999999999999</v>
       </c>
       <c r="E3" s="13">
         <f>+a!J5*a!$D$5</f>
-        <v>1.7639999999999998</v>
+        <v>1.7279999999999998</v>
       </c>
       <c r="F3" s="13">
         <f>+a!K5*a!$D$5</f>
-        <v>2.6774999999999998</v>
+        <v>2.5244999999999997</v>
       </c>
       <c r="G3" s="13">
         <f>+a!L5*a!$D$5</f>
-        <v>3.4424999999999999</v>
+        <v>3.2939999999999996</v>
       </c>
       <c r="H3" s="13">
         <f>+a!M5*a!$D$5</f>
-        <v>4.149</v>
+        <v>4.0454999999999997</v>
       </c>
       <c r="I3" s="13">
         <f>+a!N5*a!$D$5</f>
-        <v>4.9184999999999999</v>
+        <v>4.8285</v>
       </c>
       <c r="J3" s="13">
         <f>+a!O5*a!$D$5</f>
-        <v>5.5574999999999992</v>
+        <v>5.4135</v>
       </c>
       <c r="K3" s="13">
         <f>+a!P5*a!$D$5</f>
-        <v>6.1964999999999995</v>
+        <v>6.1064999999999996</v>
       </c>
       <c r="L3" s="13">
         <f>+a!Q5*a!$D$5</f>
-        <v>6.9344999999999999</v>
+        <v>6.7994999999999992</v>
       </c>
       <c r="M3" s="13">
         <f>+a!R5*a!$D$5</f>
-        <v>7.47</v>
+        <v>7.3259999999999996</v>
       </c>
       <c r="N3" s="13">
         <f>+a!S5*a!$D$5</f>
-        <v>8.0640000000000001</v>
+        <v>7.8884999999999996</v>
       </c>
       <c r="O3" s="13">
         <f>+a!T5*a!$D$5</f>
-        <v>8.5365000000000002</v>
+        <v>8.3564999999999987</v>
       </c>
       <c r="P3" s="13">
         <f>+a!U5*a!$D$5</f>
-        <v>9.0764999999999993</v>
-      </c>
-      <c r="Q3" s="13" t="e">
+        <v>8.8784999999999989</v>
+      </c>
+      <c r="Q3" s="13">
         <f>+a!V5*a!$D$5</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R3" s="13" t="e">
+        <v>9.3780000000000001</v>
+      </c>
+      <c r="R3" s="13">
         <f>+a!W5*a!$D$5</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S3" s="13" t="e">
+        <v>9.891</v>
+      </c>
+      <c r="S3" s="13">
         <f>+a!X5*a!$D$5</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T3" s="13" t="e">
+        <v>10.268999999999998</v>
+      </c>
+      <c r="T3" s="13">
         <f>+a!Y5*a!$D$5</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U3" s="13" t="e">
+        <v>10.6425</v>
+      </c>
+      <c r="U3" s="13">
         <f>+a!Z5*a!$D$5</f>
-        <v>#N/A</v>
+        <v>11.020499999999998</v>
       </c>
       <c r="V3" s="13" t="e">
         <f>+a!AA5*a!$D$5</f>
@@ -1678,75 +1678,75 @@
     <row r="4" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D4" s="13">
         <f>+a!I6*a!$D$6</f>
-        <v>12.032999999999999</v>
+        <v>11.529</v>
       </c>
       <c r="E4" s="13">
         <f>+a!J6*a!$D$6</f>
-        <v>24.696000000000002</v>
+        <v>24.192</v>
       </c>
       <c r="F4" s="13">
         <f>+a!K6*a!$D$6</f>
-        <v>37.484999999999999</v>
+        <v>35.343000000000004</v>
       </c>
       <c r="G4" s="13">
         <f>+a!L6*a!$D$6</f>
-        <v>48.195</v>
+        <v>46.116</v>
       </c>
       <c r="H4" s="13">
         <f>+a!M6*a!$D$6</f>
-        <v>58.085999999999999</v>
+        <v>56.637</v>
       </c>
       <c r="I4" s="13">
         <f>+a!N6*a!$D$6</f>
-        <v>68.858999999999995</v>
+        <v>67.599000000000004</v>
       </c>
       <c r="J4" s="13">
         <f>+a!O6*a!$D$6</f>
-        <v>77.805000000000007</v>
+        <v>75.789000000000001</v>
       </c>
       <c r="K4" s="13">
         <f>+a!P6*a!$D$6</f>
-        <v>86.751000000000005</v>
+        <v>85.491</v>
       </c>
       <c r="L4" s="13">
         <f>+a!Q6*a!$D$6</f>
-        <v>97.082999999999998</v>
+        <v>95.192999999999998</v>
       </c>
       <c r="M4" s="13">
         <f>+a!R6*a!$D$6</f>
-        <v>104.58</v>
+        <v>102.56400000000001</v>
       </c>
       <c r="N4" s="13">
         <f>+a!S6*a!$D$6</f>
-        <v>112.896</v>
+        <v>110.43900000000001</v>
       </c>
       <c r="O4" s="13">
         <f>+a!T6*a!$D$6</f>
-        <v>119.511</v>
+        <v>116.991</v>
       </c>
       <c r="P4" s="13">
         <f>+a!U6*a!$D$6</f>
-        <v>127.071</v>
-      </c>
-      <c r="Q4" s="13" t="e">
+        <v>124.29900000000001</v>
+      </c>
+      <c r="Q4" s="13">
         <f>+a!V6*a!$D$6</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R4" s="13" t="e">
+        <v>131.292</v>
+      </c>
+      <c r="R4" s="13">
         <f>+a!W6*a!$D$6</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S4" s="13" t="e">
+        <v>138.47399999999999</v>
+      </c>
+      <c r="S4" s="13">
         <f>+a!X6*a!$D$6</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T4" s="13" t="e">
+        <v>143.76599999999999</v>
+      </c>
+      <c r="T4" s="13">
         <f>+a!Y6*a!$D$6</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U4" s="13" t="e">
+        <v>148.995</v>
+      </c>
+      <c r="U4" s="13">
         <f>+a!Z6*a!$D$6</f>
-        <v>#N/A</v>
+        <v>154.28700000000001</v>
       </c>
       <c r="V4" s="13" t="e">
         <f>+a!AA6*a!$D$6</f>
@@ -1764,75 +1764,75 @@
     <row r="5" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D5" s="13">
         <f>+a!I1*a!$D$1</f>
-        <v>4.9335000000000004</v>
+        <v>5.577</v>
       </c>
       <c r="E5" s="13">
         <f>+a!J1*a!$D$1</f>
-        <v>9.9329999999999998</v>
+        <v>10.8735</v>
       </c>
       <c r="F5" s="13">
         <f>+a!K1*a!$D$1</f>
-        <v>14.5365</v>
+        <v>16.2195</v>
       </c>
       <c r="G5" s="13">
         <f>+a!L1*a!$D$1</f>
-        <v>18.612000000000002</v>
+        <v>20.823</v>
       </c>
       <c r="H5" s="13">
         <f>+a!M1*a!$D$1</f>
-        <v>23.0505</v>
+        <v>25.624500000000001</v>
       </c>
       <c r="I5" s="13">
         <f>+a!N1*a!$D$1</f>
-        <v>27.2745</v>
+        <v>30.162000000000003</v>
       </c>
       <c r="J5" s="13">
         <f>+a!O1*a!$D$1</f>
-        <v>31.432500000000001</v>
+        <v>34.782000000000004</v>
       </c>
       <c r="K5" s="13">
         <f>+a!P1*a!$D$1</f>
-        <v>34.930500000000002</v>
+        <v>38.577000000000005</v>
       </c>
       <c r="L5" s="13">
         <f>+a!Q1*a!$D$1</f>
-        <v>38.148000000000003</v>
+        <v>42.355499999999999</v>
       </c>
       <c r="M5" s="13">
         <f>+a!R1*a!$D$1</f>
-        <v>41.728500000000004</v>
+        <v>46.266000000000005</v>
       </c>
       <c r="N5" s="13">
         <f>+a!S1*a!$D$1</f>
-        <v>45.127500000000005</v>
+        <v>50.044499999999999</v>
       </c>
       <c r="O5" s="13">
         <f>+a!T1*a!$D$1</f>
-        <v>48.510000000000005</v>
+        <v>53.724000000000004</v>
       </c>
       <c r="P5" s="13">
         <f>+a!U1*a!$D$1</f>
-        <v>51.265500000000003</v>
-      </c>
-      <c r="Q5" s="13" t="e">
+        <v>56.792999999999999</v>
+      </c>
+      <c r="Q5" s="13">
         <f>+a!V1*a!$D$1</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R5" s="13" t="e">
+        <v>59.763000000000005</v>
+      </c>
+      <c r="R5" s="13">
         <f>+a!W1*a!$D$1</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S5" s="13" t="e">
+        <v>62.6175</v>
+      </c>
+      <c r="S5" s="13">
         <f>+a!X1*a!$D$1</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T5" s="13" t="e">
+        <v>65.389499999999998</v>
+      </c>
+      <c r="T5" s="13">
         <f>+a!Y1*a!$D$1</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U5" s="13" t="e">
+        <v>67.947000000000003</v>
+      </c>
+      <c r="U5" s="13">
         <f>+a!Z1*a!$D$1</f>
-        <v>#N/A</v>
+        <v>70.636499999999998</v>
       </c>
       <c r="V5" s="13" t="e">
         <f>+a!AA1*a!$D$1</f>
@@ -1850,75 +1850,75 @@
     <row r="6" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D6" s="13">
         <f>+a!I2*a!$D$2</f>
-        <v>15.548</v>
+        <v>17.576000000000001</v>
       </c>
       <c r="E6" s="13">
         <f>+a!J2*a!$D$2</f>
-        <v>31.303999999999998</v>
+        <v>34.268000000000001</v>
       </c>
       <c r="F6" s="13">
         <f>+a!K2*a!$D$2</f>
-        <v>45.811999999999998</v>
+        <v>51.116</v>
       </c>
       <c r="G6" s="13">
         <f>+a!L2*a!$D$2</f>
-        <v>58.655999999999999</v>
+        <v>65.623999999999995</v>
       </c>
       <c r="H6" s="13">
         <f>+a!M2*a!$D$2</f>
-        <v>72.643999999999991</v>
+        <v>80.756</v>
       </c>
       <c r="I6" s="13">
         <f>+a!N2*a!$D$2</f>
-        <v>85.956000000000003</v>
+        <v>95.055999999999997</v>
       </c>
       <c r="J6" s="13">
         <f>+a!O2*a!$D$2</f>
-        <v>99.06</v>
+        <v>109.616</v>
       </c>
       <c r="K6" s="13">
         <f>+a!P2*a!$D$2</f>
-        <v>110.08399999999999</v>
+        <v>121.57599999999999</v>
       </c>
       <c r="L6" s="13">
         <f>+a!Q2*a!$D$2</f>
-        <v>120.22399999999999</v>
+        <v>133.48399999999998</v>
       </c>
       <c r="M6" s="13">
         <f>+a!R2*a!$D$2</f>
-        <v>131.50799999999998</v>
+        <v>145.80799999999999</v>
       </c>
       <c r="N6" s="13">
         <f>+a!S2*a!$D$2</f>
-        <v>142.22</v>
+        <v>157.71599999999998</v>
       </c>
       <c r="O6" s="13">
         <f>+a!T2*a!$D$2</f>
-        <v>152.88</v>
+        <v>169.31199999999998</v>
       </c>
       <c r="P6" s="13">
         <f>+a!U2*a!$D$2</f>
-        <v>161.56399999999999</v>
-      </c>
-      <c r="Q6" s="13" t="e">
+        <v>178.98399999999998</v>
+      </c>
+      <c r="Q6" s="13">
         <f>+a!V2*a!$D$2</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R6" s="13" t="e">
+        <v>188.34399999999999</v>
+      </c>
+      <c r="R6" s="13">
         <f>+a!W2*a!$D$2</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S6" s="13" t="e">
+        <v>197.34</v>
+      </c>
+      <c r="S6" s="13">
         <f>+a!X2*a!$D$2</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T6" s="13" t="e">
+        <v>206.07599999999999</v>
+      </c>
+      <c r="T6" s="13">
         <f>+a!Y2*a!$D$2</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U6" s="13" t="e">
+        <v>214.136</v>
+      </c>
+      <c r="U6" s="13">
         <f>+a!Z2*a!$D$2</f>
-        <v>#N/A</v>
+        <v>222.61199999999999</v>
       </c>
       <c r="V6" s="13" t="e">
         <f>+a!AA2*a!$D$2</f>
@@ -1936,75 +1936,75 @@
     <row r="7" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D7" s="13">
         <f>+a!I3*a!$D$3</f>
-        <v>39.900000000000006</v>
+        <v>39.200000000000003</v>
       </c>
       <c r="E7" s="13">
         <f>+a!J3*a!$D$3</f>
-        <v>75.740000000000009</v>
+        <v>74.760000000000005</v>
       </c>
       <c r="F7" s="13">
         <f>+a!K3*a!$D$3</f>
-        <v>107.94000000000001</v>
+        <v>106.68</v>
       </c>
       <c r="G7" s="13">
         <f>+a!L3*a!$D$3</f>
-        <v>143.5</v>
+        <v>142.10000000000002</v>
       </c>
       <c r="H7" s="13">
         <f>+a!M3*a!$D$3</f>
-        <v>177.66000000000003</v>
+        <v>175.98000000000002</v>
       </c>
       <c r="I7" s="13">
         <f>+a!N3*a!$D$3</f>
-        <v>208.18</v>
+        <v>205.94000000000003</v>
       </c>
       <c r="J7" s="13">
         <f>+a!O3*a!$D$3</f>
-        <v>238.14000000000001</v>
+        <v>235.76000000000002</v>
       </c>
       <c r="K7" s="13">
         <f>+a!P3*a!$D$3</f>
-        <v>270.48</v>
+        <v>267.68</v>
       </c>
       <c r="L7" s="13">
         <f>+a!Q3*a!$D$3</f>
-        <v>301.28000000000003</v>
+        <v>298.06</v>
       </c>
       <c r="M7" s="13">
         <f>+a!R3*a!$D$3</f>
-        <v>326.34000000000003</v>
+        <v>322.70000000000005</v>
       </c>
       <c r="N7" s="13">
         <f>+a!S3*a!$D$3</f>
-        <v>348.6</v>
+        <v>344.82000000000005</v>
       </c>
       <c r="O7" s="13">
         <f>+a!T3*a!$D$3</f>
-        <v>374.22</v>
+        <v>370.16</v>
       </c>
       <c r="P7" s="13">
         <f>+a!U3*a!$D$3</f>
-        <v>398.58000000000004</v>
-      </c>
-      <c r="Q7" s="13" t="e">
+        <v>394.52000000000004</v>
+      </c>
+      <c r="Q7" s="13">
         <f>+a!V3*a!$D$3</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R7" s="13" t="e">
+        <v>416.36</v>
+      </c>
+      <c r="R7" s="13">
         <f>+a!W3*a!$D$3</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S7" s="13" t="e">
+        <v>436.80000000000007</v>
+      </c>
+      <c r="S7" s="13">
         <f>+a!X3*a!$D$3</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T7" s="13" t="e">
+        <v>458.08000000000004</v>
+      </c>
+      <c r="T7" s="13">
         <f>+a!Y3*a!$D$3</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U7" s="13" t="e">
+        <v>477.96000000000004</v>
+      </c>
+      <c r="U7" s="13">
         <f>+a!Z3*a!$D$3</f>
-        <v>#N/A</v>
+        <v>495.18000000000006</v>
       </c>
       <c r="V7" s="13" t="e">
         <f>+a!AA3*a!$D$3</f>
@@ -2022,75 +2022,75 @@
     <row r="8" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D8" s="13">
         <f>+a!I4*a!$D$4</f>
-        <v>29.782499999999999</v>
+        <v>29.259999999999998</v>
       </c>
       <c r="E8" s="13">
         <f>+a!J4*a!$D$4</f>
-        <v>56.534499999999994</v>
+        <v>55.802999999999997</v>
       </c>
       <c r="F8" s="13">
         <f>+a!K4*a!$D$4</f>
-        <v>80.569499999999991</v>
+        <v>79.628999999999991</v>
       </c>
       <c r="G8" s="13">
         <f>+a!L4*a!$D$4</f>
-        <v>107.1125</v>
+        <v>106.0675</v>
       </c>
       <c r="H8" s="13">
         <f>+a!M4*a!$D$4</f>
-        <v>132.6105</v>
+        <v>131.35649999999998</v>
       </c>
       <c r="I8" s="13">
         <f>+a!N4*a!$D$4</f>
-        <v>155.39150000000001</v>
+        <v>153.71949999999998</v>
       </c>
       <c r="J8" s="13">
         <f>+a!O4*a!$D$4</f>
-        <v>177.75449999999998</v>
+        <v>175.97799999999998</v>
       </c>
       <c r="K8" s="13">
         <f>+a!P4*a!$D$4</f>
-        <v>201.89400000000001</v>
+        <v>199.804</v>
       </c>
       <c r="L8" s="13">
         <f>+a!Q4*a!$D$4</f>
-        <v>224.88399999999999</v>
+        <v>222.48049999999998</v>
       </c>
       <c r="M8" s="13">
         <f>+a!R4*a!$D$4</f>
-        <v>243.58949999999999</v>
+        <v>240.8725</v>
       </c>
       <c r="N8" s="13">
         <f>+a!S4*a!$D$4</f>
-        <v>260.20499999999998</v>
+        <v>257.38349999999997</v>
       </c>
       <c r="O8" s="13">
         <f>+a!T4*a!$D$4</f>
-        <v>279.32849999999996</v>
+        <v>276.298</v>
       </c>
       <c r="P8" s="13">
         <f>+a!U4*a!$D$4</f>
-        <v>297.51150000000001</v>
-      </c>
-      <c r="Q8" s="13" t="e">
+        <v>294.48099999999999</v>
+      </c>
+      <c r="Q8" s="13">
         <f>+a!V4*a!$D$4</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R8" s="13" t="e">
+        <v>310.78300000000002</v>
+      </c>
+      <c r="R8" s="13">
         <f>+a!W4*a!$D$4</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S8" s="13" t="e">
+        <v>326.03999999999996</v>
+      </c>
+      <c r="S8" s="13">
         <f>+a!X4*a!$D$4</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T8" s="13" t="e">
+        <v>341.92399999999998</v>
+      </c>
+      <c r="T8" s="13">
         <f>+a!Y4*a!$D$4</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U8" s="13" t="e">
+        <v>356.76299999999998</v>
+      </c>
+      <c r="U8" s="13">
         <f>+a!Z4*a!$D$4</f>
-        <v>#N/A</v>
+        <v>369.61649999999997</v>
       </c>
       <c r="V8" s="13" t="e">
         <f>+a!AA4*a!$D$4</f>
@@ -2108,75 +2108,75 @@
     <row r="9" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D9" s="13">
         <f>+a!I7*a!$D$5</f>
-        <v>4.1669999999999998</v>
+        <v>3.9329999999999998</v>
       </c>
       <c r="E9" s="13">
         <f>+a!J7*a!$D$5</f>
-        <v>8.0459999999999994</v>
+        <v>7.6679999999999993</v>
       </c>
       <c r="F9" s="13">
         <f>+a!K7*a!$D$5</f>
-        <v>11.933999999999999</v>
+        <v>11.402999999999999</v>
       </c>
       <c r="G9" s="13">
         <f>+a!L7*a!$D$5</f>
-        <v>15.776999999999999</v>
+        <v>14.957999999999998</v>
       </c>
       <c r="H9" s="13">
         <f>+a!M7*a!$D$5</f>
-        <v>19.224</v>
+        <v>18.134999999999998</v>
       </c>
       <c r="I9" s="13">
         <f>+a!N7*a!$D$5</f>
-        <v>22.5</v>
+        <v>21.248999999999999</v>
       </c>
       <c r="J9" s="13">
         <f>+a!O7*a!$D$5</f>
-        <v>25.721999999999998</v>
+        <v>24.335999999999999</v>
       </c>
       <c r="K9" s="13">
         <f>+a!P7*a!$D$5</f>
-        <v>28.772999999999996</v>
+        <v>27.143999999999998</v>
       </c>
       <c r="L9" s="13">
         <f>+a!Q7*a!$D$5</f>
-        <v>31.508999999999997</v>
+        <v>29.690999999999999</v>
       </c>
       <c r="M9" s="13">
         <f>+a!R7*a!$D$5</f>
-        <v>34.460999999999999</v>
+        <v>32.507999999999996</v>
       </c>
       <c r="N9" s="13">
         <f>+a!S7*a!$D$5</f>
-        <v>37.232999999999997</v>
+        <v>35.144999999999996</v>
       </c>
       <c r="O9" s="13">
         <f>+a!T7*a!$D$5</f>
-        <v>39.698999999999998</v>
+        <v>37.475999999999999</v>
       </c>
       <c r="P9" s="13">
         <f>+a!U7*a!$D$5</f>
-        <v>42.128999999999998</v>
-      </c>
-      <c r="Q9" s="13" t="e">
+        <v>39.770999999999994</v>
+      </c>
+      <c r="Q9" s="13">
         <f>+a!V7*a!$D$5</f>
-        <v>#N/A</v>
-      </c>
-      <c r="R9" s="13" t="e">
+        <v>42.011999999999993</v>
+      </c>
+      <c r="R9" s="13">
         <f>+a!W7*a!$D$5</f>
-        <v>#N/A</v>
-      </c>
-      <c r="S9" s="13" t="e">
+        <v>44.081999999999994</v>
+      </c>
+      <c r="S9" s="13">
         <f>+a!X7*a!$D$5</f>
-        <v>#N/A</v>
-      </c>
-      <c r="T9" s="13" t="e">
+        <v>46.116</v>
+      </c>
+      <c r="T9" s="13">
         <f>+a!Y7*a!$D$5</f>
-        <v>#N/A</v>
-      </c>
-      <c r="U9" s="13" t="e">
+        <v>48.086999999999996</v>
+      </c>
+      <c r="U9" s="13">
         <f>+a!Z7*a!$D$5</f>
-        <v>#N/A</v>
+        <v>49.877999999999993</v>
       </c>
       <c r="V9" s="13" t="e">
         <f>+a!AA7*a!$D$5</f>
@@ -2194,49 +2194,49 @@
     <row r="10" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D10">
         <f>SUM(D3:D8)</f>
-        <v>103.0565</v>
+        <v>103.96549999999999</v>
       </c>
       <c r="E10" s="13">
         <f t="shared" ref="E10:M10" si="1">SUM(E3:E8)</f>
-        <v>199.97149999999999</v>
+        <v>201.62450000000001</v>
       </c>
       <c r="F10" s="13">
         <f t="shared" si="1"/>
-        <v>289.02050000000003</v>
+        <v>291.512</v>
       </c>
       <c r="G10" s="13">
         <f t="shared" si="1"/>
-        <v>379.51800000000003</v>
+        <v>384.02449999999999</v>
       </c>
       <c r="H10" s="13">
         <f t="shared" si="1"/>
-        <v>468.20000000000005</v>
+        <v>474.39949999999999</v>
       </c>
       <c r="I10" s="13">
         <f t="shared" si="1"/>
-        <v>550.57950000000005</v>
+        <v>557.30500000000006</v>
       </c>
       <c r="J10" s="13">
         <f t="shared" si="1"/>
-        <v>629.74950000000001</v>
+        <v>637.33849999999995</v>
       </c>
       <c r="K10" s="13">
         <f t="shared" si="1"/>
-        <v>710.33600000000001</v>
+        <v>719.23449999999991</v>
       </c>
       <c r="L10" s="13">
         <f t="shared" si="1"/>
-        <v>788.55349999999999</v>
+        <v>798.37250000000006</v>
       </c>
       <c r="M10" s="13">
         <f t="shared" si="1"/>
-        <v>855.21600000000012</v>
+        <v>865.53649999999993</v>
       </c>
     </row>
     <row r="14" spans="4:24" x14ac:dyDescent="0.25">
       <c r="E14" s="13">
         <f>+a!G5*a!E5*a!I5</f>
-        <v>10955344.542912001</v>
+        <v>10496481.944256</v>
       </c>
       <c r="G14" s="13">
         <f>+(a!G5+a!H5)*a!$E$7</f>
@@ -2244,13 +2244,13 @@
       </c>
       <c r="H14">
         <f>+E14/G14</f>
-        <v>92.265322580645162</v>
+        <v>88.400806451612894</v>
       </c>
     </row>
     <row r="15" spans="4:24" x14ac:dyDescent="0.25">
       <c r="E15" s="13">
         <f>+a!G6*a!E6*a!I6</f>
-        <v>10409500</v>
+        <v>9973500</v>
       </c>
       <c r="G15" s="13">
         <f>+(a!G6+a!H6)*a!$E$7</f>
@@ -2258,13 +2258,13 @@
       </c>
       <c r="H15" s="13">
         <f t="shared" ref="H15:H19" si="2">+E15/G15</f>
-        <v>83.309323729491794</v>
+        <v>79.819927971188477</v>
       </c>
     </row>
     <row r="16" spans="4:24" x14ac:dyDescent="0.25">
       <c r="E16" s="13">
         <f>+a!G1*a!E1*a!I1</f>
-        <v>7325500</v>
+        <v>8281000</v>
       </c>
       <c r="G16" s="13">
         <f>+(a!G1+a!H1)*a!$E$7</f>
@@ -2272,13 +2272,13 @@
       </c>
       <c r="H16" s="13">
         <f t="shared" si="2"/>
-        <v>60.233682514101531</v>
+        <v>68.09024979854955</v>
       </c>
     </row>
     <row r="17" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E17" s="13">
         <f>+a!G2*a!E2*a!I2</f>
-        <v>4799908.7136000004</v>
+        <v>5425983.7631999999</v>
       </c>
       <c r="G17" s="13">
         <f>+(a!G2+a!H2)*a!$E$7</f>
@@ -2286,7 +2286,7 @@
       </c>
       <c r="H17" s="13">
         <f t="shared" si="2"/>
-        <v>59.959893048128336</v>
+        <v>67.780748663101591</v>
       </c>
     </row>
     <row r="18" spans="5:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Se agregaron las graficas de la profesora laura inestroza
</commit_message>
<xml_diff>
--- a/evsim/Impac.Amb..xlsx
+++ b/evsim/Impac.Amb..xlsx
@@ -848,58 +848,58 @@
         <v>22</v>
       </c>
       <c r="I1" s="15">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="J1" s="15">
-        <v>329.5</v>
+        <v>304</v>
       </c>
       <c r="K1" s="15">
-        <v>491.5</v>
+        <v>453</v>
       </c>
       <c r="L1" s="15">
-        <v>631</v>
+        <v>582</v>
       </c>
       <c r="M1" s="15">
-        <v>776.5</v>
+        <v>721.5</v>
       </c>
       <c r="N1" s="15">
-        <v>914</v>
+        <v>845.5</v>
       </c>
       <c r="O1" s="15">
-        <v>1054</v>
+        <v>974</v>
       </c>
       <c r="P1" s="15">
-        <v>1169</v>
+        <v>1081.5</v>
       </c>
       <c r="Q1" s="15">
-        <v>1283.5</v>
+        <v>1186</v>
       </c>
       <c r="R1" s="15">
-        <v>1402</v>
+        <v>1298</v>
       </c>
       <c r="S1" s="15">
-        <v>1516.5</v>
+        <v>1409.5</v>
       </c>
       <c r="T1" s="15">
-        <v>1628</v>
+        <v>1515.5</v>
       </c>
       <c r="U1" s="15">
-        <v>1721</v>
-      </c>
-      <c r="V1" s="15">
-        <v>1811</v>
-      </c>
-      <c r="W1" s="15">
-        <v>1897.5</v>
-      </c>
-      <c r="X1" s="15">
-        <v>1981.5</v>
-      </c>
-      <c r="Y1" s="15">
-        <v>2059</v>
-      </c>
-      <c r="Z1" s="15">
-        <v>2140.5</v>
+        <v>1602</v>
+      </c>
+      <c r="V1" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="W1" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="X1" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Y1" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Z1" s="15" t="e">
+        <v>#N/A</v>
       </c>
       <c r="AA1" s="15" t="e">
         <v>#N/A</v>
@@ -937,58 +937,58 @@
         <v>61.155072000000004</v>
       </c>
       <c r="I2" s="17">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="J2" s="15">
-        <v>329.5</v>
+        <v>304</v>
       </c>
       <c r="K2" s="17">
-        <v>491.5</v>
+        <v>453</v>
       </c>
       <c r="L2" s="15">
-        <v>631</v>
+        <v>582</v>
       </c>
       <c r="M2" s="17">
-        <v>776.5</v>
+        <v>721.5</v>
       </c>
       <c r="N2" s="15">
-        <v>914</v>
+        <v>845.5</v>
       </c>
       <c r="O2" s="17">
-        <v>1054</v>
+        <v>974</v>
       </c>
       <c r="P2" s="15">
-        <v>1169</v>
+        <v>1081.5</v>
       </c>
       <c r="Q2" s="17">
-        <v>1283.5</v>
+        <v>1186</v>
       </c>
       <c r="R2" s="15">
-        <v>1402</v>
+        <v>1298</v>
       </c>
       <c r="S2" s="17">
-        <v>1516.5</v>
+        <v>1409.5</v>
       </c>
       <c r="T2" s="15">
-        <v>1628</v>
+        <v>1515.5</v>
       </c>
       <c r="U2" s="17">
-        <v>1721</v>
-      </c>
-      <c r="V2" s="15">
-        <v>1811</v>
-      </c>
-      <c r="W2" s="17">
-        <v>1897.5</v>
-      </c>
-      <c r="X2" s="15">
-        <v>1981.5</v>
-      </c>
-      <c r="Y2" s="17">
-        <v>2059</v>
-      </c>
-      <c r="Z2" s="15">
-        <v>2140.5</v>
+        <v>1602</v>
+      </c>
+      <c r="V2" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="W2" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="X2" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Y2" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Z2" s="15" t="e">
+        <v>#N/A</v>
       </c>
       <c r="AA2" s="17" t="e">
         <v>#N/A</v>
@@ -1026,58 +1026,58 @@
         <v>185</v>
       </c>
       <c r="I3" s="18">
-        <v>140</v>
+        <v>148.5</v>
       </c>
       <c r="J3" s="15">
-        <v>267</v>
+        <v>284.5</v>
       </c>
       <c r="K3" s="18">
-        <v>381</v>
+        <v>405</v>
       </c>
       <c r="L3" s="15">
-        <v>507.5</v>
+        <v>536</v>
       </c>
       <c r="M3" s="18">
-        <v>628.5</v>
+        <v>661</v>
       </c>
       <c r="N3" s="15">
-        <v>735.5</v>
+        <v>778</v>
       </c>
       <c r="O3" s="18">
-        <v>842</v>
+        <v>892</v>
       </c>
       <c r="P3" s="15">
-        <v>956</v>
+        <v>1010.5</v>
       </c>
       <c r="Q3" s="18">
-        <v>1064.5</v>
+        <v>1122.5</v>
       </c>
       <c r="R3" s="15">
-        <v>1152.5</v>
+        <v>1215</v>
       </c>
       <c r="S3" s="18">
-        <v>1231.5</v>
+        <v>1295</v>
       </c>
       <c r="T3" s="15">
-        <v>1322</v>
+        <v>1389</v>
       </c>
       <c r="U3" s="18">
-        <v>1409</v>
-      </c>
-      <c r="V3" s="15">
-        <v>1487</v>
-      </c>
-      <c r="W3" s="18">
-        <v>1560</v>
-      </c>
-      <c r="X3" s="15">
-        <v>1636</v>
-      </c>
-      <c r="Y3" s="18">
-        <v>1707</v>
-      </c>
-      <c r="Z3" s="15">
-        <v>1768.5</v>
+        <v>1480.5</v>
+      </c>
+      <c r="V3" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="W3" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="X3" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Y3" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Z3" s="15" t="e">
+        <v>#N/A</v>
       </c>
       <c r="AA3" s="18" t="e">
         <v>#N/A</v>
@@ -1115,58 +1115,58 @@
         <v>141.62227200000001</v>
       </c>
       <c r="I4" s="17">
-        <v>140</v>
+        <v>148.5</v>
       </c>
       <c r="J4" s="15">
-        <v>267</v>
+        <v>284.5</v>
       </c>
       <c r="K4" s="17">
-        <v>381</v>
+        <v>405</v>
       </c>
       <c r="L4" s="15">
-        <v>507.5</v>
+        <v>536</v>
       </c>
       <c r="M4" s="17">
-        <v>628.5</v>
+        <v>661</v>
       </c>
       <c r="N4" s="15">
-        <v>735.5</v>
+        <v>778</v>
       </c>
       <c r="O4" s="17">
-        <v>842</v>
+        <v>892</v>
       </c>
       <c r="P4" s="15">
-        <v>956</v>
+        <v>1010.5</v>
       </c>
       <c r="Q4" s="17">
-        <v>1064.5</v>
+        <v>1122.5</v>
       </c>
       <c r="R4" s="15">
-        <v>1152.5</v>
+        <v>1215</v>
       </c>
       <c r="S4" s="17">
-        <v>1231.5</v>
+        <v>1295</v>
       </c>
       <c r="T4" s="15">
-        <v>1322</v>
+        <v>1389</v>
       </c>
       <c r="U4" s="17">
-        <v>1409</v>
-      </c>
-      <c r="V4" s="15">
-        <v>1487</v>
-      </c>
-      <c r="W4" s="17">
-        <v>1560</v>
-      </c>
-      <c r="X4" s="15">
-        <v>1636</v>
-      </c>
-      <c r="Y4" s="17">
-        <v>1707</v>
-      </c>
-      <c r="Z4" s="15">
-        <v>1768.5</v>
+        <v>1480.5</v>
+      </c>
+      <c r="V4" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="W4" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="X4" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Y4" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Z4" s="15" t="e">
+        <v>#N/A</v>
       </c>
       <c r="AA4" s="17" t="e">
         <v>#N/A</v>
@@ -1204,58 +1204,58 @@
         <v>33.796224000000002</v>
       </c>
       <c r="I5" s="15">
-        <v>91.5</v>
+        <v>101</v>
       </c>
       <c r="J5" s="15">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="K5" s="15">
-        <v>280.5</v>
+        <v>307</v>
       </c>
       <c r="L5" s="15">
-        <v>366</v>
+        <v>403</v>
       </c>
       <c r="M5" s="15">
-        <v>449.5</v>
+        <v>491.5</v>
       </c>
       <c r="N5" s="15">
-        <v>536.5</v>
+        <v>586.5</v>
       </c>
       <c r="O5" s="15">
-        <v>601.5</v>
+        <v>657</v>
       </c>
       <c r="P5" s="15">
-        <v>678.5</v>
+        <v>739</v>
       </c>
       <c r="Q5" s="15">
-        <v>755.5</v>
+        <v>824.5</v>
       </c>
       <c r="R5" s="15">
-        <v>814</v>
+        <v>887.5</v>
       </c>
       <c r="S5" s="15">
-        <v>876.5</v>
+        <v>955.5</v>
       </c>
       <c r="T5" s="15">
-        <v>928.5</v>
+        <v>1009.5</v>
       </c>
       <c r="U5" s="15">
-        <v>986.5</v>
-      </c>
-      <c r="V5" s="15">
-        <v>1042</v>
-      </c>
-      <c r="W5" s="15">
-        <v>1099</v>
-      </c>
-      <c r="X5" s="15">
-        <v>1141</v>
-      </c>
-      <c r="Y5" s="15">
-        <v>1182.5</v>
-      </c>
-      <c r="Z5" s="15">
-        <v>1224.5</v>
+        <v>1071</v>
+      </c>
+      <c r="V5" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="W5" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="X5" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Y5" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Z5" s="15" t="e">
+        <v>#N/A</v>
       </c>
       <c r="AA5" s="15" t="e">
         <v>#N/A</v>
@@ -1293,58 +1293,58 @@
         <v>50</v>
       </c>
       <c r="I6" s="16">
-        <v>91.5</v>
+        <v>101</v>
       </c>
       <c r="J6" s="15">
-        <v>192</v>
+        <v>208</v>
       </c>
       <c r="K6" s="16">
-        <v>280.5</v>
+        <v>307</v>
       </c>
       <c r="L6" s="15">
-        <v>366</v>
+        <v>403</v>
       </c>
       <c r="M6" s="16">
-        <v>449.5</v>
+        <v>491.5</v>
       </c>
       <c r="N6" s="15">
-        <v>536.5</v>
+        <v>586.5</v>
       </c>
       <c r="O6" s="16">
-        <v>601.5</v>
+        <v>657</v>
       </c>
       <c r="P6" s="15">
-        <v>678.5</v>
+        <v>739</v>
       </c>
       <c r="Q6" s="16">
-        <v>755.5</v>
+        <v>824.5</v>
       </c>
       <c r="R6" s="15">
-        <v>814</v>
+        <v>887.5</v>
       </c>
       <c r="S6" s="16">
-        <v>876.5</v>
+        <v>955.5</v>
       </c>
       <c r="T6" s="15">
-        <v>928.5</v>
+        <v>1009.5</v>
       </c>
       <c r="U6" s="16">
-        <v>986.5</v>
-      </c>
-      <c r="V6" s="15">
-        <v>1042</v>
-      </c>
-      <c r="W6" s="16">
-        <v>1099</v>
-      </c>
-      <c r="X6" s="15">
-        <v>1141</v>
-      </c>
-      <c r="Y6" s="16">
-        <v>1182.5</v>
-      </c>
-      <c r="Z6" s="15">
-        <v>1224.5</v>
+        <v>1071</v>
+      </c>
+      <c r="V6" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="W6" s="16" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="X6" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Y6" s="16" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Z6" s="15" t="e">
+        <v>#N/A</v>
       </c>
       <c r="AA6" s="16" t="e">
         <v>#N/A</v>
@@ -1382,58 +1382,58 @@
         <v>0</v>
       </c>
       <c r="I7" s="18">
-        <v>437</v>
+        <v>429</v>
       </c>
       <c r="J7" s="18">
-        <v>852</v>
+        <v>836</v>
       </c>
       <c r="K7" s="18">
-        <v>1267</v>
+        <v>1243</v>
       </c>
       <c r="L7" s="18">
-        <v>1662</v>
+        <v>1629</v>
       </c>
       <c r="M7" s="18">
-        <v>2015</v>
+        <v>1976</v>
       </c>
       <c r="N7" s="18">
-        <v>2361</v>
+        <v>2313</v>
       </c>
       <c r="O7" s="18">
-        <v>2704</v>
+        <v>2653</v>
       </c>
       <c r="P7" s="18">
-        <v>3016</v>
+        <v>2961</v>
       </c>
       <c r="Q7" s="18">
-        <v>3299</v>
+        <v>3240</v>
       </c>
       <c r="R7" s="18">
-        <v>3612</v>
+        <v>3548</v>
       </c>
       <c r="S7" s="18">
-        <v>3905</v>
+        <v>3834</v>
       </c>
       <c r="T7" s="18">
-        <v>4164</v>
+        <v>4093</v>
       </c>
       <c r="U7" s="18">
-        <v>4419</v>
-      </c>
-      <c r="V7" s="18">
-        <v>4668</v>
-      </c>
-      <c r="W7" s="18">
-        <v>4898</v>
-      </c>
-      <c r="X7" s="18">
-        <v>5124</v>
-      </c>
-      <c r="Y7" s="18">
-        <v>5343</v>
-      </c>
-      <c r="Z7" s="18">
-        <v>5542</v>
+        <v>4345</v>
+      </c>
+      <c r="V7" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="W7" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="X7" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Y7" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Z7" s="18" t="e">
+        <v>#N/A</v>
       </c>
       <c r="AA7" s="18" t="e">
         <v>#N/A</v>
@@ -1466,13 +1466,13 @@
       </c>
       <c r="B10" s="31">
         <f>+I1</f>
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C10" s="22">
-        <v>8281</v>
+        <v>7595</v>
       </c>
       <c r="D10" s="25">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="H10" s="13">
         <v>40.49153908138598</v>
@@ -1484,13 +1484,13 @@
       </c>
       <c r="B11" s="31">
         <f t="shared" ref="B11:B15" si="0">+I2</f>
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="C11" s="22">
-        <v>5425.9837632000008</v>
+        <v>4976.4939839999997</v>
       </c>
       <c r="D11" s="25">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="H11" s="13">
         <v>40.30748663101604</v>
@@ -1502,7 +1502,7 @@
       </c>
       <c r="B12" s="31">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>148.5</v>
       </c>
       <c r="C12" s="22">
         <v>0</v>
@@ -1520,7 +1520,7 @@
       </c>
       <c r="B13" s="31">
         <f t="shared" si="0"/>
-        <v>140</v>
+        <v>148.5</v>
       </c>
       <c r="C13" s="22">
         <v>0</v>
@@ -1538,13 +1538,13 @@
       </c>
       <c r="B14" s="31">
         <f t="shared" si="0"/>
-        <v>91.5</v>
+        <v>101</v>
       </c>
       <c r="C14" s="22">
-        <v>10496.481944256</v>
+        <v>11586.280616064001</v>
       </c>
       <c r="D14" s="25">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="H14" s="13">
         <v>128.49516129032256</v>
@@ -1556,13 +1556,13 @@
       </c>
       <c r="B15" s="34">
         <f t="shared" si="0"/>
-        <v>91.5</v>
+        <v>101</v>
       </c>
       <c r="C15" s="26">
-        <v>9973.5</v>
+        <v>11009</v>
       </c>
       <c r="D15" s="27">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="H15" s="13">
         <v>116.02240896358543</v>
@@ -1592,75 +1592,75 @@
     <row r="3" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D3" s="13">
         <f>+a!I5*a!$D$5</f>
-        <v>0.8234999999999999</v>
+        <v>0.90899999999999992</v>
       </c>
       <c r="E3" s="13">
         <f>+a!J5*a!$D$5</f>
-        <v>1.7279999999999998</v>
+        <v>1.8719999999999999</v>
       </c>
       <c r="F3" s="13">
         <f>+a!K5*a!$D$5</f>
-        <v>2.5244999999999997</v>
+        <v>2.7629999999999999</v>
       </c>
       <c r="G3" s="13">
         <f>+a!L5*a!$D$5</f>
-        <v>3.2939999999999996</v>
+        <v>3.6269999999999998</v>
       </c>
       <c r="H3" s="13">
         <f>+a!M5*a!$D$5</f>
-        <v>4.0454999999999997</v>
+        <v>4.4234999999999998</v>
       </c>
       <c r="I3" s="13">
         <f>+a!N5*a!$D$5</f>
-        <v>4.8285</v>
+        <v>5.2784999999999993</v>
       </c>
       <c r="J3" s="13">
         <f>+a!O5*a!$D$5</f>
-        <v>5.4135</v>
+        <v>5.9129999999999994</v>
       </c>
       <c r="K3" s="13">
         <f>+a!P5*a!$D$5</f>
-        <v>6.1064999999999996</v>
+        <v>6.6509999999999998</v>
       </c>
       <c r="L3" s="13">
         <f>+a!Q5*a!$D$5</f>
-        <v>6.7994999999999992</v>
+        <v>7.4204999999999997</v>
       </c>
       <c r="M3" s="13">
         <f>+a!R5*a!$D$5</f>
-        <v>7.3259999999999996</v>
+        <v>7.9874999999999998</v>
       </c>
       <c r="N3" s="13">
         <f>+a!S5*a!$D$5</f>
-        <v>7.8884999999999996</v>
+        <v>8.599499999999999</v>
       </c>
       <c r="O3" s="13">
         <f>+a!T5*a!$D$5</f>
-        <v>8.3564999999999987</v>
+        <v>9.0854999999999997</v>
       </c>
       <c r="P3" s="13">
         <f>+a!U5*a!$D$5</f>
-        <v>8.8784999999999989</v>
-      </c>
-      <c r="Q3" s="13">
+        <v>9.6389999999999993</v>
+      </c>
+      <c r="Q3" s="13" t="e">
         <f>+a!V5*a!$D$5</f>
-        <v>9.3780000000000001</v>
-      </c>
-      <c r="R3" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="R3" s="13" t="e">
         <f>+a!W5*a!$D$5</f>
-        <v>9.891</v>
-      </c>
-      <c r="S3" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="S3" s="13" t="e">
         <f>+a!X5*a!$D$5</f>
-        <v>10.268999999999998</v>
-      </c>
-      <c r="T3" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="T3" s="13" t="e">
         <f>+a!Y5*a!$D$5</f>
-        <v>10.6425</v>
-      </c>
-      <c r="U3" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="U3" s="13" t="e">
         <f>+a!Z5*a!$D$5</f>
-        <v>11.020499999999998</v>
+        <v>#N/A</v>
       </c>
       <c r="V3" s="13" t="e">
         <f>+a!AA5*a!$D$5</f>
@@ -1678,75 +1678,75 @@
     <row r="4" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D4" s="13">
         <f>+a!I6*a!$D$6</f>
-        <v>11.529</v>
+        <v>12.726000000000001</v>
       </c>
       <c r="E4" s="13">
         <f>+a!J6*a!$D$6</f>
-        <v>24.192</v>
+        <v>26.207999999999998</v>
       </c>
       <c r="F4" s="13">
         <f>+a!K6*a!$D$6</f>
-        <v>35.343000000000004</v>
+        <v>38.682000000000002</v>
       </c>
       <c r="G4" s="13">
         <f>+a!L6*a!$D$6</f>
-        <v>46.116</v>
+        <v>50.777999999999999</v>
       </c>
       <c r="H4" s="13">
         <f>+a!M6*a!$D$6</f>
-        <v>56.637</v>
+        <v>61.929000000000002</v>
       </c>
       <c r="I4" s="13">
         <f>+a!N6*a!$D$6</f>
-        <v>67.599000000000004</v>
+        <v>73.899000000000001</v>
       </c>
       <c r="J4" s="13">
         <f>+a!O6*a!$D$6</f>
-        <v>75.789000000000001</v>
+        <v>82.781999999999996</v>
       </c>
       <c r="K4" s="13">
         <f>+a!P6*a!$D$6</f>
-        <v>85.491</v>
+        <v>93.114000000000004</v>
       </c>
       <c r="L4" s="13">
         <f>+a!Q6*a!$D$6</f>
-        <v>95.192999999999998</v>
+        <v>103.887</v>
       </c>
       <c r="M4" s="13">
         <f>+a!R6*a!$D$6</f>
-        <v>102.56400000000001</v>
+        <v>111.825</v>
       </c>
       <c r="N4" s="13">
         <f>+a!S6*a!$D$6</f>
-        <v>110.43900000000001</v>
+        <v>120.393</v>
       </c>
       <c r="O4" s="13">
         <f>+a!T6*a!$D$6</f>
-        <v>116.991</v>
+        <v>127.197</v>
       </c>
       <c r="P4" s="13">
         <f>+a!U6*a!$D$6</f>
-        <v>124.29900000000001</v>
-      </c>
-      <c r="Q4" s="13">
+        <v>134.946</v>
+      </c>
+      <c r="Q4" s="13" t="e">
         <f>+a!V6*a!$D$6</f>
-        <v>131.292</v>
-      </c>
-      <c r="R4" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="R4" s="13" t="e">
         <f>+a!W6*a!$D$6</f>
-        <v>138.47399999999999</v>
-      </c>
-      <c r="S4" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="S4" s="13" t="e">
         <f>+a!X6*a!$D$6</f>
-        <v>143.76599999999999</v>
-      </c>
-      <c r="T4" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="T4" s="13" t="e">
         <f>+a!Y6*a!$D$6</f>
-        <v>148.995</v>
-      </c>
-      <c r="U4" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="U4" s="13" t="e">
         <f>+a!Z6*a!$D$6</f>
-        <v>154.28700000000001</v>
+        <v>#N/A</v>
       </c>
       <c r="V4" s="13" t="e">
         <f>+a!AA6*a!$D$6</f>
@@ -1764,75 +1764,75 @@
     <row r="5" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D5" s="13">
         <f>+a!I1*a!$D$1</f>
-        <v>5.577</v>
+        <v>5.1150000000000002</v>
       </c>
       <c r="E5" s="13">
         <f>+a!J1*a!$D$1</f>
-        <v>10.8735</v>
+        <v>10.032</v>
       </c>
       <c r="F5" s="13">
         <f>+a!K1*a!$D$1</f>
-        <v>16.2195</v>
+        <v>14.949</v>
       </c>
       <c r="G5" s="13">
         <f>+a!L1*a!$D$1</f>
-        <v>20.823</v>
+        <v>19.206</v>
       </c>
       <c r="H5" s="13">
         <f>+a!M1*a!$D$1</f>
-        <v>25.624500000000001</v>
+        <v>23.8095</v>
       </c>
       <c r="I5" s="13">
         <f>+a!N1*a!$D$1</f>
-        <v>30.162000000000003</v>
+        <v>27.901500000000002</v>
       </c>
       <c r="J5" s="13">
         <f>+a!O1*a!$D$1</f>
-        <v>34.782000000000004</v>
+        <v>32.142000000000003</v>
       </c>
       <c r="K5" s="13">
         <f>+a!P1*a!$D$1</f>
-        <v>38.577000000000005</v>
+        <v>35.689500000000002</v>
       </c>
       <c r="L5" s="13">
         <f>+a!Q1*a!$D$1</f>
-        <v>42.355499999999999</v>
+        <v>39.138000000000005</v>
       </c>
       <c r="M5" s="13">
         <f>+a!R1*a!$D$1</f>
-        <v>46.266000000000005</v>
+        <v>42.834000000000003</v>
       </c>
       <c r="N5" s="13">
         <f>+a!S1*a!$D$1</f>
-        <v>50.044499999999999</v>
+        <v>46.513500000000001</v>
       </c>
       <c r="O5" s="13">
         <f>+a!T1*a!$D$1</f>
-        <v>53.724000000000004</v>
+        <v>50.011500000000005</v>
       </c>
       <c r="P5" s="13">
         <f>+a!U1*a!$D$1</f>
-        <v>56.792999999999999</v>
-      </c>
-      <c r="Q5" s="13">
+        <v>52.866</v>
+      </c>
+      <c r="Q5" s="13" t="e">
         <f>+a!V1*a!$D$1</f>
-        <v>59.763000000000005</v>
-      </c>
-      <c r="R5" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="R5" s="13" t="e">
         <f>+a!W1*a!$D$1</f>
-        <v>62.6175</v>
-      </c>
-      <c r="S5" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="S5" s="13" t="e">
         <f>+a!X1*a!$D$1</f>
-        <v>65.389499999999998</v>
-      </c>
-      <c r="T5" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="T5" s="13" t="e">
         <f>+a!Y1*a!$D$1</f>
-        <v>67.947000000000003</v>
-      </c>
-      <c r="U5" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="U5" s="13" t="e">
         <f>+a!Z1*a!$D$1</f>
-        <v>70.636499999999998</v>
+        <v>#N/A</v>
       </c>
       <c r="V5" s="13" t="e">
         <f>+a!AA1*a!$D$1</f>
@@ -1850,75 +1850,75 @@
     <row r="6" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D6" s="13">
         <f>+a!I2*a!$D$2</f>
-        <v>17.576000000000001</v>
+        <v>16.12</v>
       </c>
       <c r="E6" s="13">
         <f>+a!J2*a!$D$2</f>
-        <v>34.268000000000001</v>
+        <v>31.616</v>
       </c>
       <c r="F6" s="13">
         <f>+a!K2*a!$D$2</f>
-        <v>51.116</v>
+        <v>47.111999999999995</v>
       </c>
       <c r="G6" s="13">
         <f>+a!L2*a!$D$2</f>
-        <v>65.623999999999995</v>
+        <v>60.527999999999999</v>
       </c>
       <c r="H6" s="13">
         <f>+a!M2*a!$D$2</f>
-        <v>80.756</v>
+        <v>75.036000000000001</v>
       </c>
       <c r="I6" s="13">
         <f>+a!N2*a!$D$2</f>
-        <v>95.055999999999997</v>
+        <v>87.932000000000002</v>
       </c>
       <c r="J6" s="13">
         <f>+a!O2*a!$D$2</f>
-        <v>109.616</v>
+        <v>101.29599999999999</v>
       </c>
       <c r="K6" s="13">
         <f>+a!P2*a!$D$2</f>
-        <v>121.57599999999999</v>
+        <v>112.476</v>
       </c>
       <c r="L6" s="13">
         <f>+a!Q2*a!$D$2</f>
-        <v>133.48399999999998</v>
+        <v>123.34399999999999</v>
       </c>
       <c r="M6" s="13">
         <f>+a!R2*a!$D$2</f>
-        <v>145.80799999999999</v>
+        <v>134.99199999999999</v>
       </c>
       <c r="N6" s="13">
         <f>+a!S2*a!$D$2</f>
-        <v>157.71599999999998</v>
+        <v>146.58799999999999</v>
       </c>
       <c r="O6" s="13">
         <f>+a!T2*a!$D$2</f>
-        <v>169.31199999999998</v>
+        <v>157.61199999999999</v>
       </c>
       <c r="P6" s="13">
         <f>+a!U2*a!$D$2</f>
-        <v>178.98399999999998</v>
-      </c>
-      <c r="Q6" s="13">
+        <v>166.608</v>
+      </c>
+      <c r="Q6" s="13" t="e">
         <f>+a!V2*a!$D$2</f>
-        <v>188.34399999999999</v>
-      </c>
-      <c r="R6" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="R6" s="13" t="e">
         <f>+a!W2*a!$D$2</f>
-        <v>197.34</v>
-      </c>
-      <c r="S6" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="S6" s="13" t="e">
         <f>+a!X2*a!$D$2</f>
-        <v>206.07599999999999</v>
-      </c>
-      <c r="T6" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="T6" s="13" t="e">
         <f>+a!Y2*a!$D$2</f>
-        <v>214.136</v>
-      </c>
-      <c r="U6" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="U6" s="13" t="e">
         <f>+a!Z2*a!$D$2</f>
-        <v>222.61199999999999</v>
+        <v>#N/A</v>
       </c>
       <c r="V6" s="13" t="e">
         <f>+a!AA2*a!$D$2</f>
@@ -1936,75 +1936,75 @@
     <row r="7" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D7" s="13">
         <f>+a!I3*a!$D$3</f>
-        <v>39.200000000000003</v>
+        <v>41.580000000000005</v>
       </c>
       <c r="E7" s="13">
         <f>+a!J3*a!$D$3</f>
-        <v>74.760000000000005</v>
+        <v>79.660000000000011</v>
       </c>
       <c r="F7" s="13">
         <f>+a!K3*a!$D$3</f>
-        <v>106.68</v>
+        <v>113.4</v>
       </c>
       <c r="G7" s="13">
         <f>+a!L3*a!$D$3</f>
-        <v>142.10000000000002</v>
+        <v>150.08000000000001</v>
       </c>
       <c r="H7" s="13">
         <f>+a!M3*a!$D$3</f>
-        <v>175.98000000000002</v>
+        <v>185.08</v>
       </c>
       <c r="I7" s="13">
         <f>+a!N3*a!$D$3</f>
-        <v>205.94000000000003</v>
+        <v>217.84000000000003</v>
       </c>
       <c r="J7" s="13">
         <f>+a!O3*a!$D$3</f>
-        <v>235.76000000000002</v>
+        <v>249.76000000000002</v>
       </c>
       <c r="K7" s="13">
         <f>+a!P3*a!$D$3</f>
-        <v>267.68</v>
+        <v>282.94000000000005</v>
       </c>
       <c r="L7" s="13">
         <f>+a!Q3*a!$D$3</f>
-        <v>298.06</v>
+        <v>314.3</v>
       </c>
       <c r="M7" s="13">
         <f>+a!R3*a!$D$3</f>
-        <v>322.70000000000005</v>
+        <v>340.20000000000005</v>
       </c>
       <c r="N7" s="13">
         <f>+a!S3*a!$D$3</f>
-        <v>344.82000000000005</v>
+        <v>362.6</v>
       </c>
       <c r="O7" s="13">
         <f>+a!T3*a!$D$3</f>
-        <v>370.16</v>
+        <v>388.92</v>
       </c>
       <c r="P7" s="13">
         <f>+a!U3*a!$D$3</f>
-        <v>394.52000000000004</v>
-      </c>
-      <c r="Q7" s="13">
+        <v>414.54</v>
+      </c>
+      <c r="Q7" s="13" t="e">
         <f>+a!V3*a!$D$3</f>
-        <v>416.36</v>
-      </c>
-      <c r="R7" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="R7" s="13" t="e">
         <f>+a!W3*a!$D$3</f>
-        <v>436.80000000000007</v>
-      </c>
-      <c r="S7" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="S7" s="13" t="e">
         <f>+a!X3*a!$D$3</f>
-        <v>458.08000000000004</v>
-      </c>
-      <c r="T7" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="T7" s="13" t="e">
         <f>+a!Y3*a!$D$3</f>
-        <v>477.96000000000004</v>
-      </c>
-      <c r="U7" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="U7" s="13" t="e">
         <f>+a!Z3*a!$D$3</f>
-        <v>495.18000000000006</v>
+        <v>#N/A</v>
       </c>
       <c r="V7" s="13" t="e">
         <f>+a!AA3*a!$D$3</f>
@@ -2022,75 +2022,75 @@
     <row r="8" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D8" s="13">
         <f>+a!I4*a!$D$4</f>
-        <v>29.259999999999998</v>
+        <v>31.0365</v>
       </c>
       <c r="E8" s="13">
         <f>+a!J4*a!$D$4</f>
-        <v>55.802999999999997</v>
+        <v>59.460499999999996</v>
       </c>
       <c r="F8" s="13">
         <f>+a!K4*a!$D$4</f>
-        <v>79.628999999999991</v>
+        <v>84.644999999999996</v>
       </c>
       <c r="G8" s="13">
         <f>+a!L4*a!$D$4</f>
-        <v>106.0675</v>
+        <v>112.024</v>
       </c>
       <c r="H8" s="13">
         <f>+a!M4*a!$D$4</f>
-        <v>131.35649999999998</v>
+        <v>138.149</v>
       </c>
       <c r="I8" s="13">
         <f>+a!N4*a!$D$4</f>
-        <v>153.71949999999998</v>
+        <v>162.602</v>
       </c>
       <c r="J8" s="13">
         <f>+a!O4*a!$D$4</f>
-        <v>175.97799999999998</v>
+        <v>186.428</v>
       </c>
       <c r="K8" s="13">
         <f>+a!P4*a!$D$4</f>
-        <v>199.804</v>
+        <v>211.19450000000001</v>
       </c>
       <c r="L8" s="13">
         <f>+a!Q4*a!$D$4</f>
-        <v>222.48049999999998</v>
+        <v>234.60249999999999</v>
       </c>
       <c r="M8" s="13">
         <f>+a!R4*a!$D$4</f>
-        <v>240.8725</v>
+        <v>253.935</v>
       </c>
       <c r="N8" s="13">
         <f>+a!S4*a!$D$4</f>
-        <v>257.38349999999997</v>
+        <v>270.65499999999997</v>
       </c>
       <c r="O8" s="13">
         <f>+a!T4*a!$D$4</f>
-        <v>276.298</v>
+        <v>290.30099999999999</v>
       </c>
       <c r="P8" s="13">
         <f>+a!U4*a!$D$4</f>
-        <v>294.48099999999999</v>
-      </c>
-      <c r="Q8" s="13">
+        <v>309.42449999999997</v>
+      </c>
+      <c r="Q8" s="13" t="e">
         <f>+a!V4*a!$D$4</f>
-        <v>310.78300000000002</v>
-      </c>
-      <c r="R8" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="R8" s="13" t="e">
         <f>+a!W4*a!$D$4</f>
-        <v>326.03999999999996</v>
-      </c>
-      <c r="S8" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="S8" s="13" t="e">
         <f>+a!X4*a!$D$4</f>
-        <v>341.92399999999998</v>
-      </c>
-      <c r="T8" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="T8" s="13" t="e">
         <f>+a!Y4*a!$D$4</f>
-        <v>356.76299999999998</v>
-      </c>
-      <c r="U8" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="U8" s="13" t="e">
         <f>+a!Z4*a!$D$4</f>
-        <v>369.61649999999997</v>
+        <v>#N/A</v>
       </c>
       <c r="V8" s="13" t="e">
         <f>+a!AA4*a!$D$4</f>
@@ -2108,75 +2108,75 @@
     <row r="9" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D9" s="13">
         <f>+a!I7*a!$D$5</f>
-        <v>3.9329999999999998</v>
+        <v>3.8609999999999998</v>
       </c>
       <c r="E9" s="13">
         <f>+a!J7*a!$D$5</f>
-        <v>7.6679999999999993</v>
+        <v>7.5239999999999991</v>
       </c>
       <c r="F9" s="13">
         <f>+a!K7*a!$D$5</f>
-        <v>11.402999999999999</v>
+        <v>11.186999999999999</v>
       </c>
       <c r="G9" s="13">
         <f>+a!L7*a!$D$5</f>
-        <v>14.957999999999998</v>
+        <v>14.661</v>
       </c>
       <c r="H9" s="13">
         <f>+a!M7*a!$D$5</f>
-        <v>18.134999999999998</v>
+        <v>17.783999999999999</v>
       </c>
       <c r="I9" s="13">
         <f>+a!N7*a!$D$5</f>
-        <v>21.248999999999999</v>
+        <v>20.817</v>
       </c>
       <c r="J9" s="13">
         <f>+a!O7*a!$D$5</f>
-        <v>24.335999999999999</v>
+        <v>23.876999999999999</v>
       </c>
       <c r="K9" s="13">
         <f>+a!P7*a!$D$5</f>
-        <v>27.143999999999998</v>
+        <v>26.648999999999997</v>
       </c>
       <c r="L9" s="13">
         <f>+a!Q7*a!$D$5</f>
-        <v>29.690999999999999</v>
+        <v>29.159999999999997</v>
       </c>
       <c r="M9" s="13">
         <f>+a!R7*a!$D$5</f>
-        <v>32.507999999999996</v>
+        <v>31.931999999999999</v>
       </c>
       <c r="N9" s="13">
         <f>+a!S7*a!$D$5</f>
-        <v>35.144999999999996</v>
+        <v>34.506</v>
       </c>
       <c r="O9" s="13">
         <f>+a!T7*a!$D$5</f>
-        <v>37.475999999999999</v>
+        <v>36.836999999999996</v>
       </c>
       <c r="P9" s="13">
         <f>+a!U7*a!$D$5</f>
-        <v>39.770999999999994</v>
-      </c>
-      <c r="Q9" s="13">
+        <v>39.104999999999997</v>
+      </c>
+      <c r="Q9" s="13" t="e">
         <f>+a!V7*a!$D$5</f>
-        <v>42.011999999999993</v>
-      </c>
-      <c r="R9" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="R9" s="13" t="e">
         <f>+a!W7*a!$D$5</f>
-        <v>44.081999999999994</v>
-      </c>
-      <c r="S9" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="S9" s="13" t="e">
         <f>+a!X7*a!$D$5</f>
-        <v>46.116</v>
-      </c>
-      <c r="T9" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="T9" s="13" t="e">
         <f>+a!Y7*a!$D$5</f>
-        <v>48.086999999999996</v>
-      </c>
-      <c r="U9" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="U9" s="13" t="e">
         <f>+a!Z7*a!$D$5</f>
-        <v>49.877999999999993</v>
+        <v>#N/A</v>
       </c>
       <c r="V9" s="13" t="e">
         <f>+a!AA7*a!$D$5</f>
@@ -2194,49 +2194,49 @@
     <row r="10" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D10">
         <f>SUM(D3:D8)</f>
-        <v>103.96549999999999</v>
+        <v>107.48650000000002</v>
       </c>
       <c r="E10" s="13">
         <f t="shared" ref="E10:M10" si="1">SUM(E3:E8)</f>
-        <v>201.62450000000001</v>
+        <v>208.8485</v>
       </c>
       <c r="F10" s="13">
         <f t="shared" si="1"/>
-        <v>291.512</v>
+        <v>301.55099999999999</v>
       </c>
       <c r="G10" s="13">
         <f t="shared" si="1"/>
-        <v>384.02449999999999</v>
+        <v>396.24300000000005</v>
       </c>
       <c r="H10" s="13">
         <f t="shared" si="1"/>
-        <v>474.39949999999999</v>
+        <v>488.42700000000002</v>
       </c>
       <c r="I10" s="13">
         <f t="shared" si="1"/>
-        <v>557.30500000000006</v>
+        <v>575.45299999999997</v>
       </c>
       <c r="J10" s="13">
         <f t="shared" si="1"/>
-        <v>637.33849999999995</v>
+        <v>658.32100000000003</v>
       </c>
       <c r="K10" s="13">
         <f t="shared" si="1"/>
-        <v>719.23449999999991</v>
+        <v>742.06500000000005</v>
       </c>
       <c r="L10" s="13">
         <f t="shared" si="1"/>
-        <v>798.37250000000006</v>
+        <v>822.69200000000001</v>
       </c>
       <c r="M10" s="13">
         <f t="shared" si="1"/>
-        <v>865.53649999999993</v>
+        <v>891.77350000000001</v>
       </c>
     </row>
     <row r="14" spans="4:24" x14ac:dyDescent="0.25">
       <c r="E14" s="13">
         <f>+a!G5*a!E5*a!I5</f>
-        <v>10496481.944256</v>
+        <v>11586280.616064001</v>
       </c>
       <c r="G14" s="13">
         <f>+(a!G5+a!H5)*a!$E$7</f>
@@ -2244,13 +2244,13 @@
       </c>
       <c r="H14">
         <f>+E14/G14</f>
-        <v>88.400806451612894</v>
+        <v>97.579032258064515</v>
       </c>
     </row>
     <row r="15" spans="4:24" x14ac:dyDescent="0.25">
       <c r="E15" s="13">
         <f>+a!G6*a!E6*a!I6</f>
-        <v>9973500</v>
+        <v>11009000</v>
       </c>
       <c r="G15" s="13">
         <f>+(a!G6+a!H6)*a!$E$7</f>
@@ -2258,13 +2258,13 @@
       </c>
       <c r="H15" s="13">
         <f t="shared" ref="H15:H19" si="2">+E15/G15</f>
-        <v>79.819927971188477</v>
+        <v>88.107242897158869</v>
       </c>
     </row>
     <row r="16" spans="4:24" x14ac:dyDescent="0.25">
       <c r="E16" s="13">
         <f>+a!G1*a!E1*a!I1</f>
-        <v>8281000</v>
+        <v>7595000</v>
       </c>
       <c r="G16" s="13">
         <f>+(a!G1+a!H1)*a!$E$7</f>
@@ -2272,13 +2272,13 @@
       </c>
       <c r="H16" s="13">
         <f t="shared" si="2"/>
-        <v>68.09024979854955</v>
+        <v>62.449637389202259</v>
       </c>
     </row>
     <row r="17" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E17" s="13">
         <f>+a!G2*a!E2*a!I2</f>
-        <v>5425983.7631999999</v>
+        <v>4976493.9840000002</v>
       </c>
       <c r="G17" s="13">
         <f>+(a!G2+a!H2)*a!$E$7</f>
@@ -2286,7 +2286,7 @@
       </c>
       <c r="H17" s="13">
         <f t="shared" si="2"/>
-        <v>67.780748663101591</v>
+        <v>62.16577540106951</v>
       </c>
     </row>
     <row r="18" spans="5:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Se coloc[o un mensaje de advertencia para certificar que la suma de las cantidades sea igual a la variable cantidad vehiculo.
</commit_message>
<xml_diff>
--- a/evsim/Impac.Amb..xlsx
+++ b/evsim/Impac.Amb..xlsx
@@ -848,43 +848,43 @@
         <v>22</v>
       </c>
       <c r="I1" s="15">
-        <v>155</v>
+        <v>134.5</v>
       </c>
       <c r="J1" s="15">
-        <v>304</v>
+        <v>266.5</v>
       </c>
       <c r="K1" s="15">
-        <v>453</v>
+        <v>393</v>
       </c>
       <c r="L1" s="15">
-        <v>582</v>
+        <v>507.5</v>
       </c>
       <c r="M1" s="15">
-        <v>721.5</v>
+        <v>626</v>
       </c>
       <c r="N1" s="15">
-        <v>845.5</v>
+        <v>745</v>
       </c>
       <c r="O1" s="15">
-        <v>974</v>
+        <v>855.5</v>
       </c>
       <c r="P1" s="15">
-        <v>1081.5</v>
+        <v>954</v>
       </c>
       <c r="Q1" s="15">
-        <v>1186</v>
+        <v>1042.5</v>
       </c>
       <c r="R1" s="15">
-        <v>1298</v>
-      </c>
-      <c r="S1" s="15">
-        <v>1409.5</v>
-      </c>
-      <c r="T1" s="15">
-        <v>1515.5</v>
-      </c>
-      <c r="U1" s="15">
-        <v>1602</v>
+        <v>1141.5</v>
+      </c>
+      <c r="S1" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T1" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U1" s="15" t="e">
+        <v>#N/A</v>
       </c>
       <c r="V1" s="15" t="e">
         <v>#N/A</v>
@@ -937,43 +937,43 @@
         <v>61.155072000000004</v>
       </c>
       <c r="I2" s="17">
-        <v>155</v>
+        <v>134.5</v>
       </c>
       <c r="J2" s="15">
-        <v>304</v>
+        <v>266.5</v>
       </c>
       <c r="K2" s="17">
-        <v>453</v>
+        <v>393</v>
       </c>
       <c r="L2" s="15">
-        <v>582</v>
+        <v>507.5</v>
       </c>
       <c r="M2" s="17">
-        <v>721.5</v>
+        <v>626</v>
       </c>
       <c r="N2" s="15">
-        <v>845.5</v>
+        <v>745</v>
       </c>
       <c r="O2" s="17">
-        <v>974</v>
+        <v>855.5</v>
       </c>
       <c r="P2" s="15">
-        <v>1081.5</v>
+        <v>954</v>
       </c>
       <c r="Q2" s="17">
-        <v>1186</v>
+        <v>1042.5</v>
       </c>
       <c r="R2" s="15">
-        <v>1298</v>
-      </c>
-      <c r="S2" s="17">
-        <v>1409.5</v>
-      </c>
-      <c r="T2" s="15">
-        <v>1515.5</v>
-      </c>
-      <c r="U2" s="17">
-        <v>1602</v>
+        <v>1141.5</v>
+      </c>
+      <c r="S2" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T2" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U2" s="17" t="e">
+        <v>#N/A</v>
       </c>
       <c r="V2" s="15" t="e">
         <v>#N/A</v>
@@ -1026,43 +1026,43 @@
         <v>185</v>
       </c>
       <c r="I3" s="18">
-        <v>148.5</v>
+        <v>131.5</v>
       </c>
       <c r="J3" s="15">
-        <v>284.5</v>
+        <v>248.5</v>
       </c>
       <c r="K3" s="18">
-        <v>405</v>
+        <v>352.5</v>
       </c>
       <c r="L3" s="15">
-        <v>536</v>
+        <v>468</v>
       </c>
       <c r="M3" s="18">
-        <v>661</v>
+        <v>581.5</v>
       </c>
       <c r="N3" s="15">
-        <v>778</v>
+        <v>682</v>
       </c>
       <c r="O3" s="18">
-        <v>892</v>
+        <v>778.5</v>
       </c>
       <c r="P3" s="15">
-        <v>1010.5</v>
+        <v>884</v>
       </c>
       <c r="Q3" s="18">
-        <v>1122.5</v>
+        <v>983.5</v>
       </c>
       <c r="R3" s="15">
-        <v>1215</v>
-      </c>
-      <c r="S3" s="18">
-        <v>1295</v>
-      </c>
-      <c r="T3" s="15">
-        <v>1389</v>
-      </c>
-      <c r="U3" s="18">
-        <v>1480.5</v>
+        <v>1063.5</v>
+      </c>
+      <c r="S3" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T3" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U3" s="18" t="e">
+        <v>#N/A</v>
       </c>
       <c r="V3" s="15" t="e">
         <v>#N/A</v>
@@ -1115,43 +1115,43 @@
         <v>141.62227200000001</v>
       </c>
       <c r="I4" s="17">
-        <v>148.5</v>
+        <v>131.5</v>
       </c>
       <c r="J4" s="15">
-        <v>284.5</v>
+        <v>248.5</v>
       </c>
       <c r="K4" s="17">
-        <v>405</v>
+        <v>352.5</v>
       </c>
       <c r="L4" s="15">
-        <v>536</v>
+        <v>468</v>
       </c>
       <c r="M4" s="17">
-        <v>661</v>
+        <v>581.5</v>
       </c>
       <c r="N4" s="15">
-        <v>778</v>
+        <v>682</v>
       </c>
       <c r="O4" s="17">
-        <v>892</v>
+        <v>778.5</v>
       </c>
       <c r="P4" s="15">
-        <v>1010.5</v>
+        <v>884</v>
       </c>
       <c r="Q4" s="17">
-        <v>1122.5</v>
+        <v>983.5</v>
       </c>
       <c r="R4" s="15">
-        <v>1215</v>
-      </c>
-      <c r="S4" s="17">
-        <v>1295</v>
-      </c>
-      <c r="T4" s="15">
-        <v>1389</v>
-      </c>
-      <c r="U4" s="17">
-        <v>1480.5</v>
+        <v>1063.5</v>
+      </c>
+      <c r="S4" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T4" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U4" s="17" t="e">
+        <v>#N/A</v>
       </c>
       <c r="V4" s="15" t="e">
         <v>#N/A</v>
@@ -1204,43 +1204,43 @@
         <v>33.796224000000002</v>
       </c>
       <c r="I5" s="15">
-        <v>101</v>
+        <v>101.5</v>
       </c>
       <c r="J5" s="15">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="K5" s="15">
-        <v>307</v>
+        <v>317.5</v>
       </c>
       <c r="L5" s="15">
-        <v>403</v>
+        <v>405.5</v>
       </c>
       <c r="M5" s="15">
-        <v>491.5</v>
+        <v>494.5</v>
       </c>
       <c r="N5" s="15">
-        <v>586.5</v>
+        <v>575</v>
       </c>
       <c r="O5" s="15">
-        <v>657</v>
+        <v>657.5</v>
       </c>
       <c r="P5" s="15">
-        <v>739</v>
+        <v>729.5</v>
       </c>
       <c r="Q5" s="15">
-        <v>824.5</v>
+        <v>814</v>
       </c>
       <c r="R5" s="15">
-        <v>887.5</v>
-      </c>
-      <c r="S5" s="15">
-        <v>955.5</v>
-      </c>
-      <c r="T5" s="15">
-        <v>1009.5</v>
-      </c>
-      <c r="U5" s="15">
-        <v>1071</v>
+        <v>878</v>
+      </c>
+      <c r="S5" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T5" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U5" s="15" t="e">
+        <v>#N/A</v>
       </c>
       <c r="V5" s="15" t="e">
         <v>#N/A</v>
@@ -1293,43 +1293,43 @@
         <v>50</v>
       </c>
       <c r="I6" s="16">
-        <v>101</v>
+        <v>101.5</v>
       </c>
       <c r="J6" s="15">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="K6" s="16">
-        <v>307</v>
+        <v>317.5</v>
       </c>
       <c r="L6" s="15">
-        <v>403</v>
+        <v>405.5</v>
       </c>
       <c r="M6" s="16">
-        <v>491.5</v>
+        <v>494.5</v>
       </c>
       <c r="N6" s="15">
-        <v>586.5</v>
+        <v>575</v>
       </c>
       <c r="O6" s="16">
-        <v>657</v>
+        <v>657.5</v>
       </c>
       <c r="P6" s="15">
-        <v>739</v>
+        <v>729.5</v>
       </c>
       <c r="Q6" s="16">
-        <v>824.5</v>
+        <v>814</v>
       </c>
       <c r="R6" s="15">
-        <v>887.5</v>
-      </c>
-      <c r="S6" s="16">
-        <v>955.5</v>
-      </c>
-      <c r="T6" s="15">
-        <v>1009.5</v>
-      </c>
-      <c r="U6" s="16">
-        <v>1071</v>
+        <v>878</v>
+      </c>
+      <c r="S6" s="16" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T6" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U6" s="16" t="e">
+        <v>#N/A</v>
       </c>
       <c r="V6" s="15" t="e">
         <v>#N/A</v>
@@ -1382,43 +1382,43 @@
         <v>0</v>
       </c>
       <c r="I7" s="18">
-        <v>429</v>
+        <v>503</v>
       </c>
       <c r="J7" s="18">
-        <v>836</v>
+        <v>975</v>
       </c>
       <c r="K7" s="18">
-        <v>1243</v>
+        <v>1447</v>
       </c>
       <c r="L7" s="18">
-        <v>1629</v>
+        <v>1909</v>
       </c>
       <c r="M7" s="18">
-        <v>1976</v>
+        <v>2320</v>
       </c>
       <c r="N7" s="18">
-        <v>2313</v>
+        <v>2729</v>
       </c>
       <c r="O7" s="18">
-        <v>2653</v>
+        <v>3116</v>
       </c>
       <c r="P7" s="18">
-        <v>2961</v>
+        <v>3488</v>
       </c>
       <c r="Q7" s="18">
-        <v>3240</v>
+        <v>3826</v>
       </c>
       <c r="R7" s="18">
-        <v>3548</v>
-      </c>
-      <c r="S7" s="18">
-        <v>3834</v>
-      </c>
-      <c r="T7" s="18">
-        <v>4093</v>
-      </c>
-      <c r="U7" s="18">
-        <v>4345</v>
+        <v>4183</v>
+      </c>
+      <c r="S7" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="T7" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="U7" s="18" t="e">
+        <v>#N/A</v>
       </c>
       <c r="V7" s="18" t="e">
         <v>#N/A</v>
@@ -1466,13 +1466,13 @@
       </c>
       <c r="B10" s="31">
         <f>+I1</f>
-        <v>155</v>
+        <v>134.5</v>
       </c>
       <c r="C10" s="22">
-        <v>7595</v>
+        <v>6590.5</v>
       </c>
       <c r="D10" s="25">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="H10" s="13">
         <v>40.49153908138598</v>
@@ -1484,13 +1484,13 @@
       </c>
       <c r="B11" s="31">
         <f t="shared" ref="B11:B15" si="0">+I2</f>
-        <v>155</v>
+        <v>134.5</v>
       </c>
       <c r="C11" s="22">
-        <v>4976.4939839999997</v>
+        <v>4318.3125216000008</v>
       </c>
       <c r="D11" s="25">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="H11" s="13">
         <v>40.30748663101604</v>
@@ -1502,7 +1502,7 @@
       </c>
       <c r="B12" s="31">
         <f t="shared" si="0"/>
-        <v>148.5</v>
+        <v>131.5</v>
       </c>
       <c r="C12" s="22">
         <v>0</v>
@@ -1520,7 +1520,7 @@
       </c>
       <c r="B13" s="31">
         <f t="shared" si="0"/>
-        <v>148.5</v>
+        <v>131.5</v>
       </c>
       <c r="C13" s="22">
         <v>0</v>
@@ -1538,13 +1538,13 @@
       </c>
       <c r="B14" s="31">
         <f t="shared" si="0"/>
-        <v>101</v>
+        <v>101.5</v>
       </c>
       <c r="C14" s="22">
-        <v>11586.280616064001</v>
+        <v>11643.638440896</v>
       </c>
       <c r="D14" s="25">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H14" s="13">
         <v>128.49516129032256</v>
@@ -1556,10 +1556,10 @@
       </c>
       <c r="B15" s="34">
         <f t="shared" si="0"/>
-        <v>101</v>
+        <v>101.5</v>
       </c>
       <c r="C15" s="26">
-        <v>11009</v>
+        <v>11063.5</v>
       </c>
       <c r="D15" s="27">
         <v>88</v>
@@ -1592,55 +1592,55 @@
     <row r="3" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D3" s="13">
         <f>+a!I5*a!$D$5</f>
-        <v>0.90899999999999992</v>
+        <v>0.91349999999999998</v>
       </c>
       <c r="E3" s="13">
         <f>+a!J5*a!$D$5</f>
-        <v>1.8719999999999999</v>
+        <v>1.9079999999999999</v>
       </c>
       <c r="F3" s="13">
         <f>+a!K5*a!$D$5</f>
-        <v>2.7629999999999999</v>
+        <v>2.8574999999999999</v>
       </c>
       <c r="G3" s="13">
         <f>+a!L5*a!$D$5</f>
-        <v>3.6269999999999998</v>
+        <v>3.6494999999999997</v>
       </c>
       <c r="H3" s="13">
         <f>+a!M5*a!$D$5</f>
-        <v>4.4234999999999998</v>
+        <v>4.4504999999999999</v>
       </c>
       <c r="I3" s="13">
         <f>+a!N5*a!$D$5</f>
-        <v>5.2784999999999993</v>
+        <v>5.1749999999999998</v>
       </c>
       <c r="J3" s="13">
         <f>+a!O5*a!$D$5</f>
-        <v>5.9129999999999994</v>
+        <v>5.9174999999999995</v>
       </c>
       <c r="K3" s="13">
         <f>+a!P5*a!$D$5</f>
-        <v>6.6509999999999998</v>
+        <v>6.5654999999999992</v>
       </c>
       <c r="L3" s="13">
         <f>+a!Q5*a!$D$5</f>
-        <v>7.4204999999999997</v>
+        <v>7.3259999999999996</v>
       </c>
       <c r="M3" s="13">
         <f>+a!R5*a!$D$5</f>
-        <v>7.9874999999999998</v>
-      </c>
-      <c r="N3" s="13">
+        <v>7.9019999999999992</v>
+      </c>
+      <c r="N3" s="13" t="e">
         <f>+a!S5*a!$D$5</f>
-        <v>8.599499999999999</v>
-      </c>
-      <c r="O3" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="O3" s="13" t="e">
         <f>+a!T5*a!$D$5</f>
-        <v>9.0854999999999997</v>
-      </c>
-      <c r="P3" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="P3" s="13" t="e">
         <f>+a!U5*a!$D$5</f>
-        <v>9.6389999999999993</v>
+        <v>#N/A</v>
       </c>
       <c r="Q3" s="13" t="e">
         <f>+a!V5*a!$D$5</f>
@@ -1678,55 +1678,55 @@
     <row r="4" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D4" s="13">
         <f>+a!I6*a!$D$6</f>
-        <v>12.726000000000001</v>
+        <v>12.789</v>
       </c>
       <c r="E4" s="13">
         <f>+a!J6*a!$D$6</f>
-        <v>26.207999999999998</v>
+        <v>26.712</v>
       </c>
       <c r="F4" s="13">
         <f>+a!K6*a!$D$6</f>
-        <v>38.682000000000002</v>
+        <v>40.005000000000003</v>
       </c>
       <c r="G4" s="13">
         <f>+a!L6*a!$D$6</f>
-        <v>50.777999999999999</v>
+        <v>51.093000000000004</v>
       </c>
       <c r="H4" s="13">
         <f>+a!M6*a!$D$6</f>
-        <v>61.929000000000002</v>
+        <v>62.307000000000002</v>
       </c>
       <c r="I4" s="13">
         <f>+a!N6*a!$D$6</f>
-        <v>73.899000000000001</v>
+        <v>72.45</v>
       </c>
       <c r="J4" s="13">
         <f>+a!O6*a!$D$6</f>
-        <v>82.781999999999996</v>
+        <v>82.844999999999999</v>
       </c>
       <c r="K4" s="13">
         <f>+a!P6*a!$D$6</f>
-        <v>93.114000000000004</v>
+        <v>91.917000000000002</v>
       </c>
       <c r="L4" s="13">
         <f>+a!Q6*a!$D$6</f>
-        <v>103.887</v>
+        <v>102.56400000000001</v>
       </c>
       <c r="M4" s="13">
         <f>+a!R6*a!$D$6</f>
-        <v>111.825</v>
-      </c>
-      <c r="N4" s="13">
+        <v>110.628</v>
+      </c>
+      <c r="N4" s="13" t="e">
         <f>+a!S6*a!$D$6</f>
-        <v>120.393</v>
-      </c>
-      <c r="O4" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="O4" s="13" t="e">
         <f>+a!T6*a!$D$6</f>
-        <v>127.197</v>
-      </c>
-      <c r="P4" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="P4" s="13" t="e">
         <f>+a!U6*a!$D$6</f>
-        <v>134.946</v>
+        <v>#N/A</v>
       </c>
       <c r="Q4" s="13" t="e">
         <f>+a!V6*a!$D$6</f>
@@ -1764,55 +1764,55 @@
     <row r="5" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D5" s="13">
         <f>+a!I1*a!$D$1</f>
-        <v>5.1150000000000002</v>
+        <v>4.4385000000000003</v>
       </c>
       <c r="E5" s="13">
         <f>+a!J1*a!$D$1</f>
-        <v>10.032</v>
+        <v>8.7945000000000011</v>
       </c>
       <c r="F5" s="13">
         <f>+a!K1*a!$D$1</f>
-        <v>14.949</v>
+        <v>12.969000000000001</v>
       </c>
       <c r="G5" s="13">
         <f>+a!L1*a!$D$1</f>
-        <v>19.206</v>
+        <v>16.747500000000002</v>
       </c>
       <c r="H5" s="13">
         <f>+a!M1*a!$D$1</f>
-        <v>23.8095</v>
+        <v>20.658000000000001</v>
       </c>
       <c r="I5" s="13">
         <f>+a!N1*a!$D$1</f>
-        <v>27.901500000000002</v>
+        <v>24.585000000000001</v>
       </c>
       <c r="J5" s="13">
         <f>+a!O1*a!$D$1</f>
-        <v>32.142000000000003</v>
+        <v>28.2315</v>
       </c>
       <c r="K5" s="13">
         <f>+a!P1*a!$D$1</f>
-        <v>35.689500000000002</v>
+        <v>31.482000000000003</v>
       </c>
       <c r="L5" s="13">
         <f>+a!Q1*a!$D$1</f>
-        <v>39.138000000000005</v>
+        <v>34.402500000000003</v>
       </c>
       <c r="M5" s="13">
         <f>+a!R1*a!$D$1</f>
-        <v>42.834000000000003</v>
-      </c>
-      <c r="N5" s="13">
+        <v>37.669499999999999</v>
+      </c>
+      <c r="N5" s="13" t="e">
         <f>+a!S1*a!$D$1</f>
-        <v>46.513500000000001</v>
-      </c>
-      <c r="O5" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="O5" s="13" t="e">
         <f>+a!T1*a!$D$1</f>
-        <v>50.011500000000005</v>
-      </c>
-      <c r="P5" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="P5" s="13" t="e">
         <f>+a!U1*a!$D$1</f>
-        <v>52.866</v>
+        <v>#N/A</v>
       </c>
       <c r="Q5" s="13" t="e">
         <f>+a!V1*a!$D$1</f>
@@ -1850,55 +1850,55 @@
     <row r="6" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D6" s="13">
         <f>+a!I2*a!$D$2</f>
-        <v>16.12</v>
+        <v>13.988</v>
       </c>
       <c r="E6" s="13">
         <f>+a!J2*a!$D$2</f>
-        <v>31.616</v>
+        <v>27.715999999999998</v>
       </c>
       <c r="F6" s="13">
         <f>+a!K2*a!$D$2</f>
-        <v>47.111999999999995</v>
+        <v>40.872</v>
       </c>
       <c r="G6" s="13">
         <f>+a!L2*a!$D$2</f>
-        <v>60.527999999999999</v>
+        <v>52.779999999999994</v>
       </c>
       <c r="H6" s="13">
         <f>+a!M2*a!$D$2</f>
-        <v>75.036000000000001</v>
+        <v>65.103999999999999</v>
       </c>
       <c r="I6" s="13">
         <f>+a!N2*a!$D$2</f>
-        <v>87.932000000000002</v>
+        <v>77.47999999999999</v>
       </c>
       <c r="J6" s="13">
         <f>+a!O2*a!$D$2</f>
-        <v>101.29599999999999</v>
+        <v>88.971999999999994</v>
       </c>
       <c r="K6" s="13">
         <f>+a!P2*a!$D$2</f>
-        <v>112.476</v>
+        <v>99.215999999999994</v>
       </c>
       <c r="L6" s="13">
         <f>+a!Q2*a!$D$2</f>
-        <v>123.34399999999999</v>
+        <v>108.42</v>
       </c>
       <c r="M6" s="13">
         <f>+a!R2*a!$D$2</f>
-        <v>134.99199999999999</v>
-      </c>
-      <c r="N6" s="13">
+        <v>118.71599999999999</v>
+      </c>
+      <c r="N6" s="13" t="e">
         <f>+a!S2*a!$D$2</f>
-        <v>146.58799999999999</v>
-      </c>
-      <c r="O6" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="O6" s="13" t="e">
         <f>+a!T2*a!$D$2</f>
-        <v>157.61199999999999</v>
-      </c>
-      <c r="P6" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="P6" s="13" t="e">
         <f>+a!U2*a!$D$2</f>
-        <v>166.608</v>
+        <v>#N/A</v>
       </c>
       <c r="Q6" s="13" t="e">
         <f>+a!V2*a!$D$2</f>
@@ -1936,55 +1936,55 @@
     <row r="7" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D7" s="13">
         <f>+a!I3*a!$D$3</f>
-        <v>41.580000000000005</v>
+        <v>36.82</v>
       </c>
       <c r="E7" s="13">
         <f>+a!J3*a!$D$3</f>
-        <v>79.660000000000011</v>
+        <v>69.580000000000013</v>
       </c>
       <c r="F7" s="13">
         <f>+a!K3*a!$D$3</f>
-        <v>113.4</v>
+        <v>98.7</v>
       </c>
       <c r="G7" s="13">
         <f>+a!L3*a!$D$3</f>
-        <v>150.08000000000001</v>
+        <v>131.04000000000002</v>
       </c>
       <c r="H7" s="13">
         <f>+a!M3*a!$D$3</f>
-        <v>185.08</v>
+        <v>162.82000000000002</v>
       </c>
       <c r="I7" s="13">
         <f>+a!N3*a!$D$3</f>
-        <v>217.84000000000003</v>
+        <v>190.96</v>
       </c>
       <c r="J7" s="13">
         <f>+a!O3*a!$D$3</f>
-        <v>249.76000000000002</v>
+        <v>217.98000000000002</v>
       </c>
       <c r="K7" s="13">
         <f>+a!P3*a!$D$3</f>
-        <v>282.94000000000005</v>
+        <v>247.52</v>
       </c>
       <c r="L7" s="13">
         <f>+a!Q3*a!$D$3</f>
-        <v>314.3</v>
+        <v>275.38000000000005</v>
       </c>
       <c r="M7" s="13">
         <f>+a!R3*a!$D$3</f>
-        <v>340.20000000000005</v>
-      </c>
-      <c r="N7" s="13">
+        <v>297.78000000000003</v>
+      </c>
+      <c r="N7" s="13" t="e">
         <f>+a!S3*a!$D$3</f>
-        <v>362.6</v>
-      </c>
-      <c r="O7" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="O7" s="13" t="e">
         <f>+a!T3*a!$D$3</f>
-        <v>388.92</v>
-      </c>
-      <c r="P7" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="P7" s="13" t="e">
         <f>+a!U3*a!$D$3</f>
-        <v>414.54</v>
+        <v>#N/A</v>
       </c>
       <c r="Q7" s="13" t="e">
         <f>+a!V3*a!$D$3</f>
@@ -2022,55 +2022,55 @@
     <row r="8" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D8" s="13">
         <f>+a!I4*a!$D$4</f>
-        <v>31.0365</v>
+        <v>27.483499999999999</v>
       </c>
       <c r="E8" s="13">
         <f>+a!J4*a!$D$4</f>
-        <v>59.460499999999996</v>
+        <v>51.936499999999995</v>
       </c>
       <c r="F8" s="13">
         <f>+a!K4*a!$D$4</f>
-        <v>84.644999999999996</v>
+        <v>73.672499999999999</v>
       </c>
       <c r="G8" s="13">
         <f>+a!L4*a!$D$4</f>
-        <v>112.024</v>
+        <v>97.811999999999998</v>
       </c>
       <c r="H8" s="13">
         <f>+a!M4*a!$D$4</f>
-        <v>138.149</v>
+        <v>121.53349999999999</v>
       </c>
       <c r="I8" s="13">
         <f>+a!N4*a!$D$4</f>
-        <v>162.602</v>
+        <v>142.53799999999998</v>
       </c>
       <c r="J8" s="13">
         <f>+a!O4*a!$D$4</f>
-        <v>186.428</v>
+        <v>162.70650000000001</v>
       </c>
       <c r="K8" s="13">
         <f>+a!P4*a!$D$4</f>
-        <v>211.19450000000001</v>
+        <v>184.756</v>
       </c>
       <c r="L8" s="13">
         <f>+a!Q4*a!$D$4</f>
-        <v>234.60249999999999</v>
+        <v>205.5515</v>
       </c>
       <c r="M8" s="13">
         <f>+a!R4*a!$D$4</f>
-        <v>253.935</v>
-      </c>
-      <c r="N8" s="13">
+        <v>222.2715</v>
+      </c>
+      <c r="N8" s="13" t="e">
         <f>+a!S4*a!$D$4</f>
-        <v>270.65499999999997</v>
-      </c>
-      <c r="O8" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="O8" s="13" t="e">
         <f>+a!T4*a!$D$4</f>
-        <v>290.30099999999999</v>
-      </c>
-      <c r="P8" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="P8" s="13" t="e">
         <f>+a!U4*a!$D$4</f>
-        <v>309.42449999999997</v>
+        <v>#N/A</v>
       </c>
       <c r="Q8" s="13" t="e">
         <f>+a!V4*a!$D$4</f>
@@ -2108,55 +2108,55 @@
     <row r="9" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D9" s="13">
         <f>+a!I7*a!$D$5</f>
-        <v>3.8609999999999998</v>
+        <v>4.5269999999999992</v>
       </c>
       <c r="E9" s="13">
         <f>+a!J7*a!$D$5</f>
-        <v>7.5239999999999991</v>
+        <v>8.7749999999999986</v>
       </c>
       <c r="F9" s="13">
         <f>+a!K7*a!$D$5</f>
-        <v>11.186999999999999</v>
+        <v>13.023</v>
       </c>
       <c r="G9" s="13">
         <f>+a!L7*a!$D$5</f>
-        <v>14.661</v>
+        <v>17.180999999999997</v>
       </c>
       <c r="H9" s="13">
         <f>+a!M7*a!$D$5</f>
-        <v>17.783999999999999</v>
+        <v>20.88</v>
       </c>
       <c r="I9" s="13">
         <f>+a!N7*a!$D$5</f>
-        <v>20.817</v>
+        <v>24.560999999999996</v>
       </c>
       <c r="J9" s="13">
         <f>+a!O7*a!$D$5</f>
-        <v>23.876999999999999</v>
+        <v>28.043999999999997</v>
       </c>
       <c r="K9" s="13">
         <f>+a!P7*a!$D$5</f>
-        <v>26.648999999999997</v>
+        <v>31.391999999999996</v>
       </c>
       <c r="L9" s="13">
         <f>+a!Q7*a!$D$5</f>
-        <v>29.159999999999997</v>
+        <v>34.433999999999997</v>
       </c>
       <c r="M9" s="13">
         <f>+a!R7*a!$D$5</f>
-        <v>31.931999999999999</v>
-      </c>
-      <c r="N9" s="13">
+        <v>37.646999999999998</v>
+      </c>
+      <c r="N9" s="13" t="e">
         <f>+a!S7*a!$D$5</f>
-        <v>34.506</v>
-      </c>
-      <c r="O9" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="O9" s="13" t="e">
         <f>+a!T7*a!$D$5</f>
-        <v>36.836999999999996</v>
-      </c>
-      <c r="P9" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="P9" s="13" t="e">
         <f>+a!U7*a!$D$5</f>
-        <v>39.104999999999997</v>
+        <v>#N/A</v>
       </c>
       <c r="Q9" s="13" t="e">
         <f>+a!V7*a!$D$5</f>
@@ -2194,49 +2194,49 @@
     <row r="10" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D10">
         <f>SUM(D3:D8)</f>
-        <v>107.48650000000002</v>
+        <v>96.432500000000005</v>
       </c>
       <c r="E10" s="13">
         <f t="shared" ref="E10:M10" si="1">SUM(E3:E8)</f>
-        <v>208.8485</v>
+        <v>186.64700000000002</v>
       </c>
       <c r="F10" s="13">
         <f t="shared" si="1"/>
-        <v>301.55099999999999</v>
+        <v>269.07600000000002</v>
       </c>
       <c r="G10" s="13">
         <f t="shared" si="1"/>
-        <v>396.24300000000005</v>
+        <v>353.12200000000001</v>
       </c>
       <c r="H10" s="13">
         <f t="shared" si="1"/>
-        <v>488.42700000000002</v>
+        <v>436.87300000000005</v>
       </c>
       <c r="I10" s="13">
         <f t="shared" si="1"/>
-        <v>575.45299999999997</v>
+        <v>513.18799999999999</v>
       </c>
       <c r="J10" s="13">
         <f t="shared" si="1"/>
-        <v>658.32100000000003</v>
+        <v>586.65250000000003</v>
       </c>
       <c r="K10" s="13">
         <f t="shared" si="1"/>
-        <v>742.06500000000005</v>
+        <v>661.45650000000001</v>
       </c>
       <c r="L10" s="13">
         <f t="shared" si="1"/>
-        <v>822.69200000000001</v>
+        <v>733.64400000000012</v>
       </c>
       <c r="M10" s="13">
         <f t="shared" si="1"/>
-        <v>891.77350000000001</v>
+        <v>794.9670000000001</v>
       </c>
     </row>
     <row r="14" spans="4:24" x14ac:dyDescent="0.25">
       <c r="E14" s="13">
         <f>+a!G5*a!E5*a!I5</f>
-        <v>11586280.616064001</v>
+        <v>11643638.440896001</v>
       </c>
       <c r="G14" s="13">
         <f>+(a!G5+a!H5)*a!$E$7</f>
@@ -2244,13 +2244,13 @@
       </c>
       <c r="H14">
         <f>+E14/G14</f>
-        <v>97.579032258064515</v>
+        <v>98.062096774193549</v>
       </c>
     </row>
     <row r="15" spans="4:24" x14ac:dyDescent="0.25">
       <c r="E15" s="13">
         <f>+a!G6*a!E6*a!I6</f>
-        <v>11009000</v>
+        <v>11063500</v>
       </c>
       <c r="G15" s="13">
         <f>+(a!G6+a!H6)*a!$E$7</f>
@@ -2258,13 +2258,13 @@
       </c>
       <c r="H15" s="13">
         <f t="shared" ref="H15:H19" si="2">+E15/G15</f>
-        <v>88.107242897158869</v>
+        <v>88.543417366946784</v>
       </c>
     </row>
     <row r="16" spans="4:24" x14ac:dyDescent="0.25">
       <c r="E16" s="13">
         <f>+a!G1*a!E1*a!I1</f>
-        <v>7595000</v>
+        <v>6590500</v>
       </c>
       <c r="G16" s="13">
         <f>+(a!G1+a!H1)*a!$E$7</f>
@@ -2272,13 +2272,13 @@
       </c>
       <c r="H16" s="13">
         <f t="shared" si="2"/>
-        <v>62.449637389202259</v>
+        <v>54.190169218372283</v>
       </c>
     </row>
     <row r="17" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E17" s="13">
         <f>+a!G2*a!E2*a!I2</f>
-        <v>4976493.9840000002</v>
+        <v>4318312.5216000006</v>
       </c>
       <c r="G17" s="13">
         <f>+(a!G2+a!H2)*a!$E$7</f>
@@ -2286,7 +2286,7 @@
       </c>
       <c r="H17" s="13">
         <f t="shared" si="2"/>
-        <v>62.16577540106951</v>
+        <v>53.94385026737968</v>
       </c>
     </row>
     <row r="18" spans="5:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Se modificó Impacto.exe y la interfaz, colocando las variables de tipo de vehiculo fijas.
</commit_message>
<xml_diff>
--- a/evsim/Impac.Amb..xlsx
+++ b/evsim/Impac.Amb..xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="435" windowWidth="20115" windowHeight="7635"/>
+    <workbookView xWindow="240" yWindow="495" windowWidth="20115" windowHeight="7575"/>
   </bookViews>
   <sheets>
     <sheet name="a" sheetId="1" r:id="rId1"/>
@@ -125,7 +125,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="56">
   <si>
     <t>Ford Fusion Hybrid Titanium</t>
   </si>
@@ -170,16 +170,140 @@
   </si>
   <si>
     <t>Numero de Spark requeridos</t>
+  </si>
+  <si>
+    <t>VP1</t>
+  </si>
+  <si>
+    <t>VP2</t>
+  </si>
+  <si>
+    <t>VP3</t>
+  </si>
+  <si>
+    <t>VP4</t>
+  </si>
+  <si>
+    <t>VP5</t>
+  </si>
+  <si>
+    <t>CC1</t>
+  </si>
+  <si>
+    <t>CC2</t>
+  </si>
+  <si>
+    <t>CC3</t>
+  </si>
+  <si>
+    <t>CC4</t>
+  </si>
+  <si>
+    <t>CC5</t>
+  </si>
+  <si>
+    <t>CC6</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>B4</t>
+  </si>
+  <si>
+    <t>TM</t>
+  </si>
+  <si>
+    <t>ET1</t>
+  </si>
+  <si>
+    <t>ET2</t>
+  </si>
+  <si>
+    <t>MB</t>
+  </si>
+  <si>
+    <t>MBG</t>
+  </si>
+  <si>
+    <t>MC</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>T2</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>C7</t>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>No. De Vehiculos</t>
+  </si>
+  <si>
+    <t>FA (Km/Año)</t>
+  </si>
+  <si>
+    <t>Factor de Emisiones</t>
+  </si>
+  <si>
+    <t>CO2</t>
+  </si>
+  <si>
+    <t>CO</t>
+  </si>
+  <si>
+    <t>NOX</t>
+  </si>
+  <si>
+    <t>THC</t>
+  </si>
+  <si>
+    <t>PM</t>
+  </si>
+  <si>
+    <t>Tipo de Vehiculos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
     <numFmt numFmtId="166" formatCode="0.000"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -238,7 +362,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -381,12 +505,84 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -483,6 +679,54 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -786,7 +1030,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC16"/>
+  <dimension ref="A1:AC50"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D10" sqref="D10:D15"/>
@@ -848,34 +1092,34 @@
         <v>22</v>
       </c>
       <c r="I1" s="15">
-        <v>134.5</v>
+        <v>126</v>
       </c>
       <c r="J1" s="15">
-        <v>266.5</v>
+        <v>253.5</v>
       </c>
       <c r="K1" s="15">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="L1" s="15">
-        <v>507.5</v>
+        <v>489.5</v>
       </c>
       <c r="M1" s="15">
-        <v>626</v>
+        <v>604</v>
       </c>
       <c r="N1" s="15">
-        <v>745</v>
+        <v>721.5</v>
       </c>
       <c r="O1" s="15">
-        <v>855.5</v>
+        <v>829</v>
       </c>
       <c r="P1" s="15">
-        <v>954</v>
+        <v>927</v>
       </c>
       <c r="Q1" s="15">
-        <v>1042.5</v>
-      </c>
-      <c r="R1" s="15">
-        <v>1141.5</v>
+        <v>1009</v>
+      </c>
+      <c r="R1" s="15" t="e">
+        <v>#N/A</v>
       </c>
       <c r="S1" s="15" t="e">
         <v>#N/A</v>
@@ -937,34 +1181,34 @@
         <v>61.155072000000004</v>
       </c>
       <c r="I2" s="17">
-        <v>134.5</v>
+        <v>126</v>
       </c>
       <c r="J2" s="15">
-        <v>266.5</v>
+        <v>253.5</v>
       </c>
       <c r="K2" s="17">
-        <v>393</v>
+        <v>381</v>
       </c>
       <c r="L2" s="15">
-        <v>507.5</v>
+        <v>489.5</v>
       </c>
       <c r="M2" s="17">
-        <v>626</v>
+        <v>604</v>
       </c>
       <c r="N2" s="15">
-        <v>745</v>
+        <v>721.5</v>
       </c>
       <c r="O2" s="17">
-        <v>855.5</v>
+        <v>829</v>
       </c>
       <c r="P2" s="15">
-        <v>954</v>
+        <v>927</v>
       </c>
       <c r="Q2" s="17">
-        <v>1042.5</v>
-      </c>
-      <c r="R2" s="15">
-        <v>1141.5</v>
+        <v>1009</v>
+      </c>
+      <c r="R2" s="15" t="e">
+        <v>#N/A</v>
       </c>
       <c r="S2" s="17" t="e">
         <v>#N/A</v>
@@ -1026,34 +1270,34 @@
         <v>185</v>
       </c>
       <c r="I3" s="18">
-        <v>131.5</v>
+        <v>128.5</v>
       </c>
       <c r="J3" s="15">
-        <v>248.5</v>
+        <v>243</v>
       </c>
       <c r="K3" s="18">
-        <v>352.5</v>
+        <v>342</v>
       </c>
       <c r="L3" s="15">
-        <v>468</v>
+        <v>456</v>
       </c>
       <c r="M3" s="18">
-        <v>581.5</v>
+        <v>567</v>
       </c>
       <c r="N3" s="15">
-        <v>682</v>
+        <v>663</v>
       </c>
       <c r="O3" s="18">
-        <v>778.5</v>
+        <v>756.5</v>
       </c>
       <c r="P3" s="15">
-        <v>884</v>
+        <v>857</v>
       </c>
       <c r="Q3" s="18">
-        <v>983.5</v>
-      </c>
-      <c r="R3" s="15">
-        <v>1063.5</v>
+        <v>955</v>
+      </c>
+      <c r="R3" s="15" t="e">
+        <v>#N/A</v>
       </c>
       <c r="S3" s="18" t="e">
         <v>#N/A</v>
@@ -1115,34 +1359,34 @@
         <v>141.62227200000001</v>
       </c>
       <c r="I4" s="17">
-        <v>131.5</v>
+        <v>128.5</v>
       </c>
       <c r="J4" s="15">
-        <v>248.5</v>
+        <v>243</v>
       </c>
       <c r="K4" s="17">
-        <v>352.5</v>
+        <v>342</v>
       </c>
       <c r="L4" s="15">
-        <v>468</v>
+        <v>456</v>
       </c>
       <c r="M4" s="17">
-        <v>581.5</v>
+        <v>567</v>
       </c>
       <c r="N4" s="15">
-        <v>682</v>
+        <v>663</v>
       </c>
       <c r="O4" s="17">
-        <v>778.5</v>
+        <v>756.5</v>
       </c>
       <c r="P4" s="15">
-        <v>884</v>
+        <v>857</v>
       </c>
       <c r="Q4" s="17">
-        <v>983.5</v>
-      </c>
-      <c r="R4" s="15">
-        <v>1063.5</v>
+        <v>955</v>
+      </c>
+      <c r="R4" s="15" t="e">
+        <v>#N/A</v>
       </c>
       <c r="S4" s="17" t="e">
         <v>#N/A</v>
@@ -1204,34 +1448,34 @@
         <v>33.796224000000002</v>
       </c>
       <c r="I5" s="15">
-        <v>101.5</v>
+        <v>107.5</v>
       </c>
       <c r="J5" s="15">
-        <v>212</v>
+        <v>217.5</v>
       </c>
       <c r="K5" s="15">
-        <v>317.5</v>
+        <v>321.5</v>
       </c>
       <c r="L5" s="15">
-        <v>405.5</v>
+        <v>413.5</v>
       </c>
       <c r="M5" s="15">
-        <v>494.5</v>
+        <v>503</v>
       </c>
       <c r="N5" s="15">
-        <v>575</v>
+        <v>583</v>
       </c>
       <c r="O5" s="15">
-        <v>657.5</v>
+        <v>665</v>
       </c>
       <c r="P5" s="15">
-        <v>729.5</v>
+        <v>737</v>
       </c>
       <c r="Q5" s="15">
-        <v>814</v>
-      </c>
-      <c r="R5" s="15">
-        <v>878</v>
+        <v>822.5</v>
+      </c>
+      <c r="R5" s="15" t="e">
+        <v>#N/A</v>
       </c>
       <c r="S5" s="15" t="e">
         <v>#N/A</v>
@@ -1293,34 +1537,34 @@
         <v>50</v>
       </c>
       <c r="I6" s="16">
-        <v>101.5</v>
+        <v>107.5</v>
       </c>
       <c r="J6" s="15">
-        <v>212</v>
+        <v>217.5</v>
       </c>
       <c r="K6" s="16">
-        <v>317.5</v>
+        <v>321.5</v>
       </c>
       <c r="L6" s="15">
-        <v>405.5</v>
+        <v>413.5</v>
       </c>
       <c r="M6" s="16">
-        <v>494.5</v>
+        <v>503</v>
       </c>
       <c r="N6" s="15">
-        <v>575</v>
+        <v>583</v>
       </c>
       <c r="O6" s="16">
-        <v>657.5</v>
+        <v>665</v>
       </c>
       <c r="P6" s="15">
-        <v>729.5</v>
+        <v>737</v>
       </c>
       <c r="Q6" s="16">
-        <v>814</v>
-      </c>
-      <c r="R6" s="15">
-        <v>878</v>
+        <v>822.5</v>
+      </c>
+      <c r="R6" s="15" t="e">
+        <v>#N/A</v>
       </c>
       <c r="S6" s="16" t="e">
         <v>#N/A</v>
@@ -1382,34 +1626,34 @@
         <v>0</v>
       </c>
       <c r="I7" s="18">
-        <v>503</v>
+        <v>514</v>
       </c>
       <c r="J7" s="18">
-        <v>975</v>
+        <v>1001</v>
       </c>
       <c r="K7" s="18">
-        <v>1447</v>
+        <v>1484</v>
       </c>
       <c r="L7" s="18">
-        <v>1909</v>
+        <v>1953</v>
       </c>
       <c r="M7" s="18">
-        <v>2320</v>
+        <v>2376</v>
       </c>
       <c r="N7" s="18">
-        <v>2729</v>
+        <v>2798</v>
       </c>
       <c r="O7" s="18">
-        <v>3116</v>
+        <v>3198</v>
       </c>
       <c r="P7" s="18">
-        <v>3488</v>
+        <v>3581</v>
       </c>
       <c r="Q7" s="18">
-        <v>3826</v>
-      </c>
-      <c r="R7" s="18">
-        <v>4183</v>
+        <v>3933</v>
+      </c>
+      <c r="R7" s="18" t="e">
+        <v>#N/A</v>
       </c>
       <c r="S7" s="18" t="e">
         <v>#N/A</v>
@@ -1466,13 +1710,13 @@
       </c>
       <c r="B10" s="31">
         <f>+I1</f>
-        <v>134.5</v>
+        <v>126</v>
       </c>
       <c r="C10" s="22">
-        <v>6590.5</v>
+        <v>6174</v>
       </c>
       <c r="D10" s="25">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="H10" s="13">
         <v>40.49153908138598</v>
@@ -1484,13 +1728,13 @@
       </c>
       <c r="B11" s="31">
         <f t="shared" ref="B11:B15" si="0">+I2</f>
-        <v>134.5</v>
+        <v>126</v>
       </c>
       <c r="C11" s="22">
-        <v>4318.3125216000008</v>
+        <v>4045.4080128000005</v>
       </c>
       <c r="D11" s="25">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="H11" s="13">
         <v>40.30748663101604</v>
@@ -1502,7 +1746,7 @@
       </c>
       <c r="B12" s="31">
         <f t="shared" si="0"/>
-        <v>131.5</v>
+        <v>128.5</v>
       </c>
       <c r="C12" s="22">
         <v>0</v>
@@ -1520,7 +1764,7 @@
       </c>
       <c r="B13" s="31">
         <f t="shared" si="0"/>
-        <v>131.5</v>
+        <v>128.5</v>
       </c>
       <c r="C13" s="22">
         <v>0</v>
@@ -1538,13 +1782,13 @@
       </c>
       <c r="B14" s="31">
         <f t="shared" si="0"/>
-        <v>101.5</v>
+        <v>107.5</v>
       </c>
       <c r="C14" s="22">
-        <v>11643.638440896</v>
+        <v>12331.93233888</v>
       </c>
       <c r="D14" s="25">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="H14" s="13">
         <v>128.49516129032256</v>
@@ -1556,24 +1800,902 @@
       </c>
       <c r="B15" s="34">
         <f t="shared" si="0"/>
-        <v>101.5</v>
+        <v>107.5</v>
       </c>
       <c r="C15" s="26">
-        <v>11063.5</v>
+        <v>11717.5</v>
       </c>
       <c r="D15" s="27">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="H15" s="13">
         <v>116.02240896358543</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:29" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="Y16" s="13"/>
       <c r="AA16" s="13"/>
       <c r="AB16" s="13"/>
     </row>
+    <row r="17" spans="1:9" s="13" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="50" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="43" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="D17" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="E17" s="46"/>
+      <c r="F17" s="46"/>
+      <c r="G17" s="46"/>
+      <c r="H17" s="47"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="50"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="49"/>
+      <c r="D18" s="35" t="s">
+        <v>50</v>
+      </c>
+      <c r="E18" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" s="35" t="s">
+        <v>52</v>
+      </c>
+      <c r="G18" s="35" t="s">
+        <v>53</v>
+      </c>
+      <c r="H18" s="40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="35" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="42">
+        <v>0.19019918803001115</v>
+      </c>
+      <c r="C19" s="36">
+        <v>13140</v>
+      </c>
+      <c r="D19" s="36">
+        <v>232</v>
+      </c>
+      <c r="E19" s="36">
+        <v>7.2</v>
+      </c>
+      <c r="F19" s="36">
+        <v>0.73</v>
+      </c>
+      <c r="G19" s="36">
+        <v>0.9</v>
+      </c>
+      <c r="H19" s="37">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="I19" s="41"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="35" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20" s="42">
+        <v>0.12592471148581261</v>
+      </c>
+      <c r="C20" s="36">
+        <v>18250</v>
+      </c>
+      <c r="D20" s="36">
+        <v>312</v>
+      </c>
+      <c r="E20" s="36">
+        <v>8.5</v>
+      </c>
+      <c r="F20" s="36">
+        <v>0.9</v>
+      </c>
+      <c r="G20" s="36">
+        <v>0.9</v>
+      </c>
+      <c r="H20" s="37">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="I20" s="41"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="42">
+        <v>0.13007809667340331</v>
+      </c>
+      <c r="C21" s="36">
+        <v>9490</v>
+      </c>
+      <c r="D21" s="36">
+        <v>218</v>
+      </c>
+      <c r="E21" s="36">
+        <v>58</v>
+      </c>
+      <c r="F21" s="36">
+        <v>1.2</v>
+      </c>
+      <c r="G21" s="36">
+        <v>7.2</v>
+      </c>
+      <c r="H21" s="37">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="42">
+        <v>0.10829909838331163</v>
+      </c>
+      <c r="C22" s="36">
+        <v>9490</v>
+      </c>
+      <c r="D22" s="36">
+        <v>312</v>
+      </c>
+      <c r="E22" s="36">
+        <v>69</v>
+      </c>
+      <c r="F22" s="36">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="G22" s="36">
+        <v>9</v>
+      </c>
+      <c r="H22" s="37">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="35" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="42">
+        <v>1.0054513180587128E-2</v>
+      </c>
+      <c r="C23" s="36">
+        <v>12993</v>
+      </c>
+      <c r="D23" s="36">
+        <v>241</v>
+      </c>
+      <c r="E23" s="36">
+        <v>13</v>
+      </c>
+      <c r="F23" s="36">
+        <v>3.7</v>
+      </c>
+      <c r="G23" s="36">
+        <v>5</v>
+      </c>
+      <c r="H23" s="37">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="35" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="42">
+        <v>0.10486246640876162</v>
+      </c>
+      <c r="C24" s="36">
+        <v>21900</v>
+      </c>
+      <c r="D24" s="36">
+        <v>379</v>
+      </c>
+      <c r="E24" s="36">
+        <v>11</v>
+      </c>
+      <c r="F24" s="36">
+        <v>1</v>
+      </c>
+      <c r="G24" s="36">
+        <v>0.7</v>
+      </c>
+      <c r="H24" s="37">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="35" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="42">
+        <v>5.0473298840898656E-2</v>
+      </c>
+      <c r="C25" s="36">
+        <v>12331</v>
+      </c>
+      <c r="D25" s="36">
+        <v>385</v>
+      </c>
+      <c r="E25" s="36">
+        <v>73</v>
+      </c>
+      <c r="F25" s="36">
+        <v>3</v>
+      </c>
+      <c r="G25" s="36">
+        <v>10</v>
+      </c>
+      <c r="H25" s="37">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A26" s="35" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26" s="42">
+        <v>4.4451310702008272E-2</v>
+      </c>
+      <c r="C26" s="36">
+        <v>12540</v>
+      </c>
+      <c r="D26" s="36">
+        <v>460</v>
+      </c>
+      <c r="E26" s="36">
+        <v>85</v>
+      </c>
+      <c r="F26" s="36">
+        <v>4</v>
+      </c>
+      <c r="G26" s="36">
+        <v>7.5</v>
+      </c>
+      <c r="H26" s="37">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="35" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="42">
+        <v>2.7921846574876012E-2</v>
+      </c>
+      <c r="C27" s="36">
+        <v>13140</v>
+      </c>
+      <c r="D27" s="36">
+        <v>442</v>
+      </c>
+      <c r="E27" s="36">
+        <v>34</v>
+      </c>
+      <c r="F27" s="36">
+        <v>3.5</v>
+      </c>
+      <c r="G27" s="36">
+        <v>4</v>
+      </c>
+      <c r="H27" s="37">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="42">
+        <v>4.7745012417066291E-3</v>
+      </c>
+      <c r="C28" s="36">
+        <v>21900</v>
+      </c>
+      <c r="D28" s="36">
+        <v>236.92</v>
+      </c>
+      <c r="E28" s="36">
+        <v>1.39</v>
+      </c>
+      <c r="F28" s="36">
+        <v>1.01</v>
+      </c>
+      <c r="G28" s="36">
+        <v>0.79</v>
+      </c>
+      <c r="H28" s="37">
+        <v>9.7000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="B29" s="42">
+        <v>8.2289994986931344E-3</v>
+      </c>
+      <c r="C29" s="36">
+        <v>12436</v>
+      </c>
+      <c r="D29" s="36">
+        <v>310</v>
+      </c>
+      <c r="E29" s="36">
+        <v>1.39</v>
+      </c>
+      <c r="F29" s="36">
+        <v>1.01</v>
+      </c>
+      <c r="G29" s="36">
+        <v>0.79</v>
+      </c>
+      <c r="H29" s="37">
+        <v>9.7000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" s="42">
+        <v>0</v>
+      </c>
+      <c r="C30" s="36">
+        <v>65700</v>
+      </c>
+      <c r="D30" s="36">
+        <v>561.16</v>
+      </c>
+      <c r="E30" s="36">
+        <v>5.87</v>
+      </c>
+      <c r="F30" s="36">
+        <v>9.7799999999999994</v>
+      </c>
+      <c r="G30" s="36">
+        <v>1.22</v>
+      </c>
+      <c r="H30" s="37">
+        <v>0.25600000000000001</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="42">
+        <v>0</v>
+      </c>
+      <c r="C31" s="36">
+        <v>65700</v>
+      </c>
+      <c r="D31" s="36">
+        <v>787.03</v>
+      </c>
+      <c r="E31" s="36">
+        <v>9.08</v>
+      </c>
+      <c r="F31" s="36">
+        <v>15.2</v>
+      </c>
+      <c r="G31" s="36">
+        <v>1.88</v>
+      </c>
+      <c r="H31" s="37">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" s="42">
+        <v>0</v>
+      </c>
+      <c r="C32" s="36">
+        <v>65700</v>
+      </c>
+      <c r="D32" s="36">
+        <v>487.7</v>
+      </c>
+      <c r="E32" s="36">
+        <v>88.08</v>
+      </c>
+      <c r="F32" s="36">
+        <v>5.24</v>
+      </c>
+      <c r="G32" s="36">
+        <v>5.33</v>
+      </c>
+      <c r="H32" s="37">
+        <v>4.1000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="35" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="42">
+        <v>0</v>
+      </c>
+      <c r="C33" s="36">
+        <v>65700</v>
+      </c>
+      <c r="D33" s="36">
+        <v>494.4</v>
+      </c>
+      <c r="E33" s="36">
+        <v>105.94</v>
+      </c>
+      <c r="F33" s="36">
+        <v>6.23</v>
+      </c>
+      <c r="G33" s="36">
+        <v>12</v>
+      </c>
+      <c r="H33" s="37">
+        <v>4.1000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" s="42">
+        <v>0</v>
+      </c>
+      <c r="C34" s="36">
+        <v>69300</v>
+      </c>
+      <c r="D34" s="36">
+        <v>685.16</v>
+      </c>
+      <c r="E34" s="36">
+        <v>1.84</v>
+      </c>
+      <c r="F34" s="36">
+        <v>7.33</v>
+      </c>
+      <c r="G34" s="36">
+        <v>0.73</v>
+      </c>
+      <c r="H34" s="37">
+        <v>0.29399999999999998</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="B35" s="42">
+        <v>0</v>
+      </c>
+      <c r="C35" s="36">
+        <v>63000</v>
+      </c>
+      <c r="D35" s="36">
+        <v>561.16</v>
+      </c>
+      <c r="E35" s="36">
+        <v>5.87</v>
+      </c>
+      <c r="F35" s="36">
+        <v>9.7799999999999994</v>
+      </c>
+      <c r="G35" s="36">
+        <v>1.22</v>
+      </c>
+      <c r="H35" s="37">
+        <v>0.61199999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="42">
+        <v>0</v>
+      </c>
+      <c r="C36" s="36">
+        <v>63000</v>
+      </c>
+      <c r="D36" s="36">
+        <v>787.03</v>
+      </c>
+      <c r="E36" s="36">
+        <v>9.08</v>
+      </c>
+      <c r="F36" s="36">
+        <v>15.21</v>
+      </c>
+      <c r="G36" s="36">
+        <v>1.88</v>
+      </c>
+      <c r="H36" s="37">
+        <v>0.61199999999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" s="35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37" s="42">
+        <v>5.5742801201875327E-3</v>
+      </c>
+      <c r="C37" s="36">
+        <v>65700</v>
+      </c>
+      <c r="D37" s="36">
+        <v>376.19</v>
+      </c>
+      <c r="E37" s="36">
+        <v>3.32</v>
+      </c>
+      <c r="F37" s="36">
+        <v>5.99</v>
+      </c>
+      <c r="G37" s="36">
+        <v>0.7</v>
+      </c>
+      <c r="H37" s="37">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="42">
+        <v>4.9184824589889996E-3</v>
+      </c>
+      <c r="C38" s="36">
+        <v>65700</v>
+      </c>
+      <c r="D38" s="36">
+        <v>415.99</v>
+      </c>
+      <c r="E38" s="36">
+        <v>65.2</v>
+      </c>
+      <c r="F38" s="36">
+        <v>3.9</v>
+      </c>
+      <c r="G38" s="36">
+        <v>3.7</v>
+      </c>
+      <c r="H38" s="37">
+        <v>4.2000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="B39" s="42">
+        <v>8.227948540902752E-3</v>
+      </c>
+      <c r="C39" s="36">
+        <v>65700</v>
+      </c>
+      <c r="D39" s="36">
+        <v>272.83</v>
+      </c>
+      <c r="E39" s="36">
+        <v>20.12</v>
+      </c>
+      <c r="F39" s="36">
+        <v>2.27</v>
+      </c>
+      <c r="G39" s="36">
+        <v>0.11</v>
+      </c>
+      <c r="H39" s="37">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B40" s="42">
+        <v>3.2159308385697305E-2</v>
+      </c>
+      <c r="C40" s="36">
+        <v>73000</v>
+      </c>
+      <c r="D40" s="36">
+        <v>258</v>
+      </c>
+      <c r="E40" s="36">
+        <v>8.4</v>
+      </c>
+      <c r="F40" s="36">
+        <v>2</v>
+      </c>
+      <c r="G40" s="36">
+        <v>0.86</v>
+      </c>
+      <c r="H40" s="37">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" s="35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41" s="42">
+        <v>2.1439538923798202E-2</v>
+      </c>
+      <c r="C41" s="36">
+        <v>73000</v>
+      </c>
+      <c r="D41" s="36">
+        <v>241</v>
+      </c>
+      <c r="E41" s="36">
+        <v>13</v>
+      </c>
+      <c r="F41" s="36">
+        <v>3.7</v>
+      </c>
+      <c r="G41" s="36">
+        <v>5</v>
+      </c>
+      <c r="H41" s="37">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" s="35" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="42">
+        <v>0</v>
+      </c>
+      <c r="C42" s="36">
+        <v>31025</v>
+      </c>
+      <c r="D42" s="36">
+        <v>490.87</v>
+      </c>
+      <c r="E42" s="36">
+        <v>6.26</v>
+      </c>
+      <c r="F42" s="36">
+        <v>9.66</v>
+      </c>
+      <c r="G42" s="36">
+        <v>1.24</v>
+      </c>
+      <c r="H42" s="37">
+        <v>0.86899999999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43" s="42">
+        <v>0</v>
+      </c>
+      <c r="C43" s="36">
+        <v>31025</v>
+      </c>
+      <c r="D43" s="36">
+        <v>702.57</v>
+      </c>
+      <c r="E43" s="36">
+        <v>9.49</v>
+      </c>
+      <c r="F43" s="36">
+        <v>14.69</v>
+      </c>
+      <c r="G43" s="36">
+        <v>1.87</v>
+      </c>
+      <c r="H43" s="37">
+        <v>0.84499999999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="35" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44" s="42">
+        <v>0</v>
+      </c>
+      <c r="C44" s="36">
+        <v>31025</v>
+      </c>
+      <c r="D44" s="36">
+        <v>503.2</v>
+      </c>
+      <c r="E44" s="36">
+        <v>1.21</v>
+      </c>
+      <c r="F44" s="36">
+        <v>5</v>
+      </c>
+      <c r="G44" s="36">
+        <v>0.49</v>
+      </c>
+      <c r="H44" s="37">
+        <v>0.311</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45" s="42">
+        <v>0</v>
+      </c>
+      <c r="C45" s="36">
+        <v>31025</v>
+      </c>
+      <c r="D45" s="36">
+        <v>438.92</v>
+      </c>
+      <c r="E45" s="36">
+        <v>85.74</v>
+      </c>
+      <c r="F45" s="36">
+        <v>4.79</v>
+      </c>
+      <c r="G45" s="36">
+        <v>4.6399999999999997</v>
+      </c>
+      <c r="H45" s="37">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" s="35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B46" s="42">
+        <v>0</v>
+      </c>
+      <c r="C46" s="36">
+        <v>31025</v>
+      </c>
+      <c r="D46" s="36">
+        <v>474.77</v>
+      </c>
+      <c r="E46" s="36">
+        <v>108.49</v>
+      </c>
+      <c r="F46" s="36">
+        <v>6</v>
+      </c>
+      <c r="G46" s="36">
+        <v>5.87</v>
+      </c>
+      <c r="H46" s="37">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" s="42">
+        <v>0</v>
+      </c>
+      <c r="C47" s="36">
+        <v>31025</v>
+      </c>
+      <c r="D47" s="36">
+        <v>377.61</v>
+      </c>
+      <c r="E47" s="36">
+        <v>32.46</v>
+      </c>
+      <c r="F47" s="36">
+        <v>2.0099999999999998</v>
+      </c>
+      <c r="G47" s="36">
+        <v>0.15</v>
+      </c>
+      <c r="H47" s="37">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" s="35" t="s">
+        <v>44</v>
+      </c>
+      <c r="B48" s="42">
+        <v>0</v>
+      </c>
+      <c r="C48" s="36">
+        <v>31025</v>
+      </c>
+      <c r="D48" s="36">
+        <v>430.37</v>
+      </c>
+      <c r="E48" s="36">
+        <v>40.840000000000003</v>
+      </c>
+      <c r="F48" s="36">
+        <v>2.5099999999999998</v>
+      </c>
+      <c r="G48" s="36">
+        <v>0.19</v>
+      </c>
+      <c r="H48" s="37">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" s="42">
+        <v>1.6265673721746313E-2</v>
+      </c>
+      <c r="C49" s="36">
+        <v>25000</v>
+      </c>
+      <c r="D49" s="36">
+        <v>28.09</v>
+      </c>
+      <c r="E49" s="36">
+        <v>7.56</v>
+      </c>
+      <c r="F49" s="36">
+        <v>0.03</v>
+      </c>
+      <c r="G49" s="36">
+        <v>4.33</v>
+      </c>
+      <c r="H49" s="37">
+        <v>0.14799999999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A50" s="35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B50" s="42">
+        <v>0.10614673682860876</v>
+      </c>
+      <c r="C50" s="38">
+        <v>25000</v>
+      </c>
+      <c r="D50" s="38">
+        <v>33.11</v>
+      </c>
+      <c r="E50" s="38">
+        <v>6.67</v>
+      </c>
+      <c r="F50" s="38">
+        <v>0.27</v>
+      </c>
+      <c r="G50" s="38">
+        <v>1.67</v>
+      </c>
+      <c r="H50" s="39">
+        <v>0.09</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="D17:H17"/>
+    <mergeCell ref="C17:C18"/>
+    <mergeCell ref="A17:A18"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
@@ -1592,43 +2714,43 @@
     <row r="3" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D3" s="13">
         <f>+a!I5*a!$D$5</f>
-        <v>0.91349999999999998</v>
+        <v>0.96749999999999992</v>
       </c>
       <c r="E3" s="13">
         <f>+a!J5*a!$D$5</f>
-        <v>1.9079999999999999</v>
+        <v>1.9574999999999998</v>
       </c>
       <c r="F3" s="13">
         <f>+a!K5*a!$D$5</f>
-        <v>2.8574999999999999</v>
+        <v>2.8935</v>
       </c>
       <c r="G3" s="13">
         <f>+a!L5*a!$D$5</f>
-        <v>3.6494999999999997</v>
+        <v>3.7214999999999998</v>
       </c>
       <c r="H3" s="13">
         <f>+a!M5*a!$D$5</f>
-        <v>4.4504999999999999</v>
+        <v>4.5269999999999992</v>
       </c>
       <c r="I3" s="13">
         <f>+a!N5*a!$D$5</f>
-        <v>5.1749999999999998</v>
+        <v>5.2469999999999999</v>
       </c>
       <c r="J3" s="13">
         <f>+a!O5*a!$D$5</f>
-        <v>5.9174999999999995</v>
+        <v>5.9849999999999994</v>
       </c>
       <c r="K3" s="13">
         <f>+a!P5*a!$D$5</f>
-        <v>6.5654999999999992</v>
+        <v>6.6329999999999991</v>
       </c>
       <c r="L3" s="13">
         <f>+a!Q5*a!$D$5</f>
-        <v>7.3259999999999996</v>
-      </c>
-      <c r="M3" s="13">
+        <v>7.4024999999999999</v>
+      </c>
+      <c r="M3" s="13" t="e">
         <f>+a!R5*a!$D$5</f>
-        <v>7.9019999999999992</v>
+        <v>#N/A</v>
       </c>
       <c r="N3" s="13" t="e">
         <f>+a!S5*a!$D$5</f>
@@ -1678,43 +2800,43 @@
     <row r="4" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D4" s="13">
         <f>+a!I6*a!$D$6</f>
-        <v>12.789</v>
+        <v>13.545</v>
       </c>
       <c r="E4" s="13">
         <f>+a!J6*a!$D$6</f>
-        <v>26.712</v>
+        <v>27.405000000000001</v>
       </c>
       <c r="F4" s="13">
         <f>+a!K6*a!$D$6</f>
-        <v>40.005000000000003</v>
+        <v>40.509</v>
       </c>
       <c r="G4" s="13">
         <f>+a!L6*a!$D$6</f>
-        <v>51.093000000000004</v>
+        <v>52.100999999999999</v>
       </c>
       <c r="H4" s="13">
         <f>+a!M6*a!$D$6</f>
-        <v>62.307000000000002</v>
+        <v>63.378</v>
       </c>
       <c r="I4" s="13">
         <f>+a!N6*a!$D$6</f>
-        <v>72.45</v>
+        <v>73.457999999999998</v>
       </c>
       <c r="J4" s="13">
         <f>+a!O6*a!$D$6</f>
-        <v>82.844999999999999</v>
+        <v>83.79</v>
       </c>
       <c r="K4" s="13">
         <f>+a!P6*a!$D$6</f>
-        <v>91.917000000000002</v>
+        <v>92.861999999999995</v>
       </c>
       <c r="L4" s="13">
         <f>+a!Q6*a!$D$6</f>
-        <v>102.56400000000001</v>
-      </c>
-      <c r="M4" s="13">
+        <v>103.63500000000001</v>
+      </c>
+      <c r="M4" s="13" t="e">
         <f>+a!R6*a!$D$6</f>
-        <v>110.628</v>
+        <v>#N/A</v>
       </c>
       <c r="N4" s="13" t="e">
         <f>+a!S6*a!$D$6</f>
@@ -1764,43 +2886,43 @@
     <row r="5" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D5" s="13">
         <f>+a!I1*a!$D$1</f>
-        <v>4.4385000000000003</v>
+        <v>4.1580000000000004</v>
       </c>
       <c r="E5" s="13">
         <f>+a!J1*a!$D$1</f>
-        <v>8.7945000000000011</v>
+        <v>8.3655000000000008</v>
       </c>
       <c r="F5" s="13">
         <f>+a!K1*a!$D$1</f>
-        <v>12.969000000000001</v>
+        <v>12.573</v>
       </c>
       <c r="G5" s="13">
         <f>+a!L1*a!$D$1</f>
-        <v>16.747500000000002</v>
+        <v>16.153500000000001</v>
       </c>
       <c r="H5" s="13">
         <f>+a!M1*a!$D$1</f>
-        <v>20.658000000000001</v>
+        <v>19.932000000000002</v>
       </c>
       <c r="I5" s="13">
         <f>+a!N1*a!$D$1</f>
-        <v>24.585000000000001</v>
+        <v>23.8095</v>
       </c>
       <c r="J5" s="13">
         <f>+a!O1*a!$D$1</f>
-        <v>28.2315</v>
+        <v>27.357000000000003</v>
       </c>
       <c r="K5" s="13">
         <f>+a!P1*a!$D$1</f>
-        <v>31.482000000000003</v>
+        <v>30.591000000000001</v>
       </c>
       <c r="L5" s="13">
         <f>+a!Q1*a!$D$1</f>
-        <v>34.402500000000003</v>
-      </c>
-      <c r="M5" s="13">
+        <v>33.297000000000004</v>
+      </c>
+      <c r="M5" s="13" t="e">
         <f>+a!R1*a!$D$1</f>
-        <v>37.669499999999999</v>
+        <v>#N/A</v>
       </c>
       <c r="N5" s="13" t="e">
         <f>+a!S1*a!$D$1</f>
@@ -1850,43 +2972,43 @@
     <row r="6" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D6" s="13">
         <f>+a!I2*a!$D$2</f>
-        <v>13.988</v>
+        <v>13.103999999999999</v>
       </c>
       <c r="E6" s="13">
         <f>+a!J2*a!$D$2</f>
-        <v>27.715999999999998</v>
+        <v>26.363999999999997</v>
       </c>
       <c r="F6" s="13">
         <f>+a!K2*a!$D$2</f>
-        <v>40.872</v>
+        <v>39.623999999999995</v>
       </c>
       <c r="G6" s="13">
         <f>+a!L2*a!$D$2</f>
-        <v>52.779999999999994</v>
+        <v>50.907999999999994</v>
       </c>
       <c r="H6" s="13">
         <f>+a!M2*a!$D$2</f>
-        <v>65.103999999999999</v>
+        <v>62.815999999999995</v>
       </c>
       <c r="I6" s="13">
         <f>+a!N2*a!$D$2</f>
-        <v>77.47999999999999</v>
+        <v>75.036000000000001</v>
       </c>
       <c r="J6" s="13">
         <f>+a!O2*a!$D$2</f>
-        <v>88.971999999999994</v>
+        <v>86.215999999999994</v>
       </c>
       <c r="K6" s="13">
         <f>+a!P2*a!$D$2</f>
-        <v>99.215999999999994</v>
+        <v>96.408000000000001</v>
       </c>
       <c r="L6" s="13">
         <f>+a!Q2*a!$D$2</f>
-        <v>108.42</v>
-      </c>
-      <c r="M6" s="13">
+        <v>104.93599999999999</v>
+      </c>
+      <c r="M6" s="13" t="e">
         <f>+a!R2*a!$D$2</f>
-        <v>118.71599999999999</v>
+        <v>#N/A</v>
       </c>
       <c r="N6" s="13" t="e">
         <f>+a!S2*a!$D$2</f>
@@ -1936,43 +3058,43 @@
     <row r="7" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D7" s="13">
         <f>+a!I3*a!$D$3</f>
-        <v>36.82</v>
+        <v>35.980000000000004</v>
       </c>
       <c r="E7" s="13">
         <f>+a!J3*a!$D$3</f>
-        <v>69.580000000000013</v>
+        <v>68.040000000000006</v>
       </c>
       <c r="F7" s="13">
         <f>+a!K3*a!$D$3</f>
-        <v>98.7</v>
+        <v>95.76</v>
       </c>
       <c r="G7" s="13">
         <f>+a!L3*a!$D$3</f>
-        <v>131.04000000000002</v>
+        <v>127.68</v>
       </c>
       <c r="H7" s="13">
         <f>+a!M3*a!$D$3</f>
-        <v>162.82000000000002</v>
+        <v>158.76000000000002</v>
       </c>
       <c r="I7" s="13">
         <f>+a!N3*a!$D$3</f>
-        <v>190.96</v>
+        <v>185.64000000000001</v>
       </c>
       <c r="J7" s="13">
         <f>+a!O3*a!$D$3</f>
-        <v>217.98000000000002</v>
+        <v>211.82000000000002</v>
       </c>
       <c r="K7" s="13">
         <f>+a!P3*a!$D$3</f>
-        <v>247.52</v>
+        <v>239.96000000000004</v>
       </c>
       <c r="L7" s="13">
         <f>+a!Q3*a!$D$3</f>
-        <v>275.38000000000005</v>
-      </c>
-      <c r="M7" s="13">
+        <v>267.40000000000003</v>
+      </c>
+      <c r="M7" s="13" t="e">
         <f>+a!R3*a!$D$3</f>
-        <v>297.78000000000003</v>
+        <v>#N/A</v>
       </c>
       <c r="N7" s="13" t="e">
         <f>+a!S3*a!$D$3</f>
@@ -2022,43 +3144,43 @@
     <row r="8" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D8" s="13">
         <f>+a!I4*a!$D$4</f>
-        <v>27.483499999999999</v>
+        <v>26.8565</v>
       </c>
       <c r="E8" s="13">
         <f>+a!J4*a!$D$4</f>
-        <v>51.936499999999995</v>
+        <v>50.786999999999999</v>
       </c>
       <c r="F8" s="13">
         <f>+a!K4*a!$D$4</f>
-        <v>73.672499999999999</v>
+        <v>71.477999999999994</v>
       </c>
       <c r="G8" s="13">
         <f>+a!L4*a!$D$4</f>
-        <v>97.811999999999998</v>
+        <v>95.304000000000002</v>
       </c>
       <c r="H8" s="13">
         <f>+a!M4*a!$D$4</f>
-        <v>121.53349999999999</v>
+        <v>118.503</v>
       </c>
       <c r="I8" s="13">
         <f>+a!N4*a!$D$4</f>
-        <v>142.53799999999998</v>
+        <v>138.56700000000001</v>
       </c>
       <c r="J8" s="13">
         <f>+a!O4*a!$D$4</f>
-        <v>162.70650000000001</v>
+        <v>158.10849999999999</v>
       </c>
       <c r="K8" s="13">
         <f>+a!P4*a!$D$4</f>
-        <v>184.756</v>
+        <v>179.113</v>
       </c>
       <c r="L8" s="13">
         <f>+a!Q4*a!$D$4</f>
-        <v>205.5515</v>
-      </c>
-      <c r="M8" s="13">
+        <v>199.595</v>
+      </c>
+      <c r="M8" s="13" t="e">
         <f>+a!R4*a!$D$4</f>
-        <v>222.2715</v>
+        <v>#N/A</v>
       </c>
       <c r="N8" s="13" t="e">
         <f>+a!S4*a!$D$4</f>
@@ -2108,43 +3230,43 @@
     <row r="9" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D9" s="13">
         <f>+a!I7*a!$D$5</f>
-        <v>4.5269999999999992</v>
+        <v>4.6259999999999994</v>
       </c>
       <c r="E9" s="13">
         <f>+a!J7*a!$D$5</f>
-        <v>8.7749999999999986</v>
+        <v>9.0089999999999986</v>
       </c>
       <c r="F9" s="13">
         <f>+a!K7*a!$D$5</f>
-        <v>13.023</v>
+        <v>13.356</v>
       </c>
       <c r="G9" s="13">
         <f>+a!L7*a!$D$5</f>
-        <v>17.180999999999997</v>
+        <v>17.576999999999998</v>
       </c>
       <c r="H9" s="13">
         <f>+a!M7*a!$D$5</f>
-        <v>20.88</v>
+        <v>21.383999999999997</v>
       </c>
       <c r="I9" s="13">
         <f>+a!N7*a!$D$5</f>
-        <v>24.560999999999996</v>
+        <v>25.181999999999999</v>
       </c>
       <c r="J9" s="13">
         <f>+a!O7*a!$D$5</f>
-        <v>28.043999999999997</v>
+        <v>28.781999999999996</v>
       </c>
       <c r="K9" s="13">
         <f>+a!P7*a!$D$5</f>
-        <v>31.391999999999996</v>
+        <v>32.228999999999999</v>
       </c>
       <c r="L9" s="13">
         <f>+a!Q7*a!$D$5</f>
-        <v>34.433999999999997</v>
-      </c>
-      <c r="M9" s="13">
+        <v>35.396999999999998</v>
+      </c>
+      <c r="M9" s="13" t="e">
         <f>+a!R7*a!$D$5</f>
-        <v>37.646999999999998</v>
+        <v>#N/A</v>
       </c>
       <c r="N9" s="13" t="e">
         <f>+a!S7*a!$D$5</f>
@@ -2194,49 +3316,49 @@
     <row r="10" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D10">
         <f>SUM(D3:D8)</f>
-        <v>96.432500000000005</v>
+        <v>94.611000000000004</v>
       </c>
       <c r="E10" s="13">
         <f t="shared" ref="E10:M10" si="1">SUM(E3:E8)</f>
-        <v>186.64700000000002</v>
+        <v>182.91900000000001</v>
       </c>
       <c r="F10" s="13">
         <f t="shared" si="1"/>
-        <v>269.07600000000002</v>
+        <v>262.83750000000003</v>
       </c>
       <c r="G10" s="13">
         <f t="shared" si="1"/>
-        <v>353.12200000000001</v>
+        <v>345.86799999999999</v>
       </c>
       <c r="H10" s="13">
         <f t="shared" si="1"/>
-        <v>436.87300000000005</v>
+        <v>427.916</v>
       </c>
       <c r="I10" s="13">
         <f t="shared" si="1"/>
-        <v>513.18799999999999</v>
+        <v>501.75750000000005</v>
       </c>
       <c r="J10" s="13">
         <f t="shared" si="1"/>
-        <v>586.65250000000003</v>
+        <v>573.27649999999994</v>
       </c>
       <c r="K10" s="13">
         <f t="shared" si="1"/>
-        <v>661.45650000000001</v>
+        <v>645.56700000000001</v>
       </c>
       <c r="L10" s="13">
         <f t="shared" si="1"/>
-        <v>733.64400000000012</v>
-      </c>
-      <c r="M10" s="13">
+        <v>716.26550000000009</v>
+      </c>
+      <c r="M10" s="13" t="e">
         <f t="shared" si="1"/>
-        <v>794.9670000000001</v>
+        <v>#N/A</v>
       </c>
     </row>
     <row r="14" spans="4:24" x14ac:dyDescent="0.25">
       <c r="E14" s="13">
         <f>+a!G5*a!E5*a!I5</f>
-        <v>11643638.440896001</v>
+        <v>12331932.338880001</v>
       </c>
       <c r="G14" s="13">
         <f>+(a!G5+a!H5)*a!$E$7</f>
@@ -2244,13 +3366,13 @@
       </c>
       <c r="H14">
         <f>+E14/G14</f>
-        <v>98.062096774193549</v>
+        <v>103.85887096774192</v>
       </c>
     </row>
     <row r="15" spans="4:24" x14ac:dyDescent="0.25">
       <c r="E15" s="13">
         <f>+a!G6*a!E6*a!I6</f>
-        <v>11063500</v>
+        <v>11717500</v>
       </c>
       <c r="G15" s="13">
         <f>+(a!G6+a!H6)*a!$E$7</f>
@@ -2258,13 +3380,13 @@
       </c>
       <c r="H15" s="13">
         <f t="shared" ref="H15:H19" si="2">+E15/G15</f>
-        <v>88.543417366946784</v>
+        <v>93.777511004401759</v>
       </c>
     </row>
     <row r="16" spans="4:24" x14ac:dyDescent="0.25">
       <c r="E16" s="13">
         <f>+a!G1*a!E1*a!I1</f>
-        <v>6590500</v>
+        <v>6174000</v>
       </c>
       <c r="G16" s="13">
         <f>+(a!G1+a!H1)*a!$E$7</f>
@@ -2272,13 +3394,13 @@
       </c>
       <c r="H16" s="13">
         <f t="shared" si="2"/>
-        <v>54.190169218372283</v>
+        <v>50.765511684125705</v>
       </c>
     </row>
     <row r="17" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E17" s="13">
         <f>+a!G2*a!E2*a!I2</f>
-        <v>4318312.5216000006</v>
+        <v>4045408.0128000001</v>
       </c>
       <c r="G17" s="13">
         <f>+(a!G2+a!H2)*a!$E$7</f>
@@ -2286,7 +3408,7 @@
       </c>
       <c r="H17" s="13">
         <f t="shared" si="2"/>
-        <v>53.94385026737968</v>
+        <v>50.534759358288767</v>
       </c>
     </row>
     <row r="18" spans="5:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Cambios en la presentación
</commit_message>
<xml_diff>
--- a/evsim/Impac.Amb..xlsx
+++ b/evsim/Impac.Amb..xlsx
@@ -1092,31 +1092,31 @@
         <v>22</v>
       </c>
       <c r="I1" s="15">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="J1" s="15">
-        <v>253.5</v>
+        <v>216</v>
       </c>
       <c r="K1" s="15">
-        <v>381</v>
-      </c>
-      <c r="L1" s="15">
-        <v>489.5</v>
-      </c>
-      <c r="M1" s="15">
-        <v>604</v>
-      </c>
-      <c r="N1" s="15">
-        <v>721.5</v>
-      </c>
-      <c r="O1" s="15">
-        <v>829</v>
-      </c>
-      <c r="P1" s="15">
-        <v>927</v>
-      </c>
-      <c r="Q1" s="15">
-        <v>1009</v>
+        <v>312</v>
+      </c>
+      <c r="L1" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M1" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N1" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O1" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P1" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Q1" s="15" t="e">
+        <v>#N/A</v>
       </c>
       <c r="R1" s="15" t="e">
         <v>#N/A</v>
@@ -1181,31 +1181,31 @@
         <v>61.155072000000004</v>
       </c>
       <c r="I2" s="17">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="J2" s="15">
-        <v>253.5</v>
+        <v>216</v>
       </c>
       <c r="K2" s="17">
-        <v>381</v>
-      </c>
-      <c r="L2" s="15">
-        <v>489.5</v>
-      </c>
-      <c r="M2" s="17">
-        <v>604</v>
-      </c>
-      <c r="N2" s="15">
-        <v>721.5</v>
-      </c>
-      <c r="O2" s="17">
-        <v>829</v>
-      </c>
-      <c r="P2" s="15">
-        <v>927</v>
-      </c>
-      <c r="Q2" s="17">
-        <v>1009</v>
+        <v>312</v>
+      </c>
+      <c r="L2" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M2" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N2" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O2" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P2" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Q2" s="17" t="e">
+        <v>#N/A</v>
       </c>
       <c r="R2" s="15" t="e">
         <v>#N/A</v>
@@ -1270,31 +1270,31 @@
         <v>185</v>
       </c>
       <c r="I3" s="18">
-        <v>128.5</v>
+        <v>159</v>
       </c>
       <c r="J3" s="15">
-        <v>243</v>
+        <v>304</v>
       </c>
       <c r="K3" s="18">
-        <v>342</v>
-      </c>
-      <c r="L3" s="15">
-        <v>456</v>
-      </c>
-      <c r="M3" s="18">
-        <v>567</v>
-      </c>
-      <c r="N3" s="15">
-        <v>663</v>
-      </c>
-      <c r="O3" s="18">
-        <v>756.5</v>
-      </c>
-      <c r="P3" s="15">
-        <v>857</v>
-      </c>
-      <c r="Q3" s="18">
-        <v>955</v>
+        <v>439.5</v>
+      </c>
+      <c r="L3" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M3" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N3" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O3" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P3" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Q3" s="18" t="e">
+        <v>#N/A</v>
       </c>
       <c r="R3" s="15" t="e">
         <v>#N/A</v>
@@ -1359,31 +1359,31 @@
         <v>141.62227200000001</v>
       </c>
       <c r="I4" s="17">
-        <v>128.5</v>
+        <v>159</v>
       </c>
       <c r="J4" s="15">
-        <v>243</v>
+        <v>304</v>
       </c>
       <c r="K4" s="17">
-        <v>342</v>
-      </c>
-      <c r="L4" s="15">
-        <v>456</v>
-      </c>
-      <c r="M4" s="17">
-        <v>567</v>
-      </c>
-      <c r="N4" s="15">
-        <v>663</v>
-      </c>
-      <c r="O4" s="17">
-        <v>756.5</v>
-      </c>
-      <c r="P4" s="15">
-        <v>857</v>
-      </c>
-      <c r="Q4" s="17">
-        <v>955</v>
+        <v>439.5</v>
+      </c>
+      <c r="L4" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M4" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N4" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O4" s="17" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P4" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Q4" s="17" t="e">
+        <v>#N/A</v>
       </c>
       <c r="R4" s="15" t="e">
         <v>#N/A</v>
@@ -1448,31 +1448,31 @@
         <v>33.796224000000002</v>
       </c>
       <c r="I5" s="15">
-        <v>107.5</v>
+        <v>99.5</v>
       </c>
       <c r="J5" s="15">
-        <v>217.5</v>
+        <v>207</v>
       </c>
       <c r="K5" s="15">
-        <v>321.5</v>
-      </c>
-      <c r="L5" s="15">
-        <v>413.5</v>
-      </c>
-      <c r="M5" s="15">
-        <v>503</v>
-      </c>
-      <c r="N5" s="15">
-        <v>583</v>
-      </c>
-      <c r="O5" s="15">
-        <v>665</v>
-      </c>
-      <c r="P5" s="15">
-        <v>737</v>
-      </c>
-      <c r="Q5" s="15">
-        <v>822.5</v>
+        <v>311.5</v>
+      </c>
+      <c r="L5" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M5" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N5" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O5" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P5" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Q5" s="15" t="e">
+        <v>#N/A</v>
       </c>
       <c r="R5" s="15" t="e">
         <v>#N/A</v>
@@ -1537,31 +1537,31 @@
         <v>50</v>
       </c>
       <c r="I6" s="16">
-        <v>107.5</v>
+        <v>99.5</v>
       </c>
       <c r="J6" s="15">
-        <v>217.5</v>
+        <v>207</v>
       </c>
       <c r="K6" s="16">
-        <v>321.5</v>
-      </c>
-      <c r="L6" s="15">
-        <v>413.5</v>
-      </c>
-      <c r="M6" s="16">
-        <v>503</v>
-      </c>
-      <c r="N6" s="15">
-        <v>583</v>
-      </c>
-      <c r="O6" s="16">
-        <v>665</v>
-      </c>
-      <c r="P6" s="15">
-        <v>737</v>
-      </c>
-      <c r="Q6" s="16">
-        <v>822.5</v>
+        <v>311.5</v>
+      </c>
+      <c r="L6" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M6" s="16" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N6" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O6" s="16" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P6" s="15" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Q6" s="16" t="e">
+        <v>#N/A</v>
       </c>
       <c r="R6" s="15" t="e">
         <v>#N/A</v>
@@ -1626,31 +1626,31 @@
         <v>0</v>
       </c>
       <c r="I7" s="18">
-        <v>514</v>
+        <v>503</v>
       </c>
       <c r="J7" s="18">
-        <v>1001</v>
+        <v>975</v>
       </c>
       <c r="K7" s="18">
-        <v>1484</v>
-      </c>
-      <c r="L7" s="18">
-        <v>1953</v>
-      </c>
-      <c r="M7" s="18">
-        <v>2376</v>
-      </c>
-      <c r="N7" s="18">
-        <v>2798</v>
-      </c>
-      <c r="O7" s="18">
-        <v>3198</v>
-      </c>
-      <c r="P7" s="18">
-        <v>3581</v>
-      </c>
-      <c r="Q7" s="18">
-        <v>3933</v>
+        <v>1447</v>
+      </c>
+      <c r="L7" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="M7" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="N7" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="O7" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="P7" s="18" t="e">
+        <v>#N/A</v>
+      </c>
+      <c r="Q7" s="18" t="e">
+        <v>#N/A</v>
       </c>
       <c r="R7" s="18" t="e">
         <v>#N/A</v>
@@ -1710,13 +1710,13 @@
       </c>
       <c r="B10" s="31">
         <f>+I1</f>
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="C10" s="22">
-        <v>6174</v>
+        <v>5341</v>
       </c>
       <c r="D10" s="25">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H10" s="13">
         <v>40.49153908138598</v>
@@ -1728,13 +1728,13 @@
       </c>
       <c r="B11" s="31">
         <f t="shared" ref="B11:B15" si="0">+I2</f>
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="C11" s="22">
-        <v>4045.4080128000005</v>
+        <v>3499.5989952000004</v>
       </c>
       <c r="D11" s="25">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="H11" s="13">
         <v>40.30748663101604</v>
@@ -1746,7 +1746,7 @@
       </c>
       <c r="B12" s="31">
         <f t="shared" si="0"/>
-        <v>128.5</v>
+        <v>159</v>
       </c>
       <c r="C12" s="22">
         <v>0</v>
@@ -1764,7 +1764,7 @@
       </c>
       <c r="B13" s="31">
         <f t="shared" si="0"/>
-        <v>128.5</v>
+        <v>159</v>
       </c>
       <c r="C13" s="22">
         <v>0</v>
@@ -1782,13 +1782,13 @@
       </c>
       <c r="B14" s="31">
         <f t="shared" si="0"/>
-        <v>107.5</v>
+        <v>99.5</v>
       </c>
       <c r="C14" s="22">
-        <v>12331.93233888</v>
+        <v>11414.207141568002</v>
       </c>
       <c r="D14" s="25">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="H14" s="13">
         <v>128.49516129032256</v>
@@ -1800,13 +1800,13 @@
       </c>
       <c r="B15" s="34">
         <f t="shared" si="0"/>
-        <v>107.5</v>
+        <v>99.5</v>
       </c>
       <c r="C15" s="26">
-        <v>11717.5</v>
+        <v>10845.5</v>
       </c>
       <c r="D15" s="27">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="H15" s="13">
         <v>116.02240896358543</v>
@@ -2714,39 +2714,39 @@
     <row r="3" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D3" s="13">
         <f>+a!I5*a!$D$5</f>
-        <v>0.96749999999999992</v>
+        <v>0.89549999999999996</v>
       </c>
       <c r="E3" s="13">
         <f>+a!J5*a!$D$5</f>
-        <v>1.9574999999999998</v>
+        <v>1.8629999999999998</v>
       </c>
       <c r="F3" s="13">
         <f>+a!K5*a!$D$5</f>
-        <v>2.8935</v>
-      </c>
-      <c r="G3" s="13">
+        <v>2.8034999999999997</v>
+      </c>
+      <c r="G3" s="13" t="e">
         <f>+a!L5*a!$D$5</f>
-        <v>3.7214999999999998</v>
-      </c>
-      <c r="H3" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="H3" s="13" t="e">
         <f>+a!M5*a!$D$5</f>
-        <v>4.5269999999999992</v>
-      </c>
-      <c r="I3" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="I3" s="13" t="e">
         <f>+a!N5*a!$D$5</f>
-        <v>5.2469999999999999</v>
-      </c>
-      <c r="J3" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="J3" s="13" t="e">
         <f>+a!O5*a!$D$5</f>
-        <v>5.9849999999999994</v>
-      </c>
-      <c r="K3" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="K3" s="13" t="e">
         <f>+a!P5*a!$D$5</f>
-        <v>6.6329999999999991</v>
-      </c>
-      <c r="L3" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="L3" s="13" t="e">
         <f>+a!Q5*a!$D$5</f>
-        <v>7.4024999999999999</v>
+        <v>#N/A</v>
       </c>
       <c r="M3" s="13" t="e">
         <f>+a!R5*a!$D$5</f>
@@ -2800,39 +2800,39 @@
     <row r="4" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D4" s="13">
         <f>+a!I6*a!$D$6</f>
-        <v>13.545</v>
+        <v>12.537000000000001</v>
       </c>
       <c r="E4" s="13">
         <f>+a!J6*a!$D$6</f>
-        <v>27.405000000000001</v>
+        <v>26.082000000000001</v>
       </c>
       <c r="F4" s="13">
         <f>+a!K6*a!$D$6</f>
-        <v>40.509</v>
-      </c>
-      <c r="G4" s="13">
+        <v>39.249000000000002</v>
+      </c>
+      <c r="G4" s="13" t="e">
         <f>+a!L6*a!$D$6</f>
-        <v>52.100999999999999</v>
-      </c>
-      <c r="H4" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="H4" s="13" t="e">
         <f>+a!M6*a!$D$6</f>
-        <v>63.378</v>
-      </c>
-      <c r="I4" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="I4" s="13" t="e">
         <f>+a!N6*a!$D$6</f>
-        <v>73.457999999999998</v>
-      </c>
-      <c r="J4" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="J4" s="13" t="e">
         <f>+a!O6*a!$D$6</f>
-        <v>83.79</v>
-      </c>
-      <c r="K4" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="K4" s="13" t="e">
         <f>+a!P6*a!$D$6</f>
-        <v>92.861999999999995</v>
-      </c>
-      <c r="L4" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="L4" s="13" t="e">
         <f>+a!Q6*a!$D$6</f>
-        <v>103.63500000000001</v>
+        <v>#N/A</v>
       </c>
       <c r="M4" s="13" t="e">
         <f>+a!R6*a!$D$6</f>
@@ -2886,39 +2886,39 @@
     <row r="5" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D5" s="13">
         <f>+a!I1*a!$D$1</f>
-        <v>4.1580000000000004</v>
+        <v>3.597</v>
       </c>
       <c r="E5" s="13">
         <f>+a!J1*a!$D$1</f>
-        <v>8.3655000000000008</v>
+        <v>7.1280000000000001</v>
       </c>
       <c r="F5" s="13">
         <f>+a!K1*a!$D$1</f>
-        <v>12.573</v>
-      </c>
-      <c r="G5" s="13">
+        <v>10.296000000000001</v>
+      </c>
+      <c r="G5" s="13" t="e">
         <f>+a!L1*a!$D$1</f>
-        <v>16.153500000000001</v>
-      </c>
-      <c r="H5" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="H5" s="13" t="e">
         <f>+a!M1*a!$D$1</f>
-        <v>19.932000000000002</v>
-      </c>
-      <c r="I5" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="I5" s="13" t="e">
         <f>+a!N1*a!$D$1</f>
-        <v>23.8095</v>
-      </c>
-      <c r="J5" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="J5" s="13" t="e">
         <f>+a!O1*a!$D$1</f>
-        <v>27.357000000000003</v>
-      </c>
-      <c r="K5" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="K5" s="13" t="e">
         <f>+a!P1*a!$D$1</f>
-        <v>30.591000000000001</v>
-      </c>
-      <c r="L5" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="L5" s="13" t="e">
         <f>+a!Q1*a!$D$1</f>
-        <v>33.297000000000004</v>
+        <v>#N/A</v>
       </c>
       <c r="M5" s="13" t="e">
         <f>+a!R1*a!$D$1</f>
@@ -2972,39 +2972,39 @@
     <row r="6" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D6" s="13">
         <f>+a!I2*a!$D$2</f>
-        <v>13.103999999999999</v>
+        <v>11.336</v>
       </c>
       <c r="E6" s="13">
         <f>+a!J2*a!$D$2</f>
-        <v>26.363999999999997</v>
+        <v>22.463999999999999</v>
       </c>
       <c r="F6" s="13">
         <f>+a!K2*a!$D$2</f>
-        <v>39.623999999999995</v>
-      </c>
-      <c r="G6" s="13">
+        <v>32.448</v>
+      </c>
+      <c r="G6" s="13" t="e">
         <f>+a!L2*a!$D$2</f>
-        <v>50.907999999999994</v>
-      </c>
-      <c r="H6" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="H6" s="13" t="e">
         <f>+a!M2*a!$D$2</f>
-        <v>62.815999999999995</v>
-      </c>
-      <c r="I6" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="I6" s="13" t="e">
         <f>+a!N2*a!$D$2</f>
-        <v>75.036000000000001</v>
-      </c>
-      <c r="J6" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="J6" s="13" t="e">
         <f>+a!O2*a!$D$2</f>
-        <v>86.215999999999994</v>
-      </c>
-      <c r="K6" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="K6" s="13" t="e">
         <f>+a!P2*a!$D$2</f>
-        <v>96.408000000000001</v>
-      </c>
-      <c r="L6" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="L6" s="13" t="e">
         <f>+a!Q2*a!$D$2</f>
-        <v>104.93599999999999</v>
+        <v>#N/A</v>
       </c>
       <c r="M6" s="13" t="e">
         <f>+a!R2*a!$D$2</f>
@@ -3058,39 +3058,39 @@
     <row r="7" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D7" s="13">
         <f>+a!I3*a!$D$3</f>
-        <v>35.980000000000004</v>
+        <v>44.52</v>
       </c>
       <c r="E7" s="13">
         <f>+a!J3*a!$D$3</f>
-        <v>68.040000000000006</v>
+        <v>85.12</v>
       </c>
       <c r="F7" s="13">
         <f>+a!K3*a!$D$3</f>
-        <v>95.76</v>
-      </c>
-      <c r="G7" s="13">
+        <v>123.06000000000002</v>
+      </c>
+      <c r="G7" s="13" t="e">
         <f>+a!L3*a!$D$3</f>
-        <v>127.68</v>
-      </c>
-      <c r="H7" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="H7" s="13" t="e">
         <f>+a!M3*a!$D$3</f>
-        <v>158.76000000000002</v>
-      </c>
-      <c r="I7" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="I7" s="13" t="e">
         <f>+a!N3*a!$D$3</f>
-        <v>185.64000000000001</v>
-      </c>
-      <c r="J7" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="J7" s="13" t="e">
         <f>+a!O3*a!$D$3</f>
-        <v>211.82000000000002</v>
-      </c>
-      <c r="K7" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="K7" s="13" t="e">
         <f>+a!P3*a!$D$3</f>
-        <v>239.96000000000004</v>
-      </c>
-      <c r="L7" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="L7" s="13" t="e">
         <f>+a!Q3*a!$D$3</f>
-        <v>267.40000000000003</v>
+        <v>#N/A</v>
       </c>
       <c r="M7" s="13" t="e">
         <f>+a!R3*a!$D$3</f>
@@ -3144,39 +3144,39 @@
     <row r="8" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D8" s="13">
         <f>+a!I4*a!$D$4</f>
-        <v>26.8565</v>
+        <v>33.231000000000002</v>
       </c>
       <c r="E8" s="13">
         <f>+a!J4*a!$D$4</f>
-        <v>50.786999999999999</v>
+        <v>63.535999999999994</v>
       </c>
       <c r="F8" s="13">
         <f>+a!K4*a!$D$4</f>
-        <v>71.477999999999994</v>
-      </c>
-      <c r="G8" s="13">
+        <v>91.855499999999992</v>
+      </c>
+      <c r="G8" s="13" t="e">
         <f>+a!L4*a!$D$4</f>
-        <v>95.304000000000002</v>
-      </c>
-      <c r="H8" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="H8" s="13" t="e">
         <f>+a!M4*a!$D$4</f>
-        <v>118.503</v>
-      </c>
-      <c r="I8" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="I8" s="13" t="e">
         <f>+a!N4*a!$D$4</f>
-        <v>138.56700000000001</v>
-      </c>
-      <c r="J8" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="J8" s="13" t="e">
         <f>+a!O4*a!$D$4</f>
-        <v>158.10849999999999</v>
-      </c>
-      <c r="K8" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="K8" s="13" t="e">
         <f>+a!P4*a!$D$4</f>
-        <v>179.113</v>
-      </c>
-      <c r="L8" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="L8" s="13" t="e">
         <f>+a!Q4*a!$D$4</f>
-        <v>199.595</v>
+        <v>#N/A</v>
       </c>
       <c r="M8" s="13" t="e">
         <f>+a!R4*a!$D$4</f>
@@ -3230,39 +3230,39 @@
     <row r="9" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D9" s="13">
         <f>+a!I7*a!$D$5</f>
-        <v>4.6259999999999994</v>
+        <v>4.5269999999999992</v>
       </c>
       <c r="E9" s="13">
         <f>+a!J7*a!$D$5</f>
-        <v>9.0089999999999986</v>
+        <v>8.7749999999999986</v>
       </c>
       <c r="F9" s="13">
         <f>+a!K7*a!$D$5</f>
-        <v>13.356</v>
-      </c>
-      <c r="G9" s="13">
+        <v>13.023</v>
+      </c>
+      <c r="G9" s="13" t="e">
         <f>+a!L7*a!$D$5</f>
-        <v>17.576999999999998</v>
-      </c>
-      <c r="H9" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="H9" s="13" t="e">
         <f>+a!M7*a!$D$5</f>
-        <v>21.383999999999997</v>
-      </c>
-      <c r="I9" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="I9" s="13" t="e">
         <f>+a!N7*a!$D$5</f>
-        <v>25.181999999999999</v>
-      </c>
-      <c r="J9" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="J9" s="13" t="e">
         <f>+a!O7*a!$D$5</f>
-        <v>28.781999999999996</v>
-      </c>
-      <c r="K9" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="K9" s="13" t="e">
         <f>+a!P7*a!$D$5</f>
-        <v>32.228999999999999</v>
-      </c>
-      <c r="L9" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="L9" s="13" t="e">
         <f>+a!Q7*a!$D$5</f>
-        <v>35.396999999999998</v>
+        <v>#N/A</v>
       </c>
       <c r="M9" s="13" t="e">
         <f>+a!R7*a!$D$5</f>
@@ -3316,39 +3316,39 @@
     <row r="10" spans="4:24" x14ac:dyDescent="0.25">
       <c r="D10">
         <f>SUM(D3:D8)</f>
-        <v>94.611000000000004</v>
+        <v>106.1165</v>
       </c>
       <c r="E10" s="13">
         <f t="shared" ref="E10:M10" si="1">SUM(E3:E8)</f>
-        <v>182.91900000000001</v>
+        <v>206.19300000000001</v>
       </c>
       <c r="F10" s="13">
         <f t="shared" si="1"/>
-        <v>262.83750000000003</v>
-      </c>
-      <c r="G10" s="13">
+        <v>299.71200000000005</v>
+      </c>
+      <c r="G10" s="13" t="e">
         <f t="shared" si="1"/>
-        <v>345.86799999999999</v>
-      </c>
-      <c r="H10" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="H10" s="13" t="e">
         <f t="shared" si="1"/>
-        <v>427.916</v>
-      </c>
-      <c r="I10" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="I10" s="13" t="e">
         <f t="shared" si="1"/>
-        <v>501.75750000000005</v>
-      </c>
-      <c r="J10" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="J10" s="13" t="e">
         <f t="shared" si="1"/>
-        <v>573.27649999999994</v>
-      </c>
-      <c r="K10" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="K10" s="13" t="e">
         <f t="shared" si="1"/>
-        <v>645.56700000000001</v>
-      </c>
-      <c r="L10" s="13">
+        <v>#N/A</v>
+      </c>
+      <c r="L10" s="13" t="e">
         <f t="shared" si="1"/>
-        <v>716.26550000000009</v>
+        <v>#N/A</v>
       </c>
       <c r="M10" s="13" t="e">
         <f t="shared" si="1"/>
@@ -3358,7 +3358,7 @@
     <row r="14" spans="4:24" x14ac:dyDescent="0.25">
       <c r="E14" s="13">
         <f>+a!G5*a!E5*a!I5</f>
-        <v>12331932.338880001</v>
+        <v>11414207.141568001</v>
       </c>
       <c r="G14" s="13">
         <f>+(a!G5+a!H5)*a!$E$7</f>
@@ -3366,13 +3366,13 @@
       </c>
       <c r="H14">
         <f>+E14/G14</f>
-        <v>103.85887096774192</v>
+        <v>96.129838709677415</v>
       </c>
     </row>
     <row r="15" spans="4:24" x14ac:dyDescent="0.25">
       <c r="E15" s="13">
         <f>+a!G6*a!E6*a!I6</f>
-        <v>11717500</v>
+        <v>10845500</v>
       </c>
       <c r="G15" s="13">
         <f>+(a!G6+a!H6)*a!$E$7</f>
@@ -3380,13 +3380,13 @@
       </c>
       <c r="H15" s="13">
         <f t="shared" ref="H15:H19" si="2">+E15/G15</f>
-        <v>93.777511004401759</v>
+        <v>86.798719487795111</v>
       </c>
     </row>
     <row r="16" spans="4:24" x14ac:dyDescent="0.25">
       <c r="E16" s="13">
         <f>+a!G1*a!E1*a!I1</f>
-        <v>6174000</v>
+        <v>5341000</v>
       </c>
       <c r="G16" s="13">
         <f>+(a!G1+a!H1)*a!$E$7</f>
@@ -3394,13 +3394,13 @@
       </c>
       <c r="H16" s="13">
         <f t="shared" si="2"/>
-        <v>50.765511684125705</v>
+        <v>43.916196615632558</v>
       </c>
     </row>
     <row r="17" spans="5:8" x14ac:dyDescent="0.25">
       <c r="E17" s="13">
         <f>+a!G2*a!E2*a!I2</f>
-        <v>4045408.0128000001</v>
+        <v>3499598.9952000002</v>
       </c>
       <c r="G17" s="13">
         <f>+(a!G2+a!H2)*a!$E$7</f>
@@ -3408,7 +3408,7 @@
       </c>
       <c r="H17" s="13">
         <f t="shared" si="2"/>
-        <v>50.534759358288767</v>
+        <v>43.716577540106947</v>
       </c>
     </row>
     <row r="18" spans="5:8" x14ac:dyDescent="0.25">

</xml_diff>